<commit_message>
[🔥HotFix] Enemy stat temporary fix
- 적 스텟 임시 수정
- 18레벨부터 체력 반, 공격력 2배
</commit_message>
<xml_diff>
--- a/IdleGame/Assets/@Resources/Texts/ExcelTable/StageTable.xlsx
+++ b/IdleGame/Assets/@Resources/Texts/ExcelTable/StageTable.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Project\TeamProject-IdleGame\IdleGame\Assets\@Resources\Texts\ExcelTable\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E60FD034-ED13-4C1C-B84E-76B4BF55BB6A}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{60552948-EB60-4507-8768-44CFF5993B15}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="28680" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Stage" sheetId="1" r:id="rId1"/>
@@ -139,7 +139,7 @@
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
   <numFmts count="1">
-    <numFmt numFmtId="178" formatCode="0_);[Red]\(0\)"/>
+    <numFmt numFmtId="176" formatCode="0_);[Red]\(0\)"/>
   </numFmts>
   <fonts count="3" x14ac:knownFonts="1">
     <font>
@@ -210,7 +210,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
       <alignment horizontal="right"/>
     </xf>
-    <xf numFmtId="178" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
+    <xf numFmtId="176" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
       <alignment horizontal="right"/>
     </xf>
   </cellXfs>
@@ -218,50 +218,6 @@
     <cellStyle name="표준" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="20">
-    <dxf>
-      <numFmt numFmtId="178" formatCode="0_);[Red]\(0\)"/>
-      <alignment horizontal="right" vertical="bottom" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
-    </dxf>
-    <dxf>
-      <alignment horizontal="right" vertical="bottom" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
-    </dxf>
-    <dxf>
-      <numFmt numFmtId="178" formatCode="0_);[Red]\(0\)"/>
-      <alignment horizontal="right" vertical="bottom" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
-    </dxf>
-    <dxf>
-      <numFmt numFmtId="178" formatCode="0_);[Red]\(0\)"/>
-      <alignment horizontal="right" vertical="bottom" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
-    </dxf>
-    <dxf>
-      <alignment horizontal="right" vertical="bottom" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
-    </dxf>
-    <dxf>
-      <alignment horizontal="right" vertical="bottom" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
-    </dxf>
-    <dxf>
-      <numFmt numFmtId="0" formatCode="General"/>
-      <alignment horizontal="right" vertical="bottom" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
-    </dxf>
-    <dxf>
-      <alignment horizontal="right" vertical="bottom" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
-    </dxf>
-    <dxf>
-      <numFmt numFmtId="0" formatCode="General"/>
-      <alignment horizontal="right" vertical="bottom" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
-    </dxf>
-    <dxf>
-      <alignment horizontal="right" vertical="bottom" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
-    </dxf>
-    <dxf>
-      <alignment horizontal="right" vertical="bottom" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
-    </dxf>
-    <dxf>
-      <alignment horizontal="right" vertical="bottom" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
-    </dxf>
-    <dxf>
-      <alignment horizontal="right" vertical="bottom" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
-    </dxf>
     <dxf>
       <alignment horizontal="right" vertical="bottom" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
     </dxf>
@@ -286,6 +242,50 @@
     </dxf>
     <dxf>
       <numFmt numFmtId="0" formatCode="General"/>
+      <alignment horizontal="right" vertical="bottom" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <numFmt numFmtId="0" formatCode="General"/>
+      <alignment horizontal="right" vertical="bottom" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <alignment horizontal="right" vertical="bottom" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <alignment horizontal="right" vertical="bottom" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <numFmt numFmtId="0" formatCode="General"/>
+      <alignment horizontal="right" vertical="bottom" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <numFmt numFmtId="176" formatCode="0_);[Red]\(0\)"/>
+      <alignment horizontal="right" vertical="bottom" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <alignment horizontal="right" vertical="bottom" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <numFmt numFmtId="176" formatCode="0_);[Red]\(0\)"/>
+      <alignment horizontal="right" vertical="bottom" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <alignment horizontal="right" vertical="bottom" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <numFmt numFmtId="176" formatCode="0_);[Red]\(0\)"/>
+      <alignment horizontal="right" vertical="bottom" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <alignment horizontal="right" vertical="bottom" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <alignment horizontal="right" vertical="bottom" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <alignment horizontal="right" vertical="bottom" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
       <alignment horizontal="right" vertical="bottom" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
     </dxf>
     <dxf>
@@ -327,25 +327,25 @@
 <table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="1" xr:uid="{50268604-F68E-4DBD-AE64-4183B0FE7F47}" name="표1" displayName="표1" ref="A2:H302" totalsRowShown="0" headerRowDxfId="19">
   <autoFilter ref="A2:H302" xr:uid="{50268604-F68E-4DBD-AE64-4183B0FE7F47}"/>
   <tableColumns count="8">
-    <tableColumn id="1" xr3:uid="{ABEFAF0D-3E9C-4BC0-BD85-867C72E372D9}" name="Index : Int" dataDxfId="18" totalsRowDxfId="12"/>
-    <tableColumn id="4" xr3:uid="{9A52DE84-B46A-41BA-9891-9221E6FD8CA2}" name="StageConfig : String" dataDxfId="17" totalsRowDxfId="11"/>
-    <tableColumn id="5" xr3:uid="{52BABBB3-0B5B-4EA5-A096-52FE17505682}" name="StageBackground : String" dataDxfId="4" totalsRowDxfId="10"/>
-    <tableColumn id="6" xr3:uid="{8CB87B44-9BE8-4447-B7A9-5AB6AF555193}" name="EnemyHpRate : long" dataDxfId="3" totalsRowDxfId="9"/>
-    <tableColumn id="3" xr3:uid="{D9A76B69-1806-4056-859C-537F7DF173E6}" name="EnemyAttackRate : long" dataDxfId="2" totalsRowDxfId="5"/>
-    <tableColumn id="7" xr3:uid="{70C60707-1493-4007-90DF-8D1A8171AA79}" name="EnemyGoldRate : long" dataDxfId="0" totalsRowDxfId="8"/>
-    <tableColumn id="8" xr3:uid="{A1894453-017C-4920-B6D4-6CCC399479DE}" name="EnemySpawnCount : Int" dataDxfId="1" totalsRowDxfId="7"/>
-    <tableColumn id="2" xr3:uid="{27B9ED74-E3F2-4B5B-AF69-453766BB11DC}" name="IdleGoldReward : Int" dataDxfId="16" totalsRowDxfId="6"/>
+    <tableColumn id="1" xr3:uid="{ABEFAF0D-3E9C-4BC0-BD85-867C72E372D9}" name="Index : Int" dataDxfId="18" totalsRowDxfId="17"/>
+    <tableColumn id="4" xr3:uid="{9A52DE84-B46A-41BA-9891-9221E6FD8CA2}" name="StageConfig : String" dataDxfId="16" totalsRowDxfId="15"/>
+    <tableColumn id="5" xr3:uid="{52BABBB3-0B5B-4EA5-A096-52FE17505682}" name="StageBackground : String" dataDxfId="14" totalsRowDxfId="13"/>
+    <tableColumn id="6" xr3:uid="{8CB87B44-9BE8-4447-B7A9-5AB6AF555193}" name="EnemyHpRate : long" dataDxfId="12" totalsRowDxfId="11"/>
+    <tableColumn id="3" xr3:uid="{D9A76B69-1806-4056-859C-537F7DF173E6}" name="EnemyAttackRate : long" dataDxfId="10" totalsRowDxfId="9"/>
+    <tableColumn id="7" xr3:uid="{70C60707-1493-4007-90DF-8D1A8171AA79}" name="EnemyGoldRate : long" dataDxfId="8" totalsRowDxfId="7"/>
+    <tableColumn id="8" xr3:uid="{A1894453-017C-4920-B6D4-6CCC399479DE}" name="EnemySpawnCount : Int" dataDxfId="6" totalsRowDxfId="5"/>
+    <tableColumn id="2" xr3:uid="{27B9ED74-E3F2-4B5B-AF69-453766BB11DC}" name="IdleGoldReward : Int" dataDxfId="4" totalsRowDxfId="3"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleMedium6" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
 </file>
 
 <file path=xl/tables/table2.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="3" xr:uid="{35A1E681-9A85-48AE-96D7-A93EDF20787E}" name="표1_4" displayName="표1_4" ref="A2:B6" totalsRowShown="0" headerRowDxfId="15">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="3" xr:uid="{35A1E681-9A85-48AE-96D7-A93EDF20787E}" name="표1_4" displayName="표1_4" ref="A2:B6" totalsRowShown="0" headerRowDxfId="2">
   <autoFilter ref="A2:B6" xr:uid="{35A1E681-9A85-48AE-96D7-A93EDF20787E}"/>
   <tableColumns count="2">
-    <tableColumn id="1" xr3:uid="{BE9E670A-5042-4FEB-9281-05CB3F81C035}" name="Index : Int" dataDxfId="14"/>
-    <tableColumn id="4" xr3:uid="{0BE49A32-760A-4534-B1B8-33AAC060FE89}" name="UIText : String" dataDxfId="13"/>
+    <tableColumn id="1" xr3:uid="{BE9E670A-5042-4FEB-9281-05CB3F81C035}" name="Index : Int" dataDxfId="1"/>
+    <tableColumn id="4" xr3:uid="{0BE49A32-760A-4534-B1B8-33AAC060FE89}" name="UIText : String" dataDxfId="0"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleMedium6" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
@@ -616,8 +616,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:H302"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="E2" sqref="E2"/>
+    <sheetView tabSelected="1" topLeftCell="A5" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="E12" sqref="E12"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="16.5" x14ac:dyDescent="0.3"/>
@@ -743,7 +743,7 @@
       </c>
       <c r="C6" s="2"/>
       <c r="D6" s="5">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="E6" s="5">
         <v>8</v>
@@ -767,7 +767,7 @@
       </c>
       <c r="C7" s="2"/>
       <c r="D7" s="5">
-        <v>11</v>
+        <v>9</v>
       </c>
       <c r="E7" s="5">
         <v>9</v>
@@ -791,7 +791,7 @@
       </c>
       <c r="C8" s="2"/>
       <c r="D8" s="5">
-        <v>16</v>
+        <v>13</v>
       </c>
       <c r="E8" s="5">
         <v>11</v>
@@ -815,7 +815,7 @@
       </c>
       <c r="C9" s="2"/>
       <c r="D9" s="5">
-        <v>24</v>
+        <v>19</v>
       </c>
       <c r="E9" s="5">
         <v>13</v>
@@ -914,7 +914,7 @@
         <v>127</v>
       </c>
       <c r="E13" s="5">
-        <v>24</v>
+        <v>30</v>
       </c>
       <c r="F13" s="5">
         <v>13</v>
@@ -938,7 +938,7 @@
         <v>190</v>
       </c>
       <c r="E14" s="5">
-        <v>27</v>
+        <v>39</v>
       </c>
       <c r="F14" s="5">
         <v>14</v>
@@ -962,7 +962,7 @@
         <v>285</v>
       </c>
       <c r="E15" s="5">
-        <v>29</v>
+        <v>48</v>
       </c>
       <c r="F15" s="5">
         <v>15</v>
@@ -983,10 +983,10 @@
       </c>
       <c r="C16" s="2"/>
       <c r="D16" s="5">
-        <v>427</v>
+        <v>364</v>
       </c>
       <c r="E16" s="5">
-        <v>33</v>
+        <v>59</v>
       </c>
       <c r="F16" s="5">
         <v>16</v>
@@ -1007,10 +1007,10 @@
       </c>
       <c r="C17" s="2"/>
       <c r="D17" s="5">
-        <v>640</v>
+        <v>448</v>
       </c>
       <c r="E17" s="5">
-        <v>37</v>
+        <v>68</v>
       </c>
       <c r="F17" s="5">
         <v>17</v>
@@ -1031,10 +1031,10 @@
       </c>
       <c r="C18" s="2"/>
       <c r="D18" s="5">
-        <v>896</v>
+        <v>529</v>
       </c>
       <c r="E18" s="5">
-        <v>40</v>
+        <v>75</v>
       </c>
       <c r="F18" s="5">
         <v>18</v>
@@ -1055,10 +1055,10 @@
       </c>
       <c r="C19" s="2"/>
       <c r="D19" s="5">
-        <v>1164</v>
+        <v>621</v>
       </c>
       <c r="E19" s="5">
-        <v>44</v>
+        <v>88</v>
       </c>
       <c r="F19" s="5">
         <v>19</v>
@@ -1079,10 +1079,10 @@
       </c>
       <c r="C20" s="2"/>
       <c r="D20" s="5">
-        <v>1513</v>
+        <v>756</v>
       </c>
       <c r="E20" s="5">
-        <v>50</v>
+        <v>100</v>
       </c>
       <c r="F20" s="5">
         <v>20</v>
@@ -1103,10 +1103,10 @@
       </c>
       <c r="C21" s="2"/>
       <c r="D21" s="5">
-        <v>1966</v>
+        <v>983</v>
       </c>
       <c r="E21" s="5">
-        <v>55</v>
+        <v>110</v>
       </c>
       <c r="F21" s="5">
         <v>22</v>
@@ -1127,10 +1127,10 @@
       </c>
       <c r="C22" s="2"/>
       <c r="D22" s="5">
-        <v>2555</v>
+        <v>1277</v>
       </c>
       <c r="E22" s="5">
-        <v>61</v>
+        <v>122</v>
       </c>
       <c r="F22" s="5">
         <v>24</v>
@@ -1151,10 +1151,10 @@
       </c>
       <c r="C23" s="2"/>
       <c r="D23" s="5">
-        <v>3321</v>
+        <v>1660</v>
       </c>
       <c r="E23" s="5">
-        <v>67</v>
+        <v>134</v>
       </c>
       <c r="F23" s="5">
         <v>26</v>
@@ -1175,10 +1175,10 @@
       </c>
       <c r="C24" s="2"/>
       <c r="D24" s="5">
-        <v>4317</v>
+        <v>2158</v>
       </c>
       <c r="E24" s="5">
-        <v>74</v>
+        <v>148</v>
       </c>
       <c r="F24" s="5">
         <v>28</v>
@@ -1199,10 +1199,10 @@
       </c>
       <c r="C25" s="2"/>
       <c r="D25" s="5">
-        <v>5612</v>
+        <v>2806</v>
       </c>
       <c r="E25" s="5">
-        <v>82</v>
+        <v>164</v>
       </c>
       <c r="F25" s="5">
         <v>30</v>
@@ -1223,10 +1223,10 @@
       </c>
       <c r="C26" s="2"/>
       <c r="D26" s="5">
-        <v>7295</v>
+        <v>3647</v>
       </c>
       <c r="E26" s="5">
-        <v>91</v>
+        <v>182</v>
       </c>
       <c r="F26" s="5">
         <v>33</v>
@@ -1247,10 +1247,10 @@
       </c>
       <c r="C27" s="2"/>
       <c r="D27" s="5">
-        <v>9483</v>
+        <v>4741</v>
       </c>
       <c r="E27" s="5">
-        <v>99</v>
+        <v>198</v>
       </c>
       <c r="F27" s="5">
         <v>36</v>
@@ -1271,10 +1271,10 @@
       </c>
       <c r="C28" s="2"/>
       <c r="D28" s="5">
-        <v>12327</v>
+        <v>6163</v>
       </c>
       <c r="E28" s="5">
-        <v>110</v>
+        <v>220</v>
       </c>
       <c r="F28" s="5">
         <v>39</v>
@@ -1295,10 +1295,10 @@
       </c>
       <c r="C29" s="2"/>
       <c r="D29" s="5">
-        <v>16025</v>
+        <v>8012</v>
       </c>
       <c r="E29" s="5">
-        <v>121</v>
+        <v>242</v>
       </c>
       <c r="F29" s="5">
         <v>42</v>
@@ -1319,10 +1319,10 @@
       </c>
       <c r="C30" s="2"/>
       <c r="D30" s="5">
-        <v>20832</v>
+        <v>10416</v>
       </c>
       <c r="E30" s="5">
-        <v>132</v>
+        <v>264</v>
       </c>
       <c r="F30" s="5">
         <v>46</v>
@@ -1343,10 +1343,10 @@
       </c>
       <c r="C31" s="2"/>
       <c r="D31" s="5">
-        <v>27081</v>
+        <v>13540</v>
       </c>
       <c r="E31" s="5">
-        <v>144</v>
+        <v>288</v>
       </c>
       <c r="F31" s="5">
         <v>50</v>
@@ -1367,10 +1367,10 @@
       </c>
       <c r="C32" s="2"/>
       <c r="D32" s="5">
-        <v>35205</v>
+        <v>17602</v>
       </c>
       <c r="E32" s="5">
-        <v>166</v>
+        <v>332</v>
       </c>
       <c r="F32" s="5">
         <v>55</v>
@@ -1391,10 +1391,10 @@
       </c>
       <c r="C33" s="2"/>
       <c r="D33" s="5">
-        <v>42246</v>
+        <v>21123</v>
       </c>
       <c r="E33" s="5">
-        <v>182</v>
+        <v>364</v>
       </c>
       <c r="F33" s="5">
         <v>60</v>
@@ -1415,10 +1415,10 @@
       </c>
       <c r="C34" s="2"/>
       <c r="D34" s="5">
-        <v>50695</v>
+        <v>25347</v>
       </c>
       <c r="E34" s="5">
-        <v>198</v>
+        <v>396</v>
       </c>
       <c r="F34" s="5">
         <v>66</v>
@@ -1439,10 +1439,10 @@
       </c>
       <c r="C35" s="2"/>
       <c r="D35" s="5">
-        <v>60834</v>
+        <v>30417</v>
       </c>
       <c r="E35" s="5">
-        <v>215</v>
+        <v>430</v>
       </c>
       <c r="F35" s="5">
         <v>72</v>
@@ -1463,10 +1463,10 @@
       </c>
       <c r="C36" s="2"/>
       <c r="D36" s="5">
-        <v>73000</v>
+        <v>36500</v>
       </c>
       <c r="E36" s="5">
-        <v>235</v>
+        <v>470</v>
       </c>
       <c r="F36" s="5">
         <v>79</v>
@@ -1487,10 +1487,10 @@
       </c>
       <c r="C37" s="2"/>
       <c r="D37" s="5">
-        <v>87600</v>
+        <v>43800</v>
       </c>
       <c r="E37" s="5">
-        <v>256</v>
+        <v>512</v>
       </c>
       <c r="F37" s="5">
         <v>86</v>
@@ -1511,10 +1511,10 @@
       </c>
       <c r="C38" s="2"/>
       <c r="D38" s="5">
-        <v>105120</v>
+        <v>52560</v>
       </c>
       <c r="E38" s="5">
-        <v>277</v>
+        <v>554</v>
       </c>
       <c r="F38" s="5">
         <v>94</v>
@@ -1535,10 +1535,10 @@
       </c>
       <c r="C39" s="2"/>
       <c r="D39" s="5">
-        <v>126144</v>
+        <v>63072</v>
       </c>
       <c r="E39" s="5">
-        <v>300</v>
+        <v>600</v>
       </c>
       <c r="F39" s="5">
         <v>103</v>
@@ -1559,10 +1559,10 @@
       </c>
       <c r="C40" s="2"/>
       <c r="D40" s="5">
-        <v>151372</v>
+        <v>75686</v>
       </c>
       <c r="E40" s="5">
-        <v>326</v>
+        <v>652</v>
       </c>
       <c r="F40" s="5">
         <v>113</v>
@@ -1583,10 +1583,10 @@
       </c>
       <c r="C41" s="2"/>
       <c r="D41" s="5">
-        <v>181646</v>
+        <v>90823</v>
       </c>
       <c r="E41" s="5">
-        <v>353</v>
+        <v>706</v>
       </c>
       <c r="F41" s="5">
         <v>124</v>
@@ -1607,10 +1607,10 @@
       </c>
       <c r="C42" s="2"/>
       <c r="D42" s="5">
-        <v>217975</v>
+        <v>108987</v>
       </c>
       <c r="E42" s="5">
-        <v>397</v>
+        <v>794</v>
       </c>
       <c r="F42" s="5">
         <v>136</v>
@@ -1631,10 +1631,10 @@
       </c>
       <c r="C43" s="2"/>
       <c r="D43" s="5">
-        <v>261570</v>
+        <v>130785</v>
       </c>
       <c r="E43" s="5">
-        <v>428</v>
+        <v>856</v>
       </c>
       <c r="F43" s="5">
         <v>149</v>
@@ -1655,10 +1655,10 @@
       </c>
       <c r="C44" s="2"/>
       <c r="D44" s="5">
-        <v>313884</v>
+        <v>156942</v>
       </c>
       <c r="E44" s="5">
-        <v>463</v>
+        <v>926</v>
       </c>
       <c r="F44" s="5">
         <v>163</v>
@@ -1679,10 +1679,10 @@
       </c>
       <c r="C45" s="2"/>
       <c r="D45" s="5">
-        <v>376660</v>
+        <v>188330</v>
       </c>
       <c r="E45" s="5">
-        <v>499</v>
+        <v>998</v>
       </c>
       <c r="F45" s="5">
         <v>179</v>
@@ -1703,10 +1703,10 @@
       </c>
       <c r="C46" s="2"/>
       <c r="D46" s="5">
-        <v>451992</v>
+        <v>225996</v>
       </c>
       <c r="E46" s="5">
-        <v>536</v>
+        <v>1072</v>
       </c>
       <c r="F46" s="5">
         <v>196</v>
@@ -1727,10 +1727,10 @@
       </c>
       <c r="C47" s="2"/>
       <c r="D47" s="5">
-        <v>542390</v>
+        <v>271195</v>
       </c>
       <c r="E47" s="5">
-        <v>575</v>
+        <v>1150</v>
       </c>
       <c r="F47" s="5">
         <v>215</v>
@@ -1751,10 +1751,10 @@
       </c>
       <c r="C48" s="2"/>
       <c r="D48" s="5">
-        <v>650868</v>
+        <v>325434</v>
       </c>
       <c r="E48" s="5">
-        <v>618</v>
+        <v>1236</v>
       </c>
       <c r="F48" s="5">
         <v>236</v>
@@ -1775,10 +1775,10 @@
       </c>
       <c r="C49" s="2"/>
       <c r="D49" s="5">
-        <v>781041</v>
+        <v>390520</v>
       </c>
       <c r="E49" s="5">
-        <v>664</v>
+        <v>1328</v>
       </c>
       <c r="F49" s="5">
         <v>259</v>
@@ -1799,10 +1799,10 @@
       </c>
       <c r="C50" s="2"/>
       <c r="D50" s="5">
-        <v>937249</v>
+        <v>468624</v>
       </c>
       <c r="E50" s="5">
-        <v>711</v>
+        <v>1422</v>
       </c>
       <c r="F50" s="5">
         <v>284</v>
@@ -1823,10 +1823,10 @@
       </c>
       <c r="C51" s="2"/>
       <c r="D51" s="5">
-        <v>1124698</v>
+        <v>562349</v>
       </c>
       <c r="E51" s="5">
-        <v>759</v>
+        <v>1518</v>
       </c>
       <c r="F51" s="5">
         <v>312</v>
@@ -1847,10 +1847,10 @@
       </c>
       <c r="C52" s="2"/>
       <c r="D52" s="5">
-        <v>1349637</v>
+        <v>674818</v>
       </c>
       <c r="E52" s="5">
-        <v>1048</v>
+        <v>2096</v>
       </c>
       <c r="F52" s="5">
         <v>343</v>
@@ -1871,10 +1871,10 @@
       </c>
       <c r="C53" s="2"/>
       <c r="D53" s="5">
-        <v>1619564</v>
+        <v>809782</v>
       </c>
       <c r="E53" s="5">
-        <v>1120</v>
+        <v>2240</v>
       </c>
       <c r="F53" s="5">
         <v>377</v>
@@ -1895,10 +1895,10 @@
       </c>
       <c r="C54" s="2"/>
       <c r="D54" s="5">
-        <v>1943476</v>
+        <v>971738</v>
       </c>
       <c r="E54" s="5">
-        <v>1195</v>
+        <v>2390</v>
       </c>
       <c r="F54" s="5">
         <v>414</v>
@@ -1919,10 +1919,10 @@
       </c>
       <c r="C55" s="2"/>
       <c r="D55" s="5">
-        <v>2332171</v>
+        <v>1166085</v>
       </c>
       <c r="E55" s="5">
-        <v>1272</v>
+        <v>2544</v>
       </c>
       <c r="F55" s="5">
         <v>455</v>
@@ -1943,10 +1943,10 @@
       </c>
       <c r="C56" s="2"/>
       <c r="D56" s="5">
-        <v>2798605</v>
+        <v>1399302</v>
       </c>
       <c r="E56" s="5">
-        <v>1357</v>
+        <v>2714</v>
       </c>
       <c r="F56" s="5">
         <v>500</v>
@@ -1967,10 +1967,10 @@
       </c>
       <c r="C57" s="2"/>
       <c r="D57" s="5">
-        <v>3358326</v>
+        <v>1679163</v>
       </c>
       <c r="E57" s="5">
-        <v>1446</v>
+        <v>2892</v>
       </c>
       <c r="F57" s="5">
         <v>550</v>
@@ -1991,10 +1991,10 @@
       </c>
       <c r="C58" s="2"/>
       <c r="D58" s="5">
-        <v>4029991</v>
+        <v>2014995</v>
       </c>
       <c r="E58" s="5">
-        <v>1537</v>
+        <v>3074</v>
       </c>
       <c r="F58" s="5">
         <v>605</v>
@@ -2015,10 +2015,10 @@
       </c>
       <c r="C59" s="2"/>
       <c r="D59" s="5">
-        <v>4835989</v>
+        <v>2417994</v>
       </c>
       <c r="E59" s="5">
-        <v>1631</v>
+        <v>3262</v>
       </c>
       <c r="F59" s="5">
         <v>665</v>
@@ -2039,10 +2039,10 @@
       </c>
       <c r="C60" s="2"/>
       <c r="D60" s="5">
-        <v>5803186</v>
+        <v>2901593</v>
       </c>
       <c r="E60" s="5">
-        <v>1735</v>
+        <v>3470</v>
       </c>
       <c r="F60" s="5">
         <v>731</v>
@@ -2063,10 +2063,10 @@
       </c>
       <c r="C61" s="2"/>
       <c r="D61" s="5">
-        <v>6963823</v>
+        <v>3481911</v>
       </c>
       <c r="E61" s="5">
-        <v>1842</v>
+        <v>3684</v>
       </c>
       <c r="F61" s="5">
         <v>804</v>
@@ -2087,10 +2087,10 @@
       </c>
       <c r="C62" s="2"/>
       <c r="D62" s="5">
-        <v>8356587</v>
+        <v>4178293</v>
       </c>
       <c r="E62" s="5">
-        <v>2027</v>
+        <v>4054</v>
       </c>
       <c r="F62" s="5">
         <v>884</v>
@@ -2111,10 +2111,10 @@
       </c>
       <c r="C63" s="2"/>
       <c r="D63" s="5">
-        <v>10027904</v>
+        <v>5013952</v>
       </c>
       <c r="E63" s="5">
-        <v>2145</v>
+        <v>4290</v>
       </c>
       <c r="F63" s="5">
         <v>972</v>
@@ -2135,10 +2135,10 @@
       </c>
       <c r="C64" s="2"/>
       <c r="D64" s="5">
-        <v>12033484</v>
+        <v>6016742</v>
       </c>
       <c r="E64" s="5">
-        <v>2274</v>
+        <v>4548</v>
       </c>
       <c r="F64" s="5">
         <v>1069</v>
@@ -2159,10 +2159,10 @@
       </c>
       <c r="C65" s="2"/>
       <c r="D65" s="5">
-        <v>14440180</v>
+        <v>7220090</v>
       </c>
       <c r="E65" s="5">
-        <v>2407</v>
+        <v>4814</v>
       </c>
       <c r="F65" s="5">
         <v>1175</v>
@@ -2183,10 +2183,10 @@
       </c>
       <c r="C66" s="2"/>
       <c r="D66" s="5">
-        <v>17328216</v>
+        <v>8664108</v>
       </c>
       <c r="E66" s="5">
-        <v>2544</v>
+        <v>5088</v>
       </c>
       <c r="F66" s="5">
         <v>1292</v>
@@ -2207,10 +2207,10 @@
       </c>
       <c r="C67" s="2"/>
       <c r="D67" s="5">
-        <v>20793859</v>
+        <v>10396929</v>
       </c>
       <c r="E67" s="5">
-        <v>2684</v>
+        <v>5368</v>
       </c>
       <c r="F67" s="5">
         <v>1421</v>
@@ -2231,10 +2231,10 @@
       </c>
       <c r="C68" s="2"/>
       <c r="D68" s="5">
-        <v>24952630</v>
+        <v>12476315</v>
       </c>
       <c r="E68" s="5">
-        <v>2838</v>
+        <v>5676</v>
       </c>
       <c r="F68" s="5">
         <v>1563</v>
@@ -2255,10 +2255,10 @@
       </c>
       <c r="C69" s="2"/>
       <c r="D69" s="5">
-        <v>29943156</v>
+        <v>14971578</v>
       </c>
       <c r="E69" s="5">
-        <v>2995</v>
+        <v>5990</v>
       </c>
       <c r="F69" s="5">
         <v>1719</v>
@@ -2279,10 +2279,10 @@
       </c>
       <c r="C70" s="2"/>
       <c r="D70" s="5">
-        <v>35931787</v>
+        <v>17965893</v>
       </c>
       <c r="E70" s="5">
-        <v>3157</v>
+        <v>6314</v>
       </c>
       <c r="F70" s="5">
         <v>1890</v>
@@ -2303,10 +2303,10 @@
       </c>
       <c r="C71" s="2"/>
       <c r="D71" s="5">
-        <v>43118144</v>
+        <v>21559072</v>
       </c>
       <c r="E71" s="5">
-        <v>3323</v>
+        <v>6646</v>
       </c>
       <c r="F71" s="5">
         <v>2079</v>
@@ -2327,10 +2327,10 @@
       </c>
       <c r="C72" s="2"/>
       <c r="D72" s="5">
-        <v>51741772</v>
+        <v>25870886</v>
       </c>
       <c r="E72" s="5">
-        <v>4247</v>
+        <v>8494</v>
       </c>
       <c r="F72" s="5">
         <v>2286</v>
@@ -2351,10 +2351,10 @@
       </c>
       <c r="C73" s="2"/>
       <c r="D73" s="5">
-        <v>62090126</v>
+        <v>31045063</v>
       </c>
       <c r="E73" s="5">
-        <v>4472</v>
+        <v>8944</v>
       </c>
       <c r="F73" s="5">
         <v>2514</v>
@@ -2375,10 +2375,10 @@
       </c>
       <c r="C74" s="2"/>
       <c r="D74" s="5">
-        <v>74508151</v>
+        <v>37254075</v>
       </c>
       <c r="E74" s="5">
-        <v>4702</v>
+        <v>9404</v>
       </c>
       <c r="F74" s="5">
         <v>2765</v>
@@ -2399,10 +2399,10 @@
       </c>
       <c r="C75" s="2"/>
       <c r="D75" s="5">
-        <v>89409781</v>
+        <v>44704890</v>
       </c>
       <c r="E75" s="5">
-        <v>4938</v>
+        <v>9876</v>
       </c>
       <c r="F75" s="5">
         <v>3041</v>
@@ -2423,10 +2423,10 @@
       </c>
       <c r="C76" s="2"/>
       <c r="D76" s="5">
-        <v>107291737</v>
+        <v>53645868</v>
       </c>
       <c r="E76" s="5">
-        <v>5194</v>
+        <v>10388</v>
       </c>
       <c r="F76" s="5">
         <v>3345</v>
@@ -2447,10 +2447,10 @@
       </c>
       <c r="C77" s="2"/>
       <c r="D77" s="5">
-        <v>128750084</v>
+        <v>64375042</v>
       </c>
       <c r="E77" s="5">
-        <v>5456</v>
+        <v>10912</v>
       </c>
       <c r="F77" s="5">
         <v>3679</v>
@@ -2471,10 +2471,10 @@
       </c>
       <c r="C78" s="2"/>
       <c r="D78" s="5">
-        <v>154500100</v>
+        <v>77250050</v>
       </c>
       <c r="E78" s="5">
-        <v>5724</v>
+        <v>11448</v>
       </c>
       <c r="F78" s="5">
         <v>4046</v>
@@ -2495,10 +2495,10 @@
       </c>
       <c r="C79" s="2"/>
       <c r="D79" s="5">
-        <v>185400120</v>
+        <v>92700060</v>
       </c>
       <c r="E79" s="5">
-        <v>5999</v>
+        <v>11998</v>
       </c>
       <c r="F79" s="5">
         <v>4450</v>
@@ -2519,10 +2519,10 @@
       </c>
       <c r="C80" s="2"/>
       <c r="D80" s="5">
-        <v>222480144</v>
+        <v>111240072</v>
       </c>
       <c r="E80" s="5">
-        <v>6295</v>
+        <v>12590</v>
       </c>
       <c r="F80" s="5">
         <v>4895</v>
@@ -2543,10 +2543,10 @@
       </c>
       <c r="C81" s="2"/>
       <c r="D81" s="5">
-        <v>266976172</v>
+        <v>133488086</v>
       </c>
       <c r="E81" s="5">
-        <v>6598</v>
+        <v>13196</v>
       </c>
       <c r="F81" s="5">
         <v>5384</v>
@@ -2567,10 +2567,10 @@
       </c>
       <c r="C82" s="2"/>
       <c r="D82" s="5">
-        <v>320371406</v>
+        <v>160185703</v>
       </c>
       <c r="E82" s="5">
-        <v>7155</v>
+        <v>14310</v>
       </c>
       <c r="F82" s="5">
         <v>5922</v>
@@ -2591,10 +2591,10 @@
       </c>
       <c r="C83" s="2"/>
       <c r="D83" s="5">
-        <v>384445687</v>
+        <v>192222843</v>
       </c>
       <c r="E83" s="5">
-        <v>7601</v>
+        <v>15202</v>
       </c>
       <c r="F83" s="5">
         <v>7106</v>
@@ -2615,10 +2615,10 @@
       </c>
       <c r="C84" s="2"/>
       <c r="D84" s="5">
-        <v>461334824</v>
+        <v>230667412</v>
       </c>
       <c r="E84" s="5">
-        <v>8060</v>
+        <v>16120</v>
       </c>
       <c r="F84" s="5">
         <v>8527</v>
@@ -2639,10 +2639,10 @@
       </c>
       <c r="C85" s="2"/>
       <c r="D85" s="5">
-        <v>553601788</v>
+        <v>276800894</v>
       </c>
       <c r="E85" s="5">
-        <v>8551</v>
+        <v>17102</v>
       </c>
       <c r="F85" s="5">
         <v>10232</v>
@@ -2663,10 +2663,10 @@
       </c>
       <c r="C86" s="2"/>
       <c r="D86" s="5">
-        <v>664322145</v>
+        <v>332161072</v>
       </c>
       <c r="E86" s="5">
-        <v>9055</v>
+        <v>18110</v>
       </c>
       <c r="F86" s="5">
         <v>12278</v>
@@ -2687,10 +2687,10 @@
       </c>
       <c r="C87" s="2"/>
       <c r="D87" s="5">
-        <v>797186574</v>
+        <v>398593287</v>
       </c>
       <c r="E87" s="5">
-        <v>9575</v>
+        <v>19150</v>
       </c>
       <c r="F87" s="5">
         <v>14733</v>
@@ -2711,10 +2711,10 @@
       </c>
       <c r="C88" s="2"/>
       <c r="D88" s="5">
-        <v>956623888</v>
+        <v>478311944</v>
       </c>
       <c r="E88" s="5">
-        <v>10128</v>
+        <v>20256</v>
       </c>
       <c r="F88" s="5">
         <v>17679</v>
@@ -2735,10 +2735,10 @@
       </c>
       <c r="C89" s="2"/>
       <c r="D89" s="5">
-        <v>1147948665</v>
+        <v>573974332</v>
       </c>
       <c r="E89" s="5">
-        <v>10696</v>
+        <v>21392</v>
       </c>
       <c r="F89" s="5">
         <v>21214</v>
@@ -2759,10 +2759,10 @@
       </c>
       <c r="C90" s="2"/>
       <c r="D90" s="5">
-        <v>1377538398</v>
+        <v>688769199</v>
       </c>
       <c r="E90" s="5">
-        <v>11280</v>
+        <v>22560</v>
       </c>
       <c r="F90" s="5">
         <v>25456</v>
@@ -2783,10 +2783,10 @@
       </c>
       <c r="C91" s="2"/>
       <c r="D91" s="5">
-        <v>1653046077</v>
+        <v>826523038</v>
       </c>
       <c r="E91" s="5">
-        <v>11901</v>
+        <v>23802</v>
       </c>
       <c r="F91" s="5">
         <v>30547</v>
@@ -2807,10 +2807,10 @@
       </c>
       <c r="C92" s="2"/>
       <c r="D92" s="5">
-        <v>1983655292</v>
+        <v>991827646</v>
       </c>
       <c r="E92" s="5">
-        <v>12970</v>
+        <v>25940</v>
       </c>
       <c r="F92" s="5">
         <v>36656</v>
@@ -2831,10 +2831,10 @@
       </c>
       <c r="C93" s="2"/>
       <c r="D93" s="5">
-        <v>2380386350</v>
+        <v>1190193175</v>
       </c>
       <c r="E93" s="5">
-        <v>13646</v>
+        <v>27292</v>
       </c>
       <c r="F93" s="5">
         <v>43987</v>
@@ -2855,10 +2855,10 @@
       </c>
       <c r="C94" s="2"/>
       <c r="D94" s="5">
-        <v>2856463620</v>
+        <v>1428231810</v>
       </c>
       <c r="E94" s="5">
-        <v>14363</v>
+        <v>28726</v>
       </c>
       <c r="F94" s="5">
         <v>52784</v>
@@ -2879,10 +2879,10 @@
       </c>
       <c r="C95" s="2"/>
       <c r="D95" s="5">
-        <v>3427756344</v>
+        <v>1713878172</v>
       </c>
       <c r="E95" s="5">
-        <v>15098</v>
+        <v>30196</v>
       </c>
       <c r="F95" s="5">
         <v>63340</v>
@@ -2903,10 +2903,10 @@
       </c>
       <c r="C96" s="2"/>
       <c r="D96" s="5">
-        <v>4113307612</v>
+        <v>2056653806</v>
       </c>
       <c r="E96" s="5">
-        <v>15851</v>
+        <v>31702</v>
       </c>
       <c r="F96" s="5">
         <v>76008</v>
@@ -2927,10 +2927,10 @@
       </c>
       <c r="C97" s="2"/>
       <c r="D97" s="5">
-        <v>4935969134</v>
+        <v>2467984567</v>
       </c>
       <c r="E97" s="5">
-        <v>16648</v>
+        <v>33296</v>
       </c>
       <c r="F97" s="5">
         <v>91209</v>
@@ -2951,10 +2951,10 @@
       </c>
       <c r="C98" s="2"/>
       <c r="D98" s="5">
-        <v>5923162960</v>
+        <v>2961581480</v>
       </c>
       <c r="E98" s="5">
-        <v>17465</v>
+        <v>34930</v>
       </c>
       <c r="F98" s="5">
         <v>109450</v>
@@ -2975,10 +2975,10 @@
       </c>
       <c r="C99" s="2"/>
       <c r="D99" s="5">
-        <v>7107795552</v>
+        <v>3553897776</v>
       </c>
       <c r="E99" s="5">
-        <v>18301</v>
+        <v>36602</v>
       </c>
       <c r="F99" s="5">
         <v>131340</v>
@@ -2999,10 +2999,10 @@
       </c>
       <c r="C100" s="2"/>
       <c r="D100" s="5">
-        <v>8529354662</v>
+        <v>4264677331</v>
       </c>
       <c r="E100" s="5">
-        <v>19183</v>
+        <v>38366</v>
       </c>
       <c r="F100" s="5">
         <v>157608</v>
@@ -3023,10 +3023,10 @@
       </c>
       <c r="C101" s="2"/>
       <c r="D101" s="5">
-        <v>10235225594</v>
+        <v>5117612797</v>
       </c>
       <c r="E101" s="5">
-        <v>20087</v>
+        <v>40174</v>
       </c>
       <c r="F101" s="5">
         <v>189129</v>
@@ -3048,10 +3048,10 @@
       </c>
       <c r="C102" s="2"/>
       <c r="D102" s="5">
-        <v>12282270712</v>
+        <v>6141135356</v>
       </c>
       <c r="E102" s="5">
-        <v>33245</v>
+        <v>66490</v>
       </c>
       <c r="F102" s="5">
         <v>226954</v>
@@ -3073,10 +3073,10 @@
       </c>
       <c r="C103" s="2"/>
       <c r="D103" s="5">
-        <v>13510497783</v>
+        <v>6755248891</v>
       </c>
       <c r="E103" s="5">
-        <v>34786</v>
+        <v>69572</v>
       </c>
       <c r="F103" s="5">
         <v>272344</v>
@@ -3098,10 +3098,10 @@
       </c>
       <c r="C104" s="2"/>
       <c r="D104" s="5">
-        <v>14861547561</v>
+        <v>7430773780</v>
       </c>
       <c r="E104" s="5">
-        <v>36362</v>
+        <v>72724</v>
       </c>
       <c r="F104" s="5">
         <v>326812</v>
@@ -3123,10 +3123,10 @@
       </c>
       <c r="C105" s="2"/>
       <c r="D105" s="5">
-        <v>16347702317</v>
+        <v>8173851158</v>
       </c>
       <c r="E105" s="5">
-        <v>37973</v>
+        <v>75946</v>
       </c>
       <c r="F105" s="5">
         <v>392174</v>
@@ -3148,10 +3148,10 @@
       </c>
       <c r="C106" s="2"/>
       <c r="D106" s="5">
-        <v>17982472548</v>
+        <v>8991236274</v>
       </c>
       <c r="E106" s="5">
-        <v>39667</v>
+        <v>79334</v>
       </c>
       <c r="F106" s="5">
         <v>470608</v>
@@ -3173,10 +3173,10 @@
       </c>
       <c r="C107" s="2"/>
       <c r="D107" s="5">
-        <v>19780719802</v>
+        <v>9890359901</v>
       </c>
       <c r="E107" s="5">
-        <v>41398</v>
+        <v>82796</v>
       </c>
       <c r="F107" s="5">
         <v>564729</v>
@@ -3198,10 +3198,10 @@
       </c>
       <c r="C108" s="2"/>
       <c r="D108" s="5">
-        <v>21758791782</v>
+        <v>10879395891</v>
       </c>
       <c r="E108" s="5">
-        <v>43167</v>
+        <v>86334</v>
       </c>
       <c r="F108" s="5">
         <v>677674</v>
@@ -3223,10 +3223,10 @@
       </c>
       <c r="C109" s="2"/>
       <c r="D109" s="5">
-        <v>23934670960</v>
+        <v>11967335480</v>
       </c>
       <c r="E109" s="5">
-        <v>45024</v>
+        <v>90048</v>
       </c>
       <c r="F109" s="5">
         <v>813208</v>
@@ -3248,10 +3248,10 @@
       </c>
       <c r="C110" s="2"/>
       <c r="D110" s="5">
-        <v>26328138056</v>
+        <v>13164069028</v>
       </c>
       <c r="E110" s="5">
-        <v>46921</v>
+        <v>93842</v>
       </c>
       <c r="F110" s="5">
         <v>975849</v>
@@ -3273,10 +3273,10 @@
       </c>
       <c r="C111" s="2"/>
       <c r="D111" s="5">
-        <v>28960951861</v>
+        <v>14480475930</v>
       </c>
       <c r="E111" s="5">
-        <v>48856</v>
+        <v>97712</v>
       </c>
       <c r="F111" s="5">
         <v>1171018</v>
@@ -3298,10 +3298,10 @@
       </c>
       <c r="C112" s="2"/>
       <c r="D112" s="5">
-        <v>31857047047</v>
+        <v>15928523523</v>
       </c>
       <c r="E112" s="5">
-        <v>59368</v>
+        <v>118736</v>
       </c>
       <c r="F112" s="5">
         <v>1405221</v>
@@ -3323,10 +3323,10 @@
       </c>
       <c r="C113" s="2"/>
       <c r="D113" s="5">
-        <v>35679892692</v>
+        <v>17839946346</v>
       </c>
       <c r="E113" s="5">
-        <v>61784</v>
+        <v>123568</v>
       </c>
       <c r="F113" s="5">
         <v>1826787</v>
@@ -3348,10 +3348,10 @@
       </c>
       <c r="C114" s="2"/>
       <c r="D114" s="5">
-        <v>39961479815</v>
+        <v>19980739907</v>
       </c>
       <c r="E114" s="5">
-        <v>64249</v>
+        <v>128498</v>
       </c>
       <c r="F114" s="5">
         <v>2374823</v>
@@ -3373,10 +3373,10 @@
       </c>
       <c r="C115" s="2"/>
       <c r="D115" s="5">
-        <v>44756857392</v>
+        <v>22378428696</v>
       </c>
       <c r="E115" s="5">
-        <v>66831</v>
+        <v>133662</v>
       </c>
       <c r="F115" s="5">
         <v>3087269</v>
@@ -3398,10 +3398,10 @@
       </c>
       <c r="C116" s="2"/>
       <c r="D116" s="5">
-        <v>50127680279</v>
+        <v>25063840139</v>
       </c>
       <c r="E116" s="5">
-        <v>69463</v>
+        <v>138926</v>
       </c>
       <c r="F116" s="5">
         <v>4013449</v>
@@ -3423,10 +3423,10 @@
       </c>
       <c r="C117" s="2"/>
       <c r="D117" s="5">
-        <v>56143001912</v>
+        <v>28071500956</v>
       </c>
       <c r="E117" s="5">
-        <v>72147</v>
+        <v>144294</v>
       </c>
       <c r="F117" s="5">
         <v>5217483</v>
@@ -3448,10 +3448,10 @@
       </c>
       <c r="C118" s="2"/>
       <c r="D118" s="5">
-        <v>62880162141</v>
+        <v>31440081070</v>
       </c>
       <c r="E118" s="5">
-        <v>74953</v>
+        <v>149906</v>
       </c>
       <c r="F118" s="5">
         <v>6782727</v>
@@ -3473,10 +3473,10 @@
       </c>
       <c r="C119" s="2"/>
       <c r="D119" s="5">
-        <v>70425781597</v>
+        <v>35212890798</v>
       </c>
       <c r="E119" s="5">
-        <v>77814</v>
+        <v>155628</v>
       </c>
       <c r="F119" s="5">
         <v>8817545</v>
@@ -3498,10 +3498,10 @@
       </c>
       <c r="C120" s="2"/>
       <c r="D120" s="5">
-        <v>78876875388</v>
+        <v>39438437694</v>
       </c>
       <c r="E120" s="5">
-        <v>80728</v>
+        <v>161456</v>
       </c>
       <c r="F120" s="5">
         <v>11462808</v>
@@ -3523,10 +3523,10 @@
       </c>
       <c r="C121" s="2"/>
       <c r="D121" s="5">
-        <v>88342100434</v>
+        <v>44171050217</v>
       </c>
       <c r="E121" s="5">
-        <v>83772</v>
+        <v>167544</v>
       </c>
       <c r="F121" s="5">
         <v>14901650</v>
@@ -3548,10 +3548,10 @@
       </c>
       <c r="C122" s="2"/>
       <c r="D122" s="5">
-        <v>98943152486</v>
+        <v>49471576243</v>
       </c>
       <c r="E122" s="5">
-        <v>99283</v>
+        <v>198566</v>
       </c>
       <c r="F122" s="5">
         <v>19372145</v>
@@ -3573,10 +3573,10 @@
       </c>
       <c r="C123" s="2"/>
       <c r="D123" s="5">
-        <v>110816330784</v>
+        <v>55408165392</v>
       </c>
       <c r="E123" s="5">
-        <v>155717</v>
+        <v>311434</v>
       </c>
       <c r="F123" s="5">
         <v>25183788</v>
@@ -3598,10 +3598,10 @@
       </c>
       <c r="C124" s="2"/>
       <c r="D124" s="5">
-        <v>124114290478</v>
+        <v>62057145239</v>
       </c>
       <c r="E124" s="5">
-        <v>161415</v>
+        <v>322830</v>
       </c>
       <c r="F124" s="5">
         <v>32738924</v>
@@ -3623,10 +3623,10 @@
       </c>
       <c r="C125" s="2"/>
       <c r="D125" s="5">
-        <v>139008005335</v>
+        <v>69504002667</v>
       </c>
       <c r="E125" s="5">
-        <v>167215</v>
+        <v>334430</v>
       </c>
       <c r="F125" s="5">
         <v>42560601</v>
@@ -3648,10 +3648,10 @@
       </c>
       <c r="C126" s="2"/>
       <c r="D126" s="5">
-        <v>155688965975</v>
+        <v>77844482987</v>
       </c>
       <c r="E126" s="5">
-        <v>173118</v>
+        <v>346236</v>
       </c>
       <c r="F126" s="5">
         <v>55328781</v>
@@ -3673,10 +3673,10 @@
       </c>
       <c r="C127" s="2"/>
       <c r="D127" s="5">
-        <v>174371641892</v>
+        <v>87185820946</v>
       </c>
       <c r="E127" s="5">
-        <v>179270</v>
+        <v>358540</v>
       </c>
       <c r="F127" s="5">
         <v>71927415</v>
@@ -3698,10 +3698,10 @@
       </c>
       <c r="C128" s="2"/>
       <c r="D128" s="5">
-        <v>195296238919</v>
+        <v>97648119459</v>
       </c>
       <c r="E128" s="5">
-        <v>185530</v>
+        <v>371060</v>
       </c>
       <c r="F128" s="5">
         <v>93505639</v>
@@ -3723,10 +3723,10 @@
       </c>
       <c r="C129" s="2"/>
       <c r="D129" s="5">
-        <v>218731787589</v>
+        <v>109365893794</v>
       </c>
       <c r="E129" s="5">
-        <v>191897</v>
+        <v>383794</v>
       </c>
       <c r="F129" s="5">
         <v>121557330</v>
@@ -3748,10 +3748,10 @@
       </c>
       <c r="C130" s="2"/>
       <c r="D130" s="5">
-        <v>244979602099</v>
+        <v>122489801049</v>
       </c>
       <c r="E130" s="5">
-        <v>198528</v>
+        <v>397056</v>
       </c>
       <c r="F130" s="5">
         <v>158024529</v>
@@ -3773,10 +3773,10 @@
       </c>
       <c r="C131" s="2"/>
       <c r="D131" s="5">
-        <v>274377154350</v>
+        <v>137188577175</v>
       </c>
       <c r="E131" s="5">
-        <v>205271</v>
+        <v>410542</v>
       </c>
       <c r="F131" s="5">
         <v>205431887</v>
@@ -3798,10 +3798,10 @@
       </c>
       <c r="C132" s="2"/>
       <c r="D132" s="5">
-        <v>307302412872</v>
+        <v>153651206436</v>
       </c>
       <c r="E132" s="5">
-        <v>238642</v>
+        <v>477284</v>
       </c>
       <c r="F132" s="5">
         <v>267061453</v>
@@ -3823,10 +3823,10 @@
       </c>
       <c r="C133" s="2"/>
       <c r="D133" s="5">
-        <v>344178702416</v>
+        <v>172089351208</v>
       </c>
       <c r="E133" s="5">
-        <v>246664</v>
+        <v>493328</v>
       </c>
       <c r="F133" s="5">
         <v>347179888</v>
@@ -3848,10 +3848,10 @@
       </c>
       <c r="C134" s="2"/>
       <c r="D134" s="5">
-        <v>385480146705</v>
+        <v>192740073352</v>
       </c>
       <c r="E134" s="5">
-        <v>254820</v>
+        <v>509640</v>
       </c>
       <c r="F134" s="5">
         <v>451333854</v>
@@ -3873,10 +3873,10 @@
       </c>
       <c r="C135" s="2"/>
       <c r="D135" s="5">
-        <v>431737764309</v>
+        <v>215868882154</v>
       </c>
       <c r="E135" s="5">
-        <v>263108</v>
+        <v>526216</v>
       </c>
       <c r="F135" s="5">
         <v>586734010</v>
@@ -3898,10 +3898,10 @@
       </c>
       <c r="C136" s="2"/>
       <c r="D136" s="5">
-        <v>483546296026</v>
+        <v>241773148013</v>
       </c>
       <c r="E136" s="5">
-        <v>271721</v>
+        <v>543442</v>
       </c>
       <c r="F136" s="5">
         <v>762754213</v>
@@ -3923,10 +3923,10 @@
       </c>
       <c r="C137" s="2"/>
       <c r="D137" s="5">
-        <v>541571851549</v>
+        <v>270785925774</v>
       </c>
       <c r="E137" s="5">
-        <v>280473</v>
+        <v>560946</v>
       </c>
       <c r="F137" s="5">
         <v>991580476</v>
@@ -3948,10 +3948,10 @@
       </c>
       <c r="C138" s="2"/>
       <c r="D138" s="5">
-        <v>606560473734</v>
+        <v>303280236867</v>
       </c>
       <c r="E138" s="5">
-        <v>289364</v>
+        <v>578728</v>
       </c>
       <c r="F138" s="5">
         <v>1289054618</v>
@@ -3973,10 +3973,10 @@
       </c>
       <c r="C139" s="2"/>
       <c r="D139" s="5">
-        <v>679347730582</v>
+        <v>339673865291</v>
       </c>
       <c r="E139" s="5">
-        <v>298596</v>
+        <v>597192</v>
       </c>
       <c r="F139" s="5">
         <v>1675771003</v>
@@ -3998,10 +3998,10 @@
       </c>
       <c r="C140" s="2"/>
       <c r="D140" s="5">
-        <v>760869458251</v>
+        <v>380434729125</v>
       </c>
       <c r="E140" s="5">
-        <v>307973</v>
+        <v>615946</v>
       </c>
       <c r="F140" s="5">
         <v>2178502303</v>
@@ -4023,10 +4023,10 @@
       </c>
       <c r="C141" s="2"/>
       <c r="D141" s="5">
-        <v>852173793241</v>
+        <v>426086896620</v>
       </c>
       <c r="E141" s="5">
-        <v>317495</v>
+        <v>634990</v>
       </c>
       <c r="F141" s="5">
         <v>2832052993</v>
@@ -4048,10 +4048,10 @@
       </c>
       <c r="C142" s="2"/>
       <c r="D142" s="5">
-        <v>954434648429</v>
+        <v>477217324214</v>
       </c>
       <c r="E142" s="5">
-        <v>363748</v>
+        <v>727496</v>
       </c>
       <c r="F142" s="5">
         <v>3681668890</v>
@@ -4073,10 +4073,10 @@
       </c>
       <c r="C143" s="2"/>
       <c r="D143" s="5">
-        <v>1068966806240</v>
+        <v>534483403120</v>
       </c>
       <c r="E143" s="5">
-        <v>502073</v>
+        <v>1004146</v>
       </c>
       <c r="F143" s="5">
         <v>4786169557</v>
@@ -4098,10 +4098,10 @@
       </c>
       <c r="C144" s="2"/>
       <c r="D144" s="5">
-        <v>1197242822988</v>
+        <v>598621411494</v>
       </c>
       <c r="E144" s="5">
-        <v>517223</v>
+        <v>1034446</v>
       </c>
       <c r="F144" s="5">
         <v>6222020424</v>
@@ -4123,10 +4123,10 @@
       </c>
       <c r="C145" s="2"/>
       <c r="D145" s="5">
-        <v>1340911961746</v>
+        <v>670455980873</v>
       </c>
       <c r="E145" s="5">
-        <v>532927</v>
+        <v>1065854</v>
       </c>
       <c r="F145" s="5">
         <v>8088626551</v>
@@ -4148,10 +4148,10 @@
       </c>
       <c r="C146" s="2"/>
       <c r="D146" s="5">
-        <v>1501821397155</v>
+        <v>750910698577</v>
       </c>
       <c r="E146" s="5">
-        <v>548867</v>
+        <v>1097734</v>
       </c>
       <c r="F146" s="5">
         <v>10515214516</v>
@@ -4173,10 +4173,10 @@
       </c>
       <c r="C147" s="2"/>
       <c r="D147" s="5">
-        <v>1682039964813</v>
+        <v>841019982406</v>
       </c>
       <c r="E147" s="5">
-        <v>565041</v>
+        <v>1130082</v>
       </c>
       <c r="F147" s="5">
         <v>13669778870</v>
@@ -4198,10 +4198,10 @@
       </c>
       <c r="C148" s="2"/>
       <c r="D148" s="5">
-        <v>1883884760590</v>
+        <v>941942380295</v>
       </c>
       <c r="E148" s="5">
-        <v>581795</v>
+        <v>1163590</v>
       </c>
       <c r="F148" s="5">
         <v>17770712531</v>
@@ -4223,10 +4223,10 @@
       </c>
       <c r="C149" s="2"/>
       <c r="D149" s="5">
-        <v>2109950931860</v>
+        <v>1054975465930</v>
       </c>
       <c r="E149" s="5">
-        <v>598793</v>
+        <v>1197586</v>
       </c>
       <c r="F149" s="5">
         <v>23101926290</v>
@@ -4248,10 +4248,10 @@
       </c>
       <c r="C150" s="2"/>
       <c r="D150" s="5">
-        <v>2363145043683</v>
+        <v>1181572521841</v>
       </c>
       <c r="E150" s="5">
-        <v>616036</v>
+        <v>1232072</v>
       </c>
       <c r="F150" s="5">
         <v>30032504177</v>
@@ -4273,10 +4273,10 @@
       </c>
       <c r="C151" s="2"/>
       <c r="D151" s="5">
-        <v>2646722448924</v>
+        <v>1323361224462</v>
       </c>
       <c r="E151" s="5">
-        <v>633883</v>
+        <v>1267766</v>
       </c>
       <c r="F151" s="5">
         <v>39042255430</v>
@@ -4298,10 +4298,10 @@
       </c>
       <c r="C152" s="2"/>
       <c r="D152" s="5">
-        <v>2964329142794</v>
+        <v>1482164571397</v>
       </c>
       <c r="E152" s="5">
-        <v>717183</v>
+        <v>1434366</v>
       </c>
       <c r="F152" s="5">
         <v>50754932059</v>
@@ -4323,10 +4323,10 @@
       </c>
       <c r="C153" s="2"/>
       <c r="D153" s="5">
-        <v>3320048639929</v>
+        <v>1660024319964</v>
       </c>
       <c r="E153" s="5">
-        <v>737375</v>
+        <v>1474750</v>
       </c>
       <c r="F153" s="5">
         <v>65981411676</v>
@@ -4348,10 +4348,10 @@
       </c>
       <c r="C154" s="2"/>
       <c r="D154" s="5">
-        <v>3718454476720</v>
+        <v>1859227238360</v>
       </c>
       <c r="E154" s="5">
-        <v>758260</v>
+        <v>1516520</v>
       </c>
       <c r="F154" s="5">
         <v>85775835178</v>
@@ -4373,10 +4373,10 @@
       </c>
       <c r="C155" s="2"/>
       <c r="D155" s="5">
-        <v>4164669013926</v>
+        <v>2082334506963</v>
       </c>
       <c r="E155" s="5">
-        <v>779437</v>
+        <v>1558874</v>
       </c>
       <c r="F155" s="5">
         <v>111508585731</v>
@@ -4398,10 +4398,10 @@
       </c>
       <c r="C156" s="2"/>
       <c r="D156" s="5">
-        <v>4664429295597</v>
+        <v>2332214647798</v>
       </c>
       <c r="E156" s="5">
-        <v>800905</v>
+        <v>1601810</v>
       </c>
       <c r="F156" s="5">
         <v>144961161450</v>
@@ -4423,10 +4423,10 @@
       </c>
       <c r="C157" s="2"/>
       <c r="D157" s="5">
-        <v>5224160811068</v>
+        <v>2612080405534</v>
       </c>
       <c r="E157" s="5">
-        <v>823095</v>
+        <v>1646190</v>
       </c>
       <c r="F157" s="5">
         <v>188449509885</v>
@@ -4448,10 +4448,10 @@
       </c>
       <c r="C158" s="2"/>
       <c r="D158" s="5">
-        <v>5851060108396</v>
+        <v>2925530054198</v>
       </c>
       <c r="E158" s="5">
-        <v>845587</v>
+        <v>1691174</v>
       </c>
       <c r="F158" s="5">
         <v>244984362850</v>
@@ -4473,10 +4473,10 @@
       </c>
       <c r="C159" s="2"/>
       <c r="D159" s="5">
-        <v>6553187321403</v>
+        <v>3276593660701</v>
       </c>
       <c r="E159" s="5">
-        <v>868383</v>
+        <v>1736766</v>
       </c>
       <c r="F159" s="5">
         <v>318479671705</v>
@@ -4498,10 +4498,10 @@
       </c>
       <c r="C160" s="2"/>
       <c r="D160" s="5">
-        <v>7339569799971</v>
+        <v>3669784899985</v>
       </c>
       <c r="E160" s="5">
-        <v>891929</v>
+        <v>1783858</v>
       </c>
       <c r="F160" s="5">
         <v>414023573216</v>
@@ -4523,10 +4523,10 @@
       </c>
       <c r="C161" s="2"/>
       <c r="D161" s="5">
-        <v>8220318175967</v>
+        <v>4110159087983</v>
       </c>
       <c r="E161" s="5">
-        <v>915790</v>
+        <v>1831580</v>
       </c>
       <c r="F161" s="5">
         <v>538230645180</v>
@@ -4548,10 +4548,10 @@
       </c>
       <c r="C162" s="2"/>
       <c r="D162" s="5">
-        <v>9206756357083</v>
+        <v>4603378178541</v>
       </c>
       <c r="E162" s="5">
-        <v>1697711</v>
+        <v>3395422</v>
       </c>
       <c r="F162" s="5">
         <v>699699838734</v>
@@ -4573,10 +4573,10 @@
       </c>
       <c r="C163" s="2"/>
       <c r="D163" s="5">
-        <v>10311567119933</v>
+        <v>5155783559966</v>
       </c>
       <c r="E163" s="5">
-        <v>1742785</v>
+        <v>3485570</v>
       </c>
       <c r="F163" s="5">
         <v>979579774227</v>
@@ -4598,10 +4598,10 @@
       </c>
       <c r="C164" s="2"/>
       <c r="D164" s="5">
-        <v>11548955174325</v>
+        <v>5774477587162</v>
       </c>
       <c r="E164" s="5">
-        <v>1788450</v>
+        <v>3576900</v>
       </c>
       <c r="F164" s="5">
         <v>1371411683917</v>
@@ -4623,10 +4623,10 @@
       </c>
       <c r="C165" s="2"/>
       <c r="D165" s="5">
-        <v>12934829795244</v>
+        <v>6467414897622</v>
       </c>
       <c r="E165" s="5">
-        <v>1834705</v>
+        <v>3669410</v>
       </c>
       <c r="F165" s="5">
         <v>1919976357483</v>
@@ -4648,10 +4648,10 @@
       </c>
       <c r="C166" s="2"/>
       <c r="D166" s="5">
-        <v>14487009370673</v>
+        <v>7243504685336</v>
       </c>
       <c r="E166" s="5">
-        <v>1882424</v>
+        <v>3764848</v>
       </c>
       <c r="F166" s="5">
         <v>2687966900476</v>
@@ -4673,10 +4673,10 @@
       </c>
       <c r="C167" s="2"/>
       <c r="D167" s="5">
-        <v>16225450495153</v>
+        <v>8112725247576</v>
       </c>
       <c r="E167" s="5">
-        <v>1930755</v>
+        <v>3861510</v>
       </c>
       <c r="F167" s="5">
         <v>3763153660666</v>
@@ -4698,10 +4698,10 @@
       </c>
       <c r="C168" s="2"/>
       <c r="D168" s="5">
-        <v>18172504554571</v>
+        <v>9086252277285</v>
       </c>
       <c r="E168" s="5">
-        <v>1979699</v>
+        <v>3959398</v>
       </c>
       <c r="F168" s="5">
         <v>5268415124932</v>
@@ -4723,10 +4723,10 @@
       </c>
       <c r="C169" s="2"/>
       <c r="D169" s="5">
-        <v>20353205101119</v>
+        <v>10176602550559</v>
       </c>
       <c r="E169" s="5">
-        <v>2030162</v>
+        <v>4060324</v>
       </c>
       <c r="F169" s="5">
         <v>7375781174904</v>
@@ -4748,10 +4748,10 @@
       </c>
       <c r="C170" s="2"/>
       <c r="D170" s="5">
-        <v>22795589713253</v>
+        <v>11397794856626</v>
       </c>
       <c r="E170" s="5">
-        <v>2081260</v>
+        <v>4162520</v>
       </c>
       <c r="F170" s="5">
         <v>10326093644865</v>
@@ -4773,10 +4773,10 @@
       </c>
       <c r="C171" s="2"/>
       <c r="D171" s="5">
-        <v>25531060478843</v>
+        <v>12765530239421</v>
       </c>
       <c r="E171" s="5">
-        <v>2132993</v>
+        <v>4265986</v>
       </c>
       <c r="F171" s="5">
         <v>14456531102811</v>
@@ -4798,10 +4798,10 @@
       </c>
       <c r="C172" s="2"/>
       <c r="D172" s="5">
-        <v>28594787736304</v>
+        <v>14297393868152</v>
       </c>
       <c r="E172" s="5">
-        <v>2368494</v>
+        <v>4736988</v>
       </c>
       <c r="F172" s="5">
         <v>20239143543935</v>
@@ -4823,10 +4823,10 @@
       </c>
       <c r="C173" s="2"/>
       <c r="D173" s="5">
-        <v>32026162264660</v>
+        <v>16013081132330</v>
       </c>
       <c r="E173" s="5">
-        <v>2426958</v>
+        <v>4853916</v>
       </c>
       <c r="F173" s="5">
         <v>28334800961509</v>
@@ -4848,10 +4848,10 @@
       </c>
       <c r="C174" s="2"/>
       <c r="D174" s="5">
-        <v>35869301736419</v>
+        <v>17934650868209</v>
       </c>
       <c r="E174" s="5">
-        <v>2486135</v>
+        <v>4972270</v>
       </c>
       <c r="F174" s="5">
         <v>39668721346112</v>
@@ -4873,10 +4873,10 @@
       </c>
       <c r="C175" s="2"/>
       <c r="D175" s="5">
-        <v>40173617944789</v>
+        <v>20086808972394</v>
       </c>
       <c r="E175" s="5">
-        <v>2547082</v>
+        <v>5094164</v>
       </c>
       <c r="F175" s="5">
         <v>55536209884556</v>
@@ -4898,10 +4898,10 @@
       </c>
       <c r="C176" s="2"/>
       <c r="D176" s="5">
-        <v>44994452098163</v>
+        <v>22497226049081</v>
       </c>
       <c r="E176" s="5">
-        <v>2608766</v>
+        <v>5217532</v>
       </c>
       <c r="F176" s="5">
         <v>77750693838378</v>
@@ -4923,10 +4923,10 @@
       </c>
       <c r="C177" s="2"/>
       <c r="D177" s="5">
-        <v>50393786349942</v>
+        <v>25196893174971</v>
       </c>
       <c r="E177" s="5">
-        <v>2671189</v>
+        <v>5342378</v>
       </c>
       <c r="F177" s="5">
         <v>108850971373729</v>
@@ -4948,10 +4948,10 @@
       </c>
       <c r="C178" s="2"/>
       <c r="D178" s="5">
-        <v>56441040711935</v>
+        <v>28220520355967</v>
       </c>
       <c r="E178" s="5">
-        <v>2735445</v>
+        <v>5470890</v>
       </c>
       <c r="F178" s="5">
         <v>152391359923221</v>
@@ -4973,10 +4973,10 @@
       </c>
       <c r="C179" s="2"/>
       <c r="D179" s="5">
-        <v>63213965597367</v>
+        <v>31606982798683</v>
       </c>
       <c r="E179" s="5">
-        <v>2800465</v>
+        <v>5600930</v>
       </c>
       <c r="F179" s="5">
         <v>213347903892509</v>
@@ -4998,10 +4998,10 @@
       </c>
       <c r="C180" s="2"/>
       <c r="D180" s="5">
-        <v>70799641469051</v>
+        <v>35399820734525</v>
       </c>
       <c r="E180" s="5">
-        <v>2866248</v>
+        <v>5732496</v>
       </c>
       <c r="F180" s="5">
         <v>298687065449513</v>
@@ -5023,10 +5023,10 @@
       </c>
       <c r="C181" s="2"/>
       <c r="D181" s="5">
-        <v>79295598445337</v>
+        <v>39647799222668</v>
       </c>
       <c r="E181" s="5">
-        <v>2933930</v>
+        <v>5867860</v>
       </c>
       <c r="F181" s="5">
         <v>418161891629318</v>
@@ -5048,10 +5048,10 @@
       </c>
       <c r="C182" s="2"/>
       <c r="D182" s="5">
-        <v>88811070258777</v>
+        <v>44405535129388</v>
       </c>
       <c r="E182" s="5">
-        <v>6143375</v>
+        <v>12286750</v>
       </c>
       <c r="F182" s="5">
         <v>585426648281045</v>
@@ -5073,10 +5073,10 @@
       </c>
       <c r="C183" s="2"/>
       <c r="D183" s="5">
-        <v>99468398689830</v>
+        <v>49734199344915</v>
       </c>
       <c r="E183" s="5">
-        <v>6285094</v>
+        <v>12570188</v>
       </c>
       <c r="F183" s="5">
         <v>848868640007515</v>
@@ -5098,10 +5098,10 @@
       </c>
       <c r="C184" s="2"/>
       <c r="D184" s="5">
-        <v>111404606532610</v>
+        <v>55702303266305</v>
       </c>
       <c r="E184" s="5">
-        <v>6430832</v>
+        <v>12861664</v>
       </c>
       <c r="F184" s="5">
         <v>1230859528010896</v>
@@ -5123,10 +5123,10 @@
       </c>
       <c r="C185" s="2"/>
       <c r="D185" s="5">
-        <v>124773159316523</v>
+        <v>62386579658261</v>
       </c>
       <c r="E185" s="5">
-        <v>6578239</v>
+        <v>13156478</v>
       </c>
       <c r="F185" s="5">
         <v>1784746315615799</v>
@@ -5148,10 +5148,10 @@
       </c>
       <c r="C186" s="2"/>
       <c r="D186" s="5">
-        <v>139745938434506</v>
+        <v>69872969217253</v>
       </c>
       <c r="E186" s="5">
-        <v>6727317</v>
+        <v>13454634</v>
       </c>
       <c r="F186" s="5">
         <v>2587882157642908</v>
@@ -5173,10 +5173,10 @@
       </c>
       <c r="C187" s="2"/>
       <c r="D187" s="5">
-        <v>156515451046647</v>
+        <v>78257725523323</v>
       </c>
       <c r="E187" s="5">
-        <v>6880551</v>
+        <v>13761102</v>
       </c>
       <c r="F187" s="5">
         <v>3752429128582216</v>
@@ -5198,10 +5198,10 @@
       </c>
       <c r="C188" s="2"/>
       <c r="D188" s="5">
-        <v>175297305172245</v>
+        <v>87648652586122</v>
       </c>
       <c r="E188" s="5">
-        <v>7035509</v>
+        <v>14071018</v>
       </c>
       <c r="F188" s="5">
         <v>5441022236444213</v>
@@ -5223,10 +5223,10 @@
       </c>
       <c r="C189" s="2"/>
       <c r="D189" s="5">
-        <v>196332981792914</v>
+        <v>98166490896457</v>
       </c>
       <c r="E189" s="5">
-        <v>7192194</v>
+        <v>14384388</v>
       </c>
       <c r="F189" s="5">
         <v>7889482242844109</v>
@@ -5248,10 +5248,10 @@
       </c>
       <c r="C190" s="2"/>
       <c r="D190" s="5">
-        <v>219892939608064</v>
+        <v>109946469804032</v>
       </c>
       <c r="E190" s="5">
-        <v>7353173</v>
+        <v>14706346</v>
       </c>
       <c r="F190" s="5">
         <v>1.1439749252123958E+16</v>
@@ -5273,10 +5273,10 @@
       </c>
       <c r="C191" s="2"/>
       <c r="D191" s="5">
-        <v>246280092361032</v>
+        <v>123140046180516</v>
       </c>
       <c r="E191" s="5">
-        <v>7515933</v>
+        <v>15031866</v>
       </c>
       <c r="F191" s="5">
         <v>1.6587636415579738E+16</v>
@@ -5298,10 +5298,10 @@
       </c>
       <c r="C192" s="2"/>
       <c r="D192" s="5">
-        <v>275833703444356</v>
+        <v>137916851722178</v>
       </c>
       <c r="E192" s="5">
-        <v>8229081</v>
+        <v>16458162</v>
       </c>
       <c r="F192" s="5">
         <v>2.405207280259062E+16</v>
@@ -5323,10 +5323,10 @@
       </c>
       <c r="C193" s="2"/>
       <c r="D193" s="5">
-        <v>308933747857679</v>
+        <v>154466873928840</v>
       </c>
       <c r="E193" s="5">
-        <v>8410129</v>
+        <v>16820258</v>
       </c>
       <c r="F193" s="5">
         <v>3.4875505563756396E+16</v>
@@ -5348,10 +5348,10 @@
       </c>
       <c r="C194" s="2"/>
       <c r="D194" s="5">
-        <v>346005797600601</v>
+        <v>173002898800301</v>
       </c>
       <c r="E194" s="5">
-        <v>8593146</v>
+        <v>17186292</v>
       </c>
       <c r="F194" s="5">
         <v>5.0569483067446776E+16</v>
@@ -5373,10 +5373,10 @@
       </c>
       <c r="C195" s="2"/>
       <c r="D195" s="5">
-        <v>387526493312673</v>
+        <v>193763246656337</v>
       </c>
       <c r="E195" s="5">
-        <v>8778134</v>
+        <v>17556268</v>
       </c>
       <c r="F195" s="5">
         <v>7.3325750447797824E+16</v>
@@ -5398,10 +5398,10 @@
       </c>
       <c r="C196" s="2"/>
       <c r="D196" s="5">
-        <v>434029672510194</v>
+        <v>217014836255097</v>
       </c>
       <c r="E196" s="5">
-        <v>8968029</v>
+        <v>17936058</v>
       </c>
       <c r="F196" s="5">
         <v>1.0632233814930685E+17</v>
@@ -5423,10 +5423,10 @@
       </c>
       <c r="C197" s="2"/>
       <c r="D197" s="5">
-        <v>486113233211417</v>
+        <v>243056616605709</v>
       </c>
       <c r="E197" s="5">
-        <v>9159955</v>
+        <v>18319910</v>
       </c>
       <c r="F197" s="5">
         <v>1.5416739031649491E+17</v>
@@ -5448,10 +5448,10 @@
       </c>
       <c r="C198" s="2"/>
       <c r="D198" s="5">
-        <v>544446821196787</v>
+        <v>272223410598394</v>
       </c>
       <c r="E198" s="5">
-        <v>9353914</v>
+        <v>18707828</v>
       </c>
       <c r="F198" s="5">
         <v>2.235427159589176E+17</v>
@@ -5473,10 +5473,10 @@
       </c>
       <c r="C199" s="2"/>
       <c r="D199" s="5">
-        <v>609780439740402</v>
+        <v>304890219870201</v>
       </c>
       <c r="E199" s="5">
-        <v>9552935</v>
+        <v>19105870</v>
       </c>
       <c r="F199" s="5">
         <v>3.2413693814043053E+17</v>
@@ -5498,10 +5498,10 @@
       </c>
       <c r="C200" s="2"/>
       <c r="D200" s="5">
-        <v>682954092509250</v>
+        <v>341477046254625</v>
       </c>
       <c r="E200" s="5">
-        <v>9754052</v>
+        <v>19508104</v>
       </c>
       <c r="F200" s="5">
         <v>4.6999856030362426E+17</v>
@@ -5523,10 +5523,10 @@
       </c>
       <c r="C201" s="2"/>
       <c r="D201" s="5">
-        <v>764908583610360</v>
+        <v>382454291805180</v>
       </c>
       <c r="E201" s="5">
-        <v>9957263</v>
+        <v>19914526</v>
       </c>
       <c r="F201" s="5">
         <v>6.814979124402551E+17</v>
@@ -5548,10 +5548,10 @@
       </c>
       <c r="C202" s="2"/>
       <c r="D202" s="5">
-        <v>856697613643603</v>
+        <v>428348806821802</v>
       </c>
       <c r="E202" s="5">
-        <v>11562671</v>
+        <v>23125342</v>
       </c>
       <c r="F202" s="5">
         <v>9.5409707741635712E+17</v>
@@ -5573,10 +5573,10 @@
       </c>
       <c r="C203" s="2"/>
       <c r="D203" s="5">
-        <v>959501327280836</v>
+        <v>479750663640418</v>
       </c>
       <c r="E203" s="5">
-        <v>11741664</v>
+        <v>23483328</v>
       </c>
       <c r="F203" s="5">
         <v>1.3357359083829E+18</v>
@@ -5598,10 +5598,10 @@
       </c>
       <c r="C204" s="2"/>
       <c r="D204" s="5">
-        <v>1074641486554536</v>
+        <v>537320743277268</v>
       </c>
       <c r="E204" s="5">
-        <v>11925652</v>
+        <v>23851304</v>
       </c>
       <c r="F204" s="5">
         <v>1.8700302717360599E+18</v>
@@ -5623,10 +5623,10 @@
       </c>
       <c r="C205" s="2"/>
       <c r="D205" s="5">
-        <v>1203598464941080</v>
+        <v>601799232470540</v>
       </c>
       <c r="E205" s="5">
-        <v>12111071</v>
+        <v>24222142</v>
       </c>
       <c r="F205" s="5">
         <v>2.6180423804304835E+18</v>
@@ -5648,10 +5648,10 @@
       </c>
       <c r="C206" s="2"/>
       <c r="D206" s="5">
-        <v>1348030280734009</v>
+        <v>674015140367005</v>
       </c>
       <c r="E206" s="5">
-        <v>12297920</v>
+        <v>24595840</v>
       </c>
       <c r="F206" s="5">
         <v>3.6652593326026767E+18</v>
@@ -5673,10 +5673,10 @@
       </c>
       <c r="C207" s="2"/>
       <c r="D207" s="5">
-        <v>1509793914422090</v>
+        <v>754896957211045</v>
       </c>
       <c r="E207" s="5">
-        <v>12486200</v>
+        <v>24972400</v>
       </c>
       <c r="F207" s="5">
         <v>5.1313630656437473E+18</v>
@@ -5698,10 +5698,10 @@
       </c>
       <c r="C208" s="2"/>
       <c r="D208" s="5">
-        <v>1690969184152741</v>
+        <v>845484592076371</v>
       </c>
       <c r="E208" s="5">
-        <v>12679643</v>
+        <v>25359286</v>
       </c>
       <c r="F208" s="5">
         <v>7.1839082919012454E+18</v>
@@ -5723,10 +5723,10 @@
       </c>
       <c r="C209" s="2"/>
       <c r="D209" s="5">
-        <v>1893885486251070</v>
+        <v>946942743125535</v>
       </c>
       <c r="E209" s="5">
-        <v>12874574</v>
+        <v>25749148</v>
       </c>
       <c r="F209" s="5">
         <v>1.0057471608661744E+19</v>
@@ -5748,10 +5748,10 @@
       </c>
       <c r="C210" s="2"/>
       <c r="D210" s="5">
-        <v>2121151744601198</v>
+        <v>1060575872300599</v>
       </c>
       <c r="E210" s="5">
-        <v>13070992</v>
+        <v>26141984</v>
       </c>
       <c r="F210" s="5">
         <v>1.4080460252126439E+19</v>
@@ -5773,10 +5773,10 @@
       </c>
       <c r="C211" s="2"/>
       <c r="D211" s="5">
-        <v>2375689953953342</v>
+        <v>1187844976976671</v>
       </c>
       <c r="E211" s="5">
-        <v>13268897</v>
+        <v>26537794</v>
       </c>
       <c r="F211" s="5">
         <v>1.9712644352977015E+19</v>
@@ -5798,10 +5798,10 @@
       </c>
       <c r="C212" s="2"/>
       <c r="D212" s="5">
-        <v>2660772748427743</v>
+        <v>1330386374213871</v>
       </c>
       <c r="E212" s="5">
-        <v>14045420</v>
+        <v>28090840</v>
       </c>
       <c r="F212" s="5">
         <v>2.7597702094167818E+19</v>
@@ -5823,10 +5823,10 @@
       </c>
       <c r="C213" s="2"/>
       <c r="D213" s="5">
-        <v>2980065478239072</v>
+        <v>1490032739119536</v>
       </c>
       <c r="E213" s="5">
-        <v>14258919</v>
+        <v>28517838</v>
       </c>
       <c r="F213" s="5">
         <v>3.8636782931834946E+19</v>
@@ -5848,10 +5848,10 @@
       </c>
       <c r="C214" s="2"/>
       <c r="D214" s="5">
-        <v>3337673335627761</v>
+        <v>1668836667813880</v>
       </c>
       <c r="E214" s="5">
-        <v>14474029</v>
+        <v>28948058</v>
       </c>
       <c r="F214" s="5">
         <v>5.4091496104568922E+19</v>
@@ -5873,10 +5873,10 @@
       </c>
       <c r="C215" s="2"/>
       <c r="D215" s="5">
-        <v>3738194135903092</v>
+        <v>1869097067951546</v>
       </c>
       <c r="E215" s="5">
-        <v>14690749</v>
+        <v>29381498</v>
       </c>
       <c r="F215" s="5">
         <v>7.5728094546396479E+19</v>
@@ -5898,10 +5898,10 @@
       </c>
       <c r="C216" s="2"/>
       <c r="D216" s="5">
-        <v>4186777432211463</v>
+        <v>2093388716105731</v>
       </c>
       <c r="E216" s="5">
-        <v>14913215</v>
+        <v>29826430</v>
       </c>
       <c r="F216" s="5">
         <v>1.0601933236495506E+20</v>
@@ -5923,10 +5923,10 @@
       </c>
       <c r="C217" s="2"/>
       <c r="D217" s="5">
-        <v>4689190724076839</v>
+        <v>2344595362038419</v>
       </c>
       <c r="E217" s="5">
-        <v>15137352</v>
+        <v>30274704</v>
       </c>
       <c r="F217" s="5">
         <v>1.4842706531093709E+20</v>
@@ -5948,10 +5948,10 @@
       </c>
       <c r="C218" s="2"/>
       <c r="D218" s="5">
-        <v>5251893610966060</v>
+        <v>2625946805483030</v>
       </c>
       <c r="E218" s="5">
-        <v>15363161</v>
+        <v>30726322</v>
       </c>
       <c r="F218" s="5">
         <v>2.0779789143531192E+20</v>
@@ -5973,10 +5973,10 @@
       </c>
       <c r="C219" s="2"/>
       <c r="D219" s="5">
-        <v>5882120844281988</v>
+        <v>2941060422140994</v>
       </c>
       <c r="E219" s="5">
-        <v>15590642</v>
+        <v>31181284</v>
       </c>
       <c r="F219" s="5">
         <v>2.9091704800943666E+20</v>
@@ -5998,10 +5998,10 @@
       </c>
       <c r="C220" s="2"/>
       <c r="D220" s="5">
-        <v>6587975345595827</v>
+        <v>3293987672797913</v>
       </c>
       <c r="E220" s="5">
-        <v>15824054</v>
+        <v>31648108</v>
       </c>
       <c r="F220" s="5">
         <v>4.072838672132113E+20</v>
@@ -6023,10 +6023,10 @@
       </c>
       <c r="C221" s="2"/>
       <c r="D221" s="5">
-        <v>7378532387067327</v>
+        <v>3689266193533663</v>
       </c>
       <c r="E221" s="5">
-        <v>16059200</v>
+        <v>32118400</v>
       </c>
       <c r="F221" s="5">
         <v>5.701974140984958E+20</v>
@@ -6048,10 +6048,10 @@
       </c>
       <c r="C222" s="2"/>
       <c r="D222" s="5">
-        <v>8263956273515407</v>
+        <v>4131978136757703</v>
       </c>
       <c r="E222" s="5">
-        <v>16961227</v>
+        <v>33922454</v>
       </c>
       <c r="F222" s="5">
         <v>7.9827637973789403E+20</v>
@@ -6073,10 +6073,10 @@
       </c>
       <c r="C223" s="2"/>
       <c r="D223" s="5">
-        <v>9255631026337256</v>
+        <v>4627815513168628</v>
       </c>
       <c r="E223" s="5">
-        <v>17209581</v>
+        <v>34419162</v>
       </c>
       <c r="F223" s="5">
         <v>1.1175869316330515E+21</v>
@@ -6098,10 +6098,10 @@
       </c>
       <c r="C224" s="2"/>
       <c r="D224" s="5">
-        <v>1.0366306749497728E+16</v>
+        <v>5183153374748864</v>
       </c>
       <c r="E224" s="5">
-        <v>17464305</v>
+        <v>34928610</v>
       </c>
       <c r="F224" s="5">
         <v>1.564621704286272E+21</v>
@@ -6123,10 +6123,10 @@
       </c>
       <c r="C225" s="2"/>
       <c r="D225" s="5">
-        <v>1.1610263559437456E+16</v>
+        <v>5805131779718728</v>
       </c>
       <c r="E225" s="5">
-        <v>17720900</v>
+        <v>35441800</v>
       </c>
       <c r="F225" s="5">
         <v>2.1904703860007806E+21</v>
@@ -6148,10 +6148,10 @@
       </c>
       <c r="C226" s="2"/>
       <c r="D226" s="5">
-        <v>1.3003495186569952E+16</v>
+        <v>6501747593284976</v>
       </c>
       <c r="E226" s="5">
-        <v>17979367</v>
+        <v>35958734</v>
       </c>
       <c r="F226" s="5">
         <v>3.0666585404010927E+21</v>
@@ -6173,10 +6173,10 @@
       </c>
       <c r="C227" s="2"/>
       <c r="D227" s="5">
-        <v>1.4563914608958348E+16</v>
+        <v>7281957304479174</v>
       </c>
       <c r="E227" s="5">
-        <v>18239705</v>
+        <v>36479410</v>
       </c>
       <c r="F227" s="5">
         <v>4.2933219565615296E+21</v>
@@ -6198,10 +6198,10 @@
       </c>
       <c r="C228" s="2"/>
       <c r="D228" s="5">
-        <v>1.6311584362033352E+16</v>
+        <v>8155792181016676</v>
       </c>
       <c r="E228" s="5">
-        <v>18506613</v>
+        <v>37013226</v>
       </c>
       <c r="F228" s="5">
         <v>6.0106507391861407E+21</v>
@@ -6223,10 +6223,10 @@
       </c>
       <c r="C229" s="2"/>
       <c r="D229" s="5">
-        <v>1.8268974485477356E+16</v>
+        <v>9134487242738678</v>
       </c>
       <c r="E229" s="5">
-        <v>18775460</v>
+        <v>37550920</v>
       </c>
       <c r="F229" s="5">
         <v>8.4149110348605964E+21</v>
@@ -6248,10 +6248,10 @@
       </c>
       <c r="C230" s="2"/>
       <c r="D230" s="5">
-        <v>2.046125142373464E+16</v>
+        <v>1.023062571186732E+16</v>
       </c>
       <c r="E230" s="5">
-        <v>19046246</v>
+        <v>38092492</v>
       </c>
       <c r="F230" s="5">
         <v>1.1780875448804834E+22</v>
@@ -6273,10 +6273,10 @@
       </c>
       <c r="C231" s="2"/>
       <c r="D231" s="5">
-        <v>2.29166015945828E+16</v>
+        <v>1.14583007972914E+16</v>
       </c>
       <c r="E231" s="5">
-        <v>19318970</v>
+        <v>38637940</v>
       </c>
       <c r="F231" s="5">
         <v>1.6493225628326766E+22</v>
@@ -6298,10 +6298,10 @@
       </c>
       <c r="C232" s="2"/>
       <c r="D232" s="5">
-        <v>2.566659378593274E+16</v>
+        <v>1.283329689296637E+16</v>
       </c>
       <c r="E232" s="5">
-        <v>20367037</v>
+        <v>40734074</v>
       </c>
       <c r="F232" s="5">
         <v>2.3090515879657472E+22</v>
@@ -6323,10 +6323,10 @@
       </c>
       <c r="C233" s="2"/>
       <c r="D233" s="5">
-        <v>2.8746585040244672E+16</v>
+        <v>1.4373292520122336E+16</v>
       </c>
       <c r="E233" s="5">
-        <v>20659583</v>
+        <v>41319166</v>
       </c>
       <c r="F233" s="5">
         <v>3.2326722231520461E+22</v>
@@ -6348,10 +6348,10 @@
       </c>
       <c r="C234" s="2"/>
       <c r="D234" s="5">
-        <v>3.2196175245074036E+16</v>
+        <v>1.6098087622537018E+16</v>
       </c>
       <c r="E234" s="5">
-        <v>20954214</v>
+        <v>41908428</v>
       </c>
       <c r="F234" s="5">
         <v>4.5257411124128645E+22</v>
@@ -6373,10 +6373,10 @@
       </c>
       <c r="C235" s="2"/>
       <c r="D235" s="5">
-        <v>3.605971627448292E+16</v>
+        <v>1.802985813724146E+16</v>
       </c>
       <c r="E235" s="5">
-        <v>21250932</v>
+        <v>42501864</v>
       </c>
       <c r="F235" s="5">
         <v>6.3360375573780103E+22</v>
@@ -6398,10 +6398,10 @@
       </c>
       <c r="C236" s="2"/>
       <c r="D236" s="5">
-        <v>4.0386882227420872E+16</v>
+        <v>2.0193441113710436E+16</v>
       </c>
       <c r="E236" s="5">
-        <v>21554906</v>
+        <v>43109812</v>
       </c>
       <c r="F236" s="5">
         <v>8.8704525803292144E+22</v>
@@ -6423,10 +6423,10 @@
       </c>
       <c r="C237" s="2"/>
       <c r="D237" s="5">
-        <v>4.5233308094711384E+16</v>
+        <v>2.2616654047355692E+16</v>
       </c>
       <c r="E237" s="5">
-        <v>21861039</v>
+        <v>43722078</v>
       </c>
       <c r="F237" s="5">
         <v>1.24186336124609E+23</v>
@@ -6448,10 +6448,10 @@
       </c>
       <c r="C238" s="2"/>
       <c r="D238" s="5">
-        <v>5.0661305066076752E+16</v>
+        <v>2.5330652533038376E+16</v>
       </c>
       <c r="E238" s="5">
-        <v>22169330</v>
+        <v>44338660</v>
       </c>
       <c r="F238" s="5">
         <v>1.738608705744526E+23</v>
@@ -6473,10 +6473,10 @@
       </c>
       <c r="C239" s="2"/>
       <c r="D239" s="5">
-        <v>5.6740661674005968E+16</v>
+        <v>2.8370330837002984E+16</v>
       </c>
       <c r="E239" s="5">
-        <v>22479779</v>
+        <v>44959558</v>
       </c>
       <c r="F239" s="5">
         <v>2.4340521880423363E+23</v>
@@ -6498,10 +6498,10 @@
       </c>
       <c r="C240" s="2"/>
       <c r="D240" s="5">
-        <v>6.3549541074886688E+16</v>
+        <v>3.1774770537443344E+16</v>
       </c>
       <c r="E240" s="5">
-        <v>22797705</v>
+        <v>45595410</v>
       </c>
       <c r="F240" s="5">
         <v>3.4076730632592704E+23</v>
@@ -6523,10 +6523,10 @@
       </c>
       <c r="C241" s="2"/>
       <c r="D241" s="5">
-        <v>7.1175486003873096E+16</v>
+        <v>3.5587743001936548E+16</v>
       </c>
       <c r="E241" s="5">
-        <v>23117862</v>
+        <v>46235724</v>
       </c>
       <c r="F241" s="5">
         <v>4.7707422885629783E+23</v>
@@ -6548,10 +6548,10 @@
       </c>
       <c r="C242" s="2"/>
       <c r="D242" s="5">
-        <v>7.9716544324337872E+16</v>
+        <v>3.9858272162168936E+16</v>
       </c>
       <c r="E242" s="5">
-        <v>24324790</v>
+        <v>48649580</v>
       </c>
       <c r="F242" s="5">
         <v>6.6790392039881687E+23</v>
@@ -6573,10 +6573,10 @@
       </c>
       <c r="C243" s="2"/>
       <c r="D243" s="5">
-        <v>8.9282529643258432E+16</v>
+        <v>4.4641264821629216E+16</v>
       </c>
       <c r="E243" s="5">
-        <v>24661662</v>
+        <v>49323324</v>
       </c>
       <c r="F243" s="5">
         <v>9.3506548855834351E+23</v>
@@ -6598,10 +6598,10 @@
       </c>
       <c r="C244" s="2"/>
       <c r="D244" s="5">
-        <v>9.9996433200449456E+16</v>
+        <v>4.9998216600224728E+16</v>
       </c>
       <c r="E244" s="5">
-        <v>25006524</v>
+        <v>50013048</v>
       </c>
       <c r="F244" s="5">
         <v>1.3090916839816807E+24</v>
@@ -6623,10 +6623,10 @@
       </c>
       <c r="C245" s="2"/>
       <c r="D245" s="5">
-        <v>1.1199600518450341E+17</v>
+        <v>5.5998002592251704E+16</v>
       </c>
       <c r="E245" s="5">
-        <v>25353780</v>
+        <v>50707560</v>
       </c>
       <c r="F245" s="5">
         <v>1.832728357574353E+24</v>
@@ -6648,10 +6648,10 @@
       </c>
       <c r="C246" s="2"/>
       <c r="D246" s="5">
-        <v>1.2543552580664382E+17</v>
+        <v>6.2717762903321912E+16</v>
       </c>
       <c r="E246" s="5">
-        <v>25703431</v>
+        <v>51406862</v>
       </c>
       <c r="F246" s="5">
         <v>2.5658197006040939E+24</v>
@@ -6673,10 +6673,10 @@
       </c>
       <c r="C247" s="2"/>
       <c r="D247" s="5">
-        <v>1.404877889034411E+17</v>
+        <v>7.0243894451720552E+16</v>
       </c>
       <c r="E247" s="5">
-        <v>26055476</v>
+        <v>52110952</v>
       </c>
       <c r="F247" s="5">
         <v>3.5921475808457311E+24</v>
@@ -6698,10 +6698,10 @@
       </c>
       <c r="C248" s="2"/>
       <c r="D248" s="5">
-        <v>1.5734632357185405E+17</v>
+        <v>7.8673161785927024E+16</v>
       </c>
       <c r="E248" s="5">
-        <v>26415746</v>
+        <v>52831492</v>
       </c>
       <c r="F248" s="5">
         <v>5.0290066131840228E+24</v>
@@ -6723,10 +6723,10 @@
       </c>
       <c r="C249" s="2"/>
       <c r="D249" s="5">
-        <v>1.7622788240047654E+17</v>
+        <v>8.8113941200238272E+16</v>
       </c>
       <c r="E249" s="5">
-        <v>26778489</v>
+        <v>53556978</v>
       </c>
       <c r="F249" s="5">
         <v>7.0406092584576311E+24</v>
@@ -6748,10 +6748,10 @@
       </c>
       <c r="C250" s="2"/>
       <c r="D250" s="5">
-        <v>1.9737522828853376E+17</v>
+        <v>9.868761414426688E+16</v>
       </c>
       <c r="E250" s="5">
-        <v>27143706</v>
+        <v>54287412</v>
       </c>
       <c r="F250" s="5">
         <v>9.8568529618406831E+24</v>
@@ -6773,10 +6773,10 @@
       </c>
       <c r="C251" s="2"/>
       <c r="D251" s="5">
-        <v>2.2106025568315782E+17</v>
+        <v>1.1053012784157891E+17</v>
       </c>
       <c r="E251" s="5">
-        <v>27511397</v>
+        <v>55022794</v>
       </c>
       <c r="F251" s="5">
         <v>1.3799594146576956E+25</v>
@@ -6798,10 +6798,10 @@
       </c>
       <c r="C252" s="2"/>
       <c r="D252" s="5">
-        <v>2.475874863651368E+17</v>
+        <v>1.237937431825684E+17</v>
       </c>
       <c r="E252" s="5">
-        <v>36404957</v>
+        <v>72809914</v>
       </c>
       <c r="F252" s="5">
         <v>2.0009411512536584E+25</v>
@@ -6823,10 +6823,10 @@
       </c>
       <c r="C253" s="2"/>
       <c r="D253" s="5">
-        <v>2.7729798472895325E+17</v>
+        <v>1.3864899236447662E+17</v>
       </c>
       <c r="E253" s="5">
-        <v>36899331</v>
+        <v>73798662</v>
       </c>
       <c r="F253" s="5">
         <v>2.9013646693178048E+25</v>
@@ -6848,10 +6848,10 @@
       </c>
       <c r="C254" s="2"/>
       <c r="D254" s="5">
-        <v>3.1057374289642765E+17</v>
+        <v>1.5528687144821382E+17</v>
       </c>
       <c r="E254" s="5">
-        <v>37397039</v>
+        <v>74794078</v>
       </c>
       <c r="F254" s="5">
         <v>4.206978770510817E+25</v>
@@ -6873,10 +6873,10 @@
       </c>
       <c r="C255" s="2"/>
       <c r="D255" s="5">
-        <v>3.4784259204399898E+17</v>
+        <v>1.7392129602199949E+17</v>
       </c>
       <c r="E255" s="5">
-        <v>37898082</v>
+        <v>75796164</v>
       </c>
       <c r="F255" s="5">
         <v>6.1001192172406847E+25</v>
@@ -6898,10 +6898,10 @@
       </c>
       <c r="C256" s="2"/>
       <c r="D256" s="5">
-        <v>3.8958370308927891E+17</v>
+        <v>1.9479185154463946E+17</v>
       </c>
       <c r="E256" s="5">
-        <v>38410491</v>
+        <v>76820982</v>
       </c>
       <c r="F256" s="5">
         <v>8.8451728649989929E+25</v>
@@ -6923,10 +6923,10 @@
       </c>
       <c r="C257" s="2"/>
       <c r="D257" s="5">
-        <v>4.3633374745999245E+17</v>
+        <v>2.1816687372999622E+17</v>
       </c>
       <c r="E257" s="5">
-        <v>38926341</v>
+        <v>77852682</v>
       </c>
       <c r="F257" s="5">
         <v>1.282550065424854E+26</v>
@@ -6948,10 +6948,10 @@
       </c>
       <c r="C258" s="2"/>
       <c r="D258" s="5">
-        <v>4.8869379715519162E+17</v>
+        <v>2.4434689857759581E+17</v>
       </c>
       <c r="E258" s="5">
-        <v>39445632</v>
+        <v>78891264</v>
       </c>
       <c r="F258" s="5">
         <v>1.8596975948660382E+26</v>
@@ -6973,10 +6973,10 @@
       </c>
       <c r="C259" s="2"/>
       <c r="D259" s="5">
-        <v>5.4733705281381466E+17</v>
+        <v>2.7366852640690733E+17</v>
       </c>
       <c r="E259" s="5">
-        <v>39968364</v>
+        <v>79936728</v>
       </c>
       <c r="F259" s="5">
         <v>2.6965615125557555E+26</v>
@@ -6998,10 +6998,10 @@
       </c>
       <c r="C260" s="2"/>
       <c r="D260" s="5">
-        <v>6.1301749915147251E+17</v>
+        <v>3.0650874957573626E+17</v>
       </c>
       <c r="E260" s="5">
-        <v>40502786</v>
+        <v>81005572</v>
       </c>
       <c r="F260" s="5">
         <v>3.9100141932058453E+26</v>
@@ -7023,10 +7023,10 @@
       </c>
       <c r="C261" s="2"/>
       <c r="D261" s="5">
-        <v>6.8657959904964928E+17</v>
+        <v>3.4328979952482464E+17</v>
       </c>
       <c r="E261" s="5">
-        <v>41040756</v>
+        <v>82081512</v>
       </c>
       <c r="F261" s="5">
         <v>5.6695205801484756E+26</v>
@@ -7048,10 +7048,10 @@
       </c>
       <c r="C262" s="2"/>
       <c r="D262" s="5">
-        <v>7.689691509356073E+17</v>
+        <v>3.8448457546780365E+17</v>
       </c>
       <c r="E262" s="5">
-        <v>43041303</v>
+        <v>86082606</v>
       </c>
       <c r="F262" s="5">
         <v>8.2208048412152888E+26</v>
@@ -7073,10 +7073,10 @@
       </c>
       <c r="C263" s="2"/>
       <c r="D263" s="5">
-        <v>8.6124544904788019E+17</v>
+        <v>4.306227245239401E+17</v>
       </c>
       <c r="E263" s="5">
-        <v>43605497</v>
+        <v>87210994</v>
       </c>
       <c r="F263" s="5">
         <v>1.1920167019762168E+27</v>
@@ -7098,10 +7098,10 @@
       </c>
       <c r="C264" s="2"/>
       <c r="D264" s="5">
-        <v>9.6459490293362586E+17</v>
+        <v>4.8229745146681293E+17</v>
       </c>
       <c r="E264" s="5">
-        <v>44182130</v>
+        <v>88364260</v>
       </c>
       <c r="F264" s="5">
         <v>1.7284242178655144E+27</v>
@@ -7123,10 +7123,10 @@
       </c>
       <c r="C265" s="2"/>
       <c r="D265" s="5">
-        <v>1.0803462912856611E+18</v>
+        <v>5.4017314564283053E+17</v>
       </c>
       <c r="E265" s="5">
-        <v>44762550</v>
+        <v>89525100</v>
       </c>
       <c r="F265" s="5">
         <v>2.5062151159049959E+27</v>
@@ -7148,10 +7148,10 @@
       </c>
       <c r="C266" s="2"/>
       <c r="D266" s="5">
-        <v>1.2099878462399406E+18</v>
+        <v>6.049939231199703E+17</v>
       </c>
       <c r="E266" s="5">
-        <v>45346758</v>
+        <v>90693516</v>
       </c>
       <c r="F266" s="5">
         <v>3.634011918062244E+27</v>
@@ -7173,10 +7173,10 @@
       </c>
       <c r="C267" s="2"/>
       <c r="D267" s="5">
-        <v>1.3551863877887337E+18</v>
+        <v>6.7759319389436685E+17</v>
       </c>
       <c r="E267" s="5">
-        <v>45934754</v>
+        <v>91869508</v>
       </c>
       <c r="F267" s="5">
         <v>5.2693172811902539E+27</v>
@@ -7198,10 +7198,10 @@
       </c>
       <c r="C268" s="2"/>
       <c r="D268" s="5">
-        <v>1.5178087543233818E+18</v>
+        <v>7.5890437716169088E+17</v>
       </c>
       <c r="E268" s="5">
-        <v>46535533</v>
+        <v>93071066</v>
       </c>
       <c r="F268" s="5">
         <v>7.640510057725868E+27</v>
@@ -7223,10 +7223,10 @@
       </c>
       <c r="C269" s="2"/>
       <c r="D269" s="5">
-        <v>1.6999458048421878E+18</v>
+        <v>8.4997290242109389E+17</v>
       </c>
       <c r="E269" s="5">
-        <v>47140215</v>
+        <v>94280430</v>
       </c>
       <c r="F269" s="5">
         <v>1.1078739583702508E+28</v>
@@ -7248,10 +7248,10 @@
       </c>
       <c r="C270" s="2"/>
       <c r="D270" s="5">
-        <v>1.9039393014232504E+18</v>
+        <v>9.5196965071162522E+17</v>
       </c>
       <c r="E270" s="5">
-        <v>47748800</v>
+        <v>95497600</v>
       </c>
       <c r="F270" s="5">
         <v>1.6064172396368638E+28</v>
@@ -7273,10 +7273,10 @@
       </c>
       <c r="C271" s="2"/>
       <c r="D271" s="5">
-        <v>2.1324120175940406E+18</v>
+        <v>1.0662060087970203E+18</v>
       </c>
       <c r="E271" s="5">
-        <v>48361289</v>
+        <v>96722578</v>
       </c>
       <c r="F271" s="5">
         <v>2.3293049974734522E+28</v>
@@ -7298,10 +7298,10 @@
       </c>
       <c r="C272" s="2"/>
       <c r="D272" s="5">
-        <v>2.3883014597053256E+18</v>
+        <v>1.1941507298526628E+18</v>
       </c>
       <c r="E272" s="5">
-        <v>50647483</v>
+        <v>101294966</v>
       </c>
       <c r="F272" s="5">
         <v>3.3774922463365056E+28</v>
@@ -7323,10 +7323,10 @@
       </c>
       <c r="C273" s="2"/>
       <c r="D273" s="5">
-        <v>2.6748976348699648E+18</v>
+        <v>1.3374488174349824E+18</v>
       </c>
       <c r="E273" s="5">
-        <v>51298469</v>
+        <v>102596938</v>
       </c>
       <c r="F273" s="5">
         <v>4.8973637571879329E+28</v>
@@ -7348,10 +7348,10 @@
       </c>
       <c r="C274" s="2"/>
       <c r="D274" s="5">
-        <v>2.9958853510543611E+18</v>
+        <v>1.4979426755271805E+18</v>
       </c>
       <c r="E274" s="5">
-        <v>51953611</v>
+        <v>103907222</v>
       </c>
       <c r="F274" s="5">
         <v>7.1011774479225024E+28</v>
@@ -7373,10 +7373,10 @@
       </c>
       <c r="C275" s="2"/>
       <c r="D275" s="5">
-        <v>3.355391593180885E+18</v>
+        <v>1.6776957965904425E+18</v>
       </c>
       <c r="E275" s="5">
-        <v>52612911</v>
+        <v>105225822</v>
       </c>
       <c r="F275" s="5">
         <v>1.0296707299487628E+29</v>
@@ -7398,10 +7398,10 @@
       </c>
       <c r="C276" s="2"/>
       <c r="D276" s="5">
-        <v>3.7580385843625917E+18</v>
+        <v>1.8790192921812959E+18</v>
       </c>
       <c r="E276" s="5">
-        <v>53286155</v>
+        <v>106572310</v>
       </c>
       <c r="F276" s="5">
         <v>1.493022558425706E+29</v>
@@ -7423,10 +7423,10 @@
       </c>
       <c r="C277" s="2"/>
       <c r="D277" s="5">
-        <v>4.209003214486103E+18</v>
+        <v>2.1045016072430515E+18</v>
       </c>
       <c r="E277" s="5">
-        <v>53963679</v>
+        <v>107927358</v>
       </c>
       <c r="F277" s="5">
         <v>2.1648827097172737E+29</v>
@@ -7448,10 +7448,10 @@
       </c>
       <c r="C278" s="2"/>
       <c r="D278" s="5">
-        <v>4.7140836002244362E+18</v>
+        <v>2.3570418001122181E+18</v>
       </c>
       <c r="E278" s="5">
-        <v>54645483</v>
+        <v>109290966</v>
       </c>
       <c r="F278" s="5">
         <v>3.1390799290900469E+29</v>
@@ -7473,10 +7473,10 @@
       </c>
       <c r="C279" s="2"/>
       <c r="D279" s="5">
-        <v>5.2797736322513695E+18</v>
+        <v>2.6398868161256847E+18</v>
       </c>
       <c r="E279" s="5">
-        <v>55331568</v>
+        <v>110663136</v>
       </c>
       <c r="F279" s="5">
         <v>4.5516658971805678E+29</v>
@@ -7498,10 +7498,10 @@
       </c>
       <c r="C280" s="2"/>
       <c r="D280" s="5">
-        <v>5.9133464681215345E+18</v>
+        <v>2.9566732340607672E+18</v>
       </c>
       <c r="E280" s="5">
-        <v>56031969</v>
+        <v>112063938</v>
       </c>
       <c r="F280" s="5">
         <v>6.5999155509118237E+29</v>
@@ -7523,10 +7523,10 @@
       </c>
       <c r="C281" s="2"/>
       <c r="D281" s="5">
-        <v>6.6229480442961193E+18</v>
+        <v>3.3114740221480596E+18</v>
       </c>
       <c r="E281" s="5">
-        <v>56736775</v>
+        <v>113473550</v>
       </c>
       <c r="F281" s="5">
         <v>9.5698775488221441E+29</v>
@@ -7548,10 +7548,10 @@
       </c>
       <c r="C282" s="2"/>
       <c r="D282" s="5">
-        <v>7.4177018096116541E+18</v>
+        <v>3.7088509048058271E+18</v>
       </c>
       <c r="E282" s="5">
-        <v>59329461</v>
+        <v>118658922</v>
       </c>
       <c r="F282" s="5">
         <v>1.387632244579211E+30</v>
@@ -7573,10 +7573,10 @@
       </c>
       <c r="C283" s="2"/>
       <c r="D283" s="5">
-        <v>8.3078260267650529E+18</v>
+        <v>4.1539130133825265E+18</v>
       </c>
       <c r="E283" s="5">
-        <v>60066475</v>
+        <v>120132950</v>
       </c>
       <c r="F283" s="5">
         <v>2.0120667546398558E+30</v>
@@ -7598,10 +7598,10 @@
       </c>
       <c r="C284" s="2"/>
       <c r="D284" s="5">
-        <v>9.3047651499768607E+18</v>
+        <v>4.6523825749884303E+18</v>
       </c>
       <c r="E284" s="5">
-        <v>60818664</v>
+        <v>121637328</v>
       </c>
       <c r="F284" s="5">
         <v>2.9174967942277906E+30</v>
@@ -7623,10 +7623,10 @@
       </c>
       <c r="C285" s="2"/>
       <c r="D285" s="5">
-        <v>1.0421336967974085E+19</v>
+        <v>5.2106684839870423E+18</v>
       </c>
       <c r="E285" s="5">
-        <v>61575535</v>
+        <v>123151070</v>
       </c>
       <c r="F285" s="5">
         <v>4.2303703516302961E+30</v>
@@ -7648,10 +7648,10 @@
       </c>
       <c r="C286" s="2"/>
       <c r="D286" s="5">
-        <v>1.1671897404130976E+19</v>
+        <v>5.8359487020654879E+18</v>
       </c>
       <c r="E286" s="5">
-        <v>62337085</v>
+        <v>124674170</v>
       </c>
       <c r="F286" s="5">
         <v>6.1340370098639291E+30</v>
@@ -7673,10 +7673,10 @@
       </c>
       <c r="C287" s="2"/>
       <c r="D287" s="5">
-        <v>1.3072525092626694E+19</v>
+        <v>6.5362625463133471E+18</v>
       </c>
       <c r="E287" s="5">
-        <v>63103316</v>
+        <v>126206632</v>
       </c>
       <c r="F287" s="5">
         <v>8.8943536643026963E+30</v>
@@ -7698,10 +7698,10 @@
       </c>
       <c r="C288" s="2"/>
       <c r="D288" s="5">
-        <v>1.4641228103741899E+19</v>
+        <v>7.3206140518709494E+18</v>
       </c>
       <c r="E288" s="5">
-        <v>63885118</v>
+        <v>127770236</v>
       </c>
       <c r="F288" s="5">
         <v>1.2896812813238908E+31</v>
@@ -7723,10 +7723,10 @@
       </c>
       <c r="C289" s="2"/>
       <c r="D289" s="5">
-        <v>1.6398175476190929E+19</v>
+        <v>8.1990877380954644E+18</v>
       </c>
       <c r="E289" s="5">
-        <v>64671734</v>
+        <v>129343468</v>
       </c>
       <c r="F289" s="5">
         <v>1.8700378579196416E+31</v>
@@ -7748,10 +7748,10 @@
       </c>
       <c r="C290" s="2"/>
       <c r="D290" s="5">
-        <v>1.8365956533333842E+19</v>
+        <v>9.182978266666921E+18</v>
       </c>
       <c r="E290" s="5">
-        <v>65463163</v>
+        <v>130926326</v>
       </c>
       <c r="F290" s="5">
         <v>2.7115548939834801E+31</v>
@@ -7773,10 +7773,10 @@
       </c>
       <c r="C291" s="2"/>
       <c r="D291" s="5">
-        <v>2.0569871317333905E+19</v>
+        <v>1.0284935658666953E+19</v>
       </c>
       <c r="E291" s="5">
-        <v>66259405</v>
+        <v>132518810</v>
       </c>
       <c r="F291" s="5">
         <v>3.931754596276046E+31</v>
@@ -7798,10 +7798,10 @@
       </c>
       <c r="C292" s="2"/>
       <c r="D292" s="5">
-        <v>2.3038255875413975E+19</v>
+        <v>1.1519127937706988E+19</v>
       </c>
       <c r="E292" s="5">
-        <v>69200878</v>
+        <v>138401756</v>
       </c>
       <c r="F292" s="5">
         <v>5.7010441646002668E+31</v>
@@ -7823,10 +7823,10 @@
       </c>
       <c r="C293" s="2"/>
       <c r="D293" s="5">
-        <v>2.5802846580463653E+19</v>
+        <v>1.2901423290231826E+19</v>
       </c>
       <c r="E293" s="5">
-        <v>70043982</v>
+        <v>140087964</v>
       </c>
       <c r="F293" s="5">
         <v>8.2665140386703858E+31</v>
@@ -7848,10 +7848,10 @@
       </c>
       <c r="C294" s="2"/>
       <c r="D294" s="5">
-        <v>2.8899188170119295E+19</v>
+        <v>1.4449594085059647E+19</v>
       </c>
       <c r="E294" s="5">
-        <v>70892191</v>
+        <v>141784382</v>
       </c>
       <c r="F294" s="5">
         <v>1.1986445356072058E+32</v>
@@ -7873,10 +7873,10 @@
       </c>
       <c r="C295" s="2"/>
       <c r="D295" s="5">
-        <v>3.2367090750533612E+19</v>
+        <v>1.6183545375266806E+19</v>
       </c>
       <c r="E295" s="5">
-        <v>71745505</v>
+        <v>143491010</v>
       </c>
       <c r="F295" s="5">
         <v>1.7380345766304485E+32</v>
@@ -7898,10 +7898,10 @@
       </c>
       <c r="C296" s="2"/>
       <c r="D296" s="5">
-        <v>3.6251141640597647E+19</v>
+        <v>1.8125570820298824E+19</v>
       </c>
       <c r="E296" s="5">
-        <v>72615718</v>
+        <v>145231436</v>
       </c>
       <c r="F296" s="5">
         <v>2.5201501361141504E+32</v>
@@ -7923,10 +7923,10 @@
       </c>
       <c r="C297" s="2"/>
       <c r="D297" s="5">
-        <v>4.0601278637469368E+19</v>
+        <v>2.0300639318734684E+19</v>
       </c>
       <c r="E297" s="5">
-        <v>73491177</v>
+        <v>146982354</v>
       </c>
       <c r="F297" s="5">
         <v>3.6542176973655177E+32</v>
@@ -7948,10 +7948,10 @@
       </c>
       <c r="C298" s="2"/>
       <c r="D298" s="5">
-        <v>4.5473432073965699E+19</v>
+        <v>2.273671603698285E+19</v>
       </c>
       <c r="E298" s="5">
-        <v>74371882</v>
+        <v>148743764</v>
       </c>
       <c r="F298" s="5">
         <v>5.2986156611800007E+32</v>
@@ -7973,10 +7973,10 @@
       </c>
       <c r="C299" s="2"/>
       <c r="D299" s="5">
-        <v>5.0930243922841592E+19</v>
+        <v>2.5465121961420796E+19</v>
       </c>
       <c r="E299" s="5">
-        <v>75257833</v>
+        <v>150515666</v>
       </c>
       <c r="F299" s="5">
         <v>7.6829927087110012E+32</v>
@@ -7998,10 +7998,10 @@
       </c>
       <c r="C300" s="2"/>
       <c r="D300" s="5">
-        <v>5.7041873193582592E+19</v>
+        <v>2.8520936596791296E+19</v>
       </c>
       <c r="E300" s="5">
-        <v>76161108</v>
+        <v>152322216</v>
       </c>
       <c r="F300" s="5">
         <v>1.1140339427630951E+33</v>
@@ -8023,10 +8023,10 @@
       </c>
       <c r="C301" s="2"/>
       <c r="D301" s="5">
-        <v>6.3886897976812511E+19</v>
+        <v>3.1943448988406256E+19</v>
       </c>
       <c r="E301" s="5">
-        <v>77069771</v>
+        <v>154139542</v>
       </c>
       <c r="F301" s="5">
         <v>1.615349217006488E+33</v>
@@ -8048,10 +8048,10 @@
       </c>
       <c r="C302" s="2"/>
       <c r="D302" s="5">
-        <v>7.1553325734030017E+19</v>
+        <v>3.5776662867015008E+19</v>
       </c>
       <c r="E302" s="5">
-        <v>80383326</v>
+        <v>160766652</v>
       </c>
       <c r="F302" s="5">
         <v>2.3422563646594074E+33</v>

</xml_diff>

<commit_message>
[🛠️Fix] Stage Balance fix
- 스테이지 밸런스 수정
- 체력회복에 장비 보유효과 적용되게 수정
</commit_message>
<xml_diff>
--- a/IdleGame/Assets/@Resources/Texts/ExcelTable/StageTable.xlsx
+++ b/IdleGame/Assets/@Resources/Texts/ExcelTable/StageTable.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Project\TeamProject-IdleGame\IdleGame\Assets\@Resources\Texts\ExcelTable\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E60FD034-ED13-4C1C-B84E-76B4BF55BB6A}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{07EDDC9B-7B36-40A4-ACB4-36E9E4459C5E}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="28680" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Stage" sheetId="1" r:id="rId1"/>
@@ -139,7 +139,7 @@
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
   <numFmts count="1">
-    <numFmt numFmtId="178" formatCode="0_);[Red]\(0\)"/>
+    <numFmt numFmtId="176" formatCode="0_);[Red]\(0\)"/>
   </numFmts>
   <fonts count="3" x14ac:knownFonts="1">
     <font>
@@ -210,7 +210,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
       <alignment horizontal="right"/>
     </xf>
-    <xf numFmtId="178" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
+    <xf numFmtId="176" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
       <alignment horizontal="right"/>
     </xf>
   </cellXfs>
@@ -218,50 +218,6 @@
     <cellStyle name="표준" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="20">
-    <dxf>
-      <numFmt numFmtId="178" formatCode="0_);[Red]\(0\)"/>
-      <alignment horizontal="right" vertical="bottom" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
-    </dxf>
-    <dxf>
-      <alignment horizontal="right" vertical="bottom" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
-    </dxf>
-    <dxf>
-      <numFmt numFmtId="178" formatCode="0_);[Red]\(0\)"/>
-      <alignment horizontal="right" vertical="bottom" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
-    </dxf>
-    <dxf>
-      <numFmt numFmtId="178" formatCode="0_);[Red]\(0\)"/>
-      <alignment horizontal="right" vertical="bottom" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
-    </dxf>
-    <dxf>
-      <alignment horizontal="right" vertical="bottom" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
-    </dxf>
-    <dxf>
-      <alignment horizontal="right" vertical="bottom" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
-    </dxf>
-    <dxf>
-      <numFmt numFmtId="0" formatCode="General"/>
-      <alignment horizontal="right" vertical="bottom" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
-    </dxf>
-    <dxf>
-      <alignment horizontal="right" vertical="bottom" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
-    </dxf>
-    <dxf>
-      <numFmt numFmtId="0" formatCode="General"/>
-      <alignment horizontal="right" vertical="bottom" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
-    </dxf>
-    <dxf>
-      <alignment horizontal="right" vertical="bottom" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
-    </dxf>
-    <dxf>
-      <alignment horizontal="right" vertical="bottom" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
-    </dxf>
-    <dxf>
-      <alignment horizontal="right" vertical="bottom" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
-    </dxf>
-    <dxf>
-      <alignment horizontal="right" vertical="bottom" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
-    </dxf>
     <dxf>
       <alignment horizontal="right" vertical="bottom" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
     </dxf>
@@ -286,6 +242,50 @@
     </dxf>
     <dxf>
       <numFmt numFmtId="0" formatCode="General"/>
+      <alignment horizontal="right" vertical="bottom" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <numFmt numFmtId="0" formatCode="General"/>
+      <alignment horizontal="right" vertical="bottom" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <alignment horizontal="right" vertical="bottom" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <alignment horizontal="right" vertical="bottom" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <numFmt numFmtId="0" formatCode="General"/>
+      <alignment horizontal="right" vertical="bottom" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <numFmt numFmtId="176" formatCode="0_);[Red]\(0\)"/>
+      <alignment horizontal="right" vertical="bottom" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <alignment horizontal="right" vertical="bottom" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <numFmt numFmtId="176" formatCode="0_);[Red]\(0\)"/>
+      <alignment horizontal="right" vertical="bottom" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <alignment horizontal="right" vertical="bottom" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <numFmt numFmtId="176" formatCode="0_);[Red]\(0\)"/>
+      <alignment horizontal="right" vertical="bottom" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <alignment horizontal="right" vertical="bottom" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <alignment horizontal="right" vertical="bottom" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <alignment horizontal="right" vertical="bottom" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
       <alignment horizontal="right" vertical="bottom" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
     </dxf>
     <dxf>
@@ -327,25 +327,25 @@
 <table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="1" xr:uid="{50268604-F68E-4DBD-AE64-4183B0FE7F47}" name="표1" displayName="표1" ref="A2:H302" totalsRowShown="0" headerRowDxfId="19">
   <autoFilter ref="A2:H302" xr:uid="{50268604-F68E-4DBD-AE64-4183B0FE7F47}"/>
   <tableColumns count="8">
-    <tableColumn id="1" xr3:uid="{ABEFAF0D-3E9C-4BC0-BD85-867C72E372D9}" name="Index : Int" dataDxfId="18" totalsRowDxfId="12"/>
-    <tableColumn id="4" xr3:uid="{9A52DE84-B46A-41BA-9891-9221E6FD8CA2}" name="StageConfig : String" dataDxfId="17" totalsRowDxfId="11"/>
-    <tableColumn id="5" xr3:uid="{52BABBB3-0B5B-4EA5-A096-52FE17505682}" name="StageBackground : String" dataDxfId="4" totalsRowDxfId="10"/>
-    <tableColumn id="6" xr3:uid="{8CB87B44-9BE8-4447-B7A9-5AB6AF555193}" name="EnemyHpRate : long" dataDxfId="3" totalsRowDxfId="9"/>
-    <tableColumn id="3" xr3:uid="{D9A76B69-1806-4056-859C-537F7DF173E6}" name="EnemyAttackRate : long" dataDxfId="2" totalsRowDxfId="5"/>
-    <tableColumn id="7" xr3:uid="{70C60707-1493-4007-90DF-8D1A8171AA79}" name="EnemyGoldRate : long" dataDxfId="0" totalsRowDxfId="8"/>
-    <tableColumn id="8" xr3:uid="{A1894453-017C-4920-B6D4-6CCC399479DE}" name="EnemySpawnCount : Int" dataDxfId="1" totalsRowDxfId="7"/>
-    <tableColumn id="2" xr3:uid="{27B9ED74-E3F2-4B5B-AF69-453766BB11DC}" name="IdleGoldReward : Int" dataDxfId="16" totalsRowDxfId="6"/>
+    <tableColumn id="1" xr3:uid="{ABEFAF0D-3E9C-4BC0-BD85-867C72E372D9}" name="Index : Int" dataDxfId="18" totalsRowDxfId="17"/>
+    <tableColumn id="4" xr3:uid="{9A52DE84-B46A-41BA-9891-9221E6FD8CA2}" name="StageConfig : String" dataDxfId="16" totalsRowDxfId="15"/>
+    <tableColumn id="5" xr3:uid="{52BABBB3-0B5B-4EA5-A096-52FE17505682}" name="StageBackground : String" dataDxfId="14" totalsRowDxfId="13"/>
+    <tableColumn id="6" xr3:uid="{8CB87B44-9BE8-4447-B7A9-5AB6AF555193}" name="EnemyHpRate : long" dataDxfId="12" totalsRowDxfId="11"/>
+    <tableColumn id="3" xr3:uid="{D9A76B69-1806-4056-859C-537F7DF173E6}" name="EnemyAttackRate : long" dataDxfId="10" totalsRowDxfId="9"/>
+    <tableColumn id="7" xr3:uid="{70C60707-1493-4007-90DF-8D1A8171AA79}" name="EnemyGoldRate : long" dataDxfId="8" totalsRowDxfId="7"/>
+    <tableColumn id="8" xr3:uid="{A1894453-017C-4920-B6D4-6CCC399479DE}" name="EnemySpawnCount : Int" dataDxfId="6" totalsRowDxfId="5"/>
+    <tableColumn id="2" xr3:uid="{27B9ED74-E3F2-4B5B-AF69-453766BB11DC}" name="IdleGoldReward : Int" dataDxfId="4" totalsRowDxfId="3"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleMedium6" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
 </file>
 
 <file path=xl/tables/table2.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="3" xr:uid="{35A1E681-9A85-48AE-96D7-A93EDF20787E}" name="표1_4" displayName="표1_4" ref="A2:B6" totalsRowShown="0" headerRowDxfId="15">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="3" xr:uid="{35A1E681-9A85-48AE-96D7-A93EDF20787E}" name="표1_4" displayName="표1_4" ref="A2:B6" totalsRowShown="0" headerRowDxfId="2">
   <autoFilter ref="A2:B6" xr:uid="{35A1E681-9A85-48AE-96D7-A93EDF20787E}"/>
   <tableColumns count="2">
-    <tableColumn id="1" xr3:uid="{BE9E670A-5042-4FEB-9281-05CB3F81C035}" name="Index : Int" dataDxfId="14"/>
-    <tableColumn id="4" xr3:uid="{0BE49A32-760A-4534-B1B8-33AAC060FE89}" name="UIText : String" dataDxfId="13"/>
+    <tableColumn id="1" xr3:uid="{BE9E670A-5042-4FEB-9281-05CB3F81C035}" name="Index : Int" dataDxfId="1"/>
+    <tableColumn id="4" xr3:uid="{0BE49A32-760A-4534-B1B8-33AAC060FE89}" name="UIText : String" dataDxfId="0"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleMedium6" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
@@ -617,7 +617,7 @@
   <dimension ref="A1:H302"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="E2" sqref="E2"/>
+      <selection activeCell="G10" sqref="G10"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="16.5" x14ac:dyDescent="0.3"/>
@@ -674,7 +674,7 @@
         <v>1</v>
       </c>
       <c r="E3" s="5">
-        <v>5</v>
+        <v>11</v>
       </c>
       <c r="F3" s="5">
         <v>1</v>
@@ -698,7 +698,7 @@
         <v>2</v>
       </c>
       <c r="E4" s="5">
-        <v>6</v>
+        <v>14</v>
       </c>
       <c r="F4" s="5">
         <v>2</v>
@@ -722,7 +722,7 @@
         <v>4</v>
       </c>
       <c r="E5" s="5">
-        <v>7</v>
+        <v>16</v>
       </c>
       <c r="F5" s="5">
         <v>3</v>
@@ -743,10 +743,10 @@
       </c>
       <c r="C6" s="2"/>
       <c r="D6" s="5">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="E6" s="5">
-        <v>8</v>
+        <v>19</v>
       </c>
       <c r="F6" s="5">
         <v>4</v>
@@ -767,10 +767,10 @@
       </c>
       <c r="C7" s="2"/>
       <c r="D7" s="5">
-        <v>11</v>
+        <v>9</v>
       </c>
       <c r="E7" s="5">
-        <v>9</v>
+        <v>23</v>
       </c>
       <c r="F7" s="5">
         <v>5</v>
@@ -791,10 +791,10 @@
       </c>
       <c r="C8" s="2"/>
       <c r="D8" s="5">
-        <v>16</v>
+        <v>13</v>
       </c>
       <c r="E8" s="5">
-        <v>11</v>
+        <v>27</v>
       </c>
       <c r="F8" s="5">
         <v>6</v>
@@ -815,10 +815,10 @@
       </c>
       <c r="C9" s="2"/>
       <c r="D9" s="5">
-        <v>24</v>
+        <v>19</v>
       </c>
       <c r="E9" s="5">
-        <v>13</v>
+        <v>31</v>
       </c>
       <c r="F9" s="5">
         <v>7</v>
@@ -842,7 +842,7 @@
         <v>38</v>
       </c>
       <c r="E10" s="5">
-        <v>15</v>
+        <v>38</v>
       </c>
       <c r="F10" s="5">
         <v>8</v>
@@ -866,7 +866,7 @@
         <v>57</v>
       </c>
       <c r="E11" s="5">
-        <v>18</v>
+        <v>44</v>
       </c>
       <c r="F11" s="5">
         <v>10</v>
@@ -890,7 +890,7 @@
         <v>85</v>
       </c>
       <c r="E12" s="5">
-        <v>21</v>
+        <v>51</v>
       </c>
       <c r="F12" s="5">
         <v>12</v>
@@ -914,7 +914,7 @@
         <v>127</v>
       </c>
       <c r="E13" s="5">
-        <v>24</v>
+        <v>59</v>
       </c>
       <c r="F13" s="5">
         <v>13</v>
@@ -935,10 +935,10 @@
       </c>
       <c r="C14" s="2"/>
       <c r="D14" s="5">
-        <v>190</v>
+        <v>152</v>
       </c>
       <c r="E14" s="5">
-        <v>27</v>
+        <v>65</v>
       </c>
       <c r="F14" s="5">
         <v>14</v>
@@ -959,10 +959,10 @@
       </c>
       <c r="C15" s="2"/>
       <c r="D15" s="5">
-        <v>285</v>
+        <v>182</v>
       </c>
       <c r="E15" s="5">
-        <v>29</v>
+        <v>71</v>
       </c>
       <c r="F15" s="5">
         <v>15</v>
@@ -983,10 +983,10 @@
       </c>
       <c r="C16" s="2"/>
       <c r="D16" s="5">
-        <v>427</v>
+        <v>218</v>
       </c>
       <c r="E16" s="5">
-        <v>33</v>
+        <v>80</v>
       </c>
       <c r="F16" s="5">
         <v>16</v>
@@ -1007,10 +1007,10 @@
       </c>
       <c r="C17" s="2"/>
       <c r="D17" s="5">
-        <v>640</v>
+        <v>261</v>
       </c>
       <c r="E17" s="5">
-        <v>37</v>
+        <v>89</v>
       </c>
       <c r="F17" s="5">
         <v>17</v>
@@ -1031,10 +1031,10 @@
       </c>
       <c r="C18" s="2"/>
       <c r="D18" s="5">
-        <v>896</v>
+        <v>313</v>
       </c>
       <c r="E18" s="5">
-        <v>40</v>
+        <v>98</v>
       </c>
       <c r="F18" s="5">
         <v>18</v>
@@ -1055,10 +1055,10 @@
       </c>
       <c r="C19" s="2"/>
       <c r="D19" s="5">
-        <v>1164</v>
+        <v>375</v>
       </c>
       <c r="E19" s="5">
-        <v>44</v>
+        <v>108</v>
       </c>
       <c r="F19" s="5">
         <v>19</v>
@@ -1079,10 +1079,10 @@
       </c>
       <c r="C20" s="2"/>
       <c r="D20" s="5">
-        <v>1513</v>
+        <v>450</v>
       </c>
       <c r="E20" s="5">
-        <v>50</v>
+        <v>121</v>
       </c>
       <c r="F20" s="5">
         <v>20</v>
@@ -1103,10 +1103,10 @@
       </c>
       <c r="C21" s="2"/>
       <c r="D21" s="5">
-        <v>1966</v>
+        <v>540</v>
       </c>
       <c r="E21" s="5">
-        <v>55</v>
+        <v>134</v>
       </c>
       <c r="F21" s="5">
         <v>22</v>
@@ -1127,10 +1127,10 @@
       </c>
       <c r="C22" s="2"/>
       <c r="D22" s="5">
-        <v>2555</v>
+        <v>648</v>
       </c>
       <c r="E22" s="5">
-        <v>61</v>
+        <v>148</v>
       </c>
       <c r="F22" s="5">
         <v>24</v>
@@ -1151,10 +1151,10 @@
       </c>
       <c r="C23" s="2"/>
       <c r="D23" s="5">
-        <v>3321</v>
+        <v>907</v>
       </c>
       <c r="E23" s="5">
-        <v>67</v>
+        <v>189</v>
       </c>
       <c r="F23" s="5">
         <v>26</v>
@@ -1175,10 +1175,10 @@
       </c>
       <c r="C24" s="2"/>
       <c r="D24" s="5">
-        <v>4317</v>
+        <v>1133</v>
       </c>
       <c r="E24" s="5">
-        <v>74</v>
+        <v>210</v>
       </c>
       <c r="F24" s="5">
         <v>28</v>
@@ -1199,10 +1199,10 @@
       </c>
       <c r="C25" s="2"/>
       <c r="D25" s="5">
-        <v>5612</v>
+        <v>1416</v>
       </c>
       <c r="E25" s="5">
-        <v>82</v>
+        <v>233</v>
       </c>
       <c r="F25" s="5">
         <v>30</v>
@@ -1223,10 +1223,10 @@
       </c>
       <c r="C26" s="2"/>
       <c r="D26" s="5">
-        <v>7295</v>
+        <v>1770</v>
       </c>
       <c r="E26" s="5">
-        <v>91</v>
+        <v>256</v>
       </c>
       <c r="F26" s="5">
         <v>33</v>
@@ -1247,10 +1247,10 @@
       </c>
       <c r="C27" s="2"/>
       <c r="D27" s="5">
-        <v>9483</v>
+        <v>2212</v>
       </c>
       <c r="E27" s="5">
-        <v>99</v>
+        <v>280</v>
       </c>
       <c r="F27" s="5">
         <v>36</v>
@@ -1271,10 +1271,10 @@
       </c>
       <c r="C28" s="2"/>
       <c r="D28" s="5">
-        <v>12327</v>
+        <v>2765</v>
       </c>
       <c r="E28" s="5">
-        <v>110</v>
+        <v>310</v>
       </c>
       <c r="F28" s="5">
         <v>39</v>
@@ -1295,10 +1295,10 @@
       </c>
       <c r="C29" s="2"/>
       <c r="D29" s="5">
-        <v>16025</v>
+        <v>3456</v>
       </c>
       <c r="E29" s="5">
-        <v>121</v>
+        <v>341</v>
       </c>
       <c r="F29" s="5">
         <v>42</v>
@@ -1319,10 +1319,10 @@
       </c>
       <c r="C30" s="2"/>
       <c r="D30" s="5">
-        <v>20832</v>
+        <v>4320</v>
       </c>
       <c r="E30" s="5">
-        <v>132</v>
+        <v>373</v>
       </c>
       <c r="F30" s="5">
         <v>46</v>
@@ -1343,10 +1343,10 @@
       </c>
       <c r="C31" s="2"/>
       <c r="D31" s="5">
-        <v>27081</v>
+        <v>5400</v>
       </c>
       <c r="E31" s="5">
-        <v>144</v>
+        <v>407</v>
       </c>
       <c r="F31" s="5">
         <v>50</v>
@@ -1367,10 +1367,10 @@
       </c>
       <c r="C32" s="2"/>
       <c r="D32" s="5">
-        <v>35205</v>
+        <v>6750</v>
       </c>
       <c r="E32" s="5">
-        <v>166</v>
+        <v>468</v>
       </c>
       <c r="F32" s="5">
         <v>55</v>
@@ -1391,10 +1391,10 @@
       </c>
       <c r="C33" s="2"/>
       <c r="D33" s="5">
-        <v>42246</v>
+        <v>8437</v>
       </c>
       <c r="E33" s="5">
-        <v>182</v>
+        <v>512</v>
       </c>
       <c r="F33" s="5">
         <v>60</v>
@@ -1415,10 +1415,10 @@
       </c>
       <c r="C34" s="2"/>
       <c r="D34" s="5">
-        <v>50695</v>
+        <v>10546</v>
       </c>
       <c r="E34" s="5">
-        <v>198</v>
+        <v>558</v>
       </c>
       <c r="F34" s="5">
         <v>66</v>
@@ -1439,10 +1439,10 @@
       </c>
       <c r="C35" s="2"/>
       <c r="D35" s="5">
-        <v>60834</v>
+        <v>13182</v>
       </c>
       <c r="E35" s="5">
-        <v>215</v>
+        <v>606</v>
       </c>
       <c r="F35" s="5">
         <v>72</v>
@@ -1463,10 +1463,10 @@
       </c>
       <c r="C36" s="2"/>
       <c r="D36" s="5">
-        <v>73000</v>
+        <v>16477</v>
       </c>
       <c r="E36" s="5">
-        <v>235</v>
+        <v>662</v>
       </c>
       <c r="F36" s="5">
         <v>79</v>
@@ -1487,10 +1487,10 @@
       </c>
       <c r="C37" s="2"/>
       <c r="D37" s="5">
-        <v>87600</v>
+        <v>20596</v>
       </c>
       <c r="E37" s="5">
-        <v>256</v>
+        <v>720</v>
       </c>
       <c r="F37" s="5">
         <v>86</v>
@@ -1511,10 +1511,10 @@
       </c>
       <c r="C38" s="2"/>
       <c r="D38" s="5">
-        <v>105120</v>
+        <v>25745</v>
       </c>
       <c r="E38" s="5">
-        <v>277</v>
+        <v>781</v>
       </c>
       <c r="F38" s="5">
         <v>94</v>
@@ -1535,10 +1535,10 @@
       </c>
       <c r="C39" s="2"/>
       <c r="D39" s="5">
-        <v>126144</v>
+        <v>32181</v>
       </c>
       <c r="E39" s="5">
-        <v>300</v>
+        <v>844</v>
       </c>
       <c r="F39" s="5">
         <v>103</v>
@@ -1559,10 +1559,10 @@
       </c>
       <c r="C40" s="2"/>
       <c r="D40" s="5">
-        <v>151372</v>
+        <v>40226</v>
       </c>
       <c r="E40" s="5">
-        <v>326</v>
+        <v>918</v>
       </c>
       <c r="F40" s="5">
         <v>113</v>
@@ -1583,10 +1583,10 @@
       </c>
       <c r="C41" s="2"/>
       <c r="D41" s="5">
-        <v>181646</v>
+        <v>50282</v>
       </c>
       <c r="E41" s="5">
-        <v>353</v>
+        <v>994</v>
       </c>
       <c r="F41" s="5">
         <v>124</v>
@@ -1607,10 +1607,10 @@
       </c>
       <c r="C42" s="2"/>
       <c r="D42" s="5">
-        <v>217975</v>
+        <v>62852</v>
       </c>
       <c r="E42" s="5">
-        <v>397</v>
+        <v>1120</v>
       </c>
       <c r="F42" s="5">
         <v>136</v>
@@ -1631,10 +1631,10 @@
       </c>
       <c r="C43" s="2"/>
       <c r="D43" s="5">
-        <v>261570</v>
+        <v>78565</v>
       </c>
       <c r="E43" s="5">
-        <v>428</v>
+        <v>1205</v>
       </c>
       <c r="F43" s="5">
         <v>149</v>
@@ -1655,10 +1655,10 @@
       </c>
       <c r="C44" s="2"/>
       <c r="D44" s="5">
-        <v>313884</v>
+        <v>98206</v>
       </c>
       <c r="E44" s="5">
-        <v>463</v>
+        <v>1303</v>
       </c>
       <c r="F44" s="5">
         <v>163</v>
@@ -1679,10 +1679,10 @@
       </c>
       <c r="C45" s="2"/>
       <c r="D45" s="5">
-        <v>376660</v>
+        <v>122757</v>
       </c>
       <c r="E45" s="5">
-        <v>499</v>
+        <v>1404</v>
       </c>
       <c r="F45" s="5">
         <v>179</v>
@@ -1703,10 +1703,10 @@
       </c>
       <c r="C46" s="2"/>
       <c r="D46" s="5">
-        <v>451992</v>
+        <v>153446</v>
       </c>
       <c r="E46" s="5">
-        <v>536</v>
+        <v>1510</v>
       </c>
       <c r="F46" s="5">
         <v>196</v>
@@ -1727,10 +1727,10 @@
       </c>
       <c r="C47" s="2"/>
       <c r="D47" s="5">
-        <v>542390</v>
+        <v>191807</v>
       </c>
       <c r="E47" s="5">
-        <v>575</v>
+        <v>1619</v>
       </c>
       <c r="F47" s="5">
         <v>215</v>
@@ -1751,10 +1751,10 @@
       </c>
       <c r="C48" s="2"/>
       <c r="D48" s="5">
-        <v>650868</v>
+        <v>239758</v>
       </c>
       <c r="E48" s="5">
-        <v>618</v>
+        <v>1742</v>
       </c>
       <c r="F48" s="5">
         <v>236</v>
@@ -1775,10 +1775,10 @@
       </c>
       <c r="C49" s="2"/>
       <c r="D49" s="5">
-        <v>781041</v>
+        <v>299697</v>
       </c>
       <c r="E49" s="5">
-        <v>664</v>
+        <v>1869</v>
       </c>
       <c r="F49" s="5">
         <v>259</v>
@@ -1799,10 +1799,10 @@
       </c>
       <c r="C50" s="2"/>
       <c r="D50" s="5">
-        <v>937249</v>
+        <v>374621</v>
       </c>
       <c r="E50" s="5">
-        <v>711</v>
+        <v>2001</v>
       </c>
       <c r="F50" s="5">
         <v>284</v>
@@ -1823,10 +1823,10 @@
       </c>
       <c r="C51" s="2"/>
       <c r="D51" s="5">
-        <v>1124698</v>
+        <v>468276</v>
       </c>
       <c r="E51" s="5">
-        <v>759</v>
+        <v>2138</v>
       </c>
       <c r="F51" s="5">
         <v>312</v>
@@ -1847,10 +1847,10 @@
       </c>
       <c r="C52" s="2"/>
       <c r="D52" s="5">
-        <v>1349637</v>
+        <v>561931</v>
       </c>
       <c r="E52" s="5">
-        <v>1048</v>
+        <v>2950</v>
       </c>
       <c r="F52" s="5">
         <v>343</v>
@@ -1871,10 +1871,10 @@
       </c>
       <c r="C53" s="2"/>
       <c r="D53" s="5">
-        <v>1619564</v>
+        <v>674317</v>
       </c>
       <c r="E53" s="5">
-        <v>1120</v>
+        <v>3153</v>
       </c>
       <c r="F53" s="5">
         <v>377</v>
@@ -1895,10 +1895,10 @@
       </c>
       <c r="C54" s="2"/>
       <c r="D54" s="5">
-        <v>1943476</v>
+        <v>809180</v>
       </c>
       <c r="E54" s="5">
-        <v>1195</v>
+        <v>3363</v>
       </c>
       <c r="F54" s="5">
         <v>414</v>
@@ -1919,10 +1919,10 @@
       </c>
       <c r="C55" s="2"/>
       <c r="D55" s="5">
-        <v>2332171</v>
+        <v>971016</v>
       </c>
       <c r="E55" s="5">
-        <v>1272</v>
+        <v>3580</v>
       </c>
       <c r="F55" s="5">
         <v>455</v>
@@ -1943,10 +1943,10 @@
       </c>
       <c r="C56" s="2"/>
       <c r="D56" s="5">
-        <v>2798605</v>
+        <v>1165219</v>
       </c>
       <c r="E56" s="5">
-        <v>1357</v>
+        <v>3822</v>
       </c>
       <c r="F56" s="5">
         <v>500</v>
@@ -1967,10 +1967,10 @@
       </c>
       <c r="C57" s="2"/>
       <c r="D57" s="5">
-        <v>3358326</v>
+        <v>1398262</v>
       </c>
       <c r="E57" s="5">
-        <v>1446</v>
+        <v>4071</v>
       </c>
       <c r="F57" s="5">
         <v>550</v>
@@ -1991,10 +1991,10 @@
       </c>
       <c r="C58" s="2"/>
       <c r="D58" s="5">
-        <v>4029991</v>
+        <v>1677914</v>
       </c>
       <c r="E58" s="5">
-        <v>1537</v>
+        <v>4328</v>
       </c>
       <c r="F58" s="5">
         <v>605</v>
@@ -2015,10 +2015,10 @@
       </c>
       <c r="C59" s="2"/>
       <c r="D59" s="5">
-        <v>4835989</v>
+        <v>2013496</v>
       </c>
       <c r="E59" s="5">
-        <v>1631</v>
+        <v>4592</v>
       </c>
       <c r="F59" s="5">
         <v>665</v>
@@ -2039,10 +2039,10 @@
       </c>
       <c r="C60" s="2"/>
       <c r="D60" s="5">
-        <v>5803186</v>
+        <v>2416195</v>
       </c>
       <c r="E60" s="5">
-        <v>1735</v>
+        <v>4884</v>
       </c>
       <c r="F60" s="5">
         <v>731</v>
@@ -2063,10 +2063,10 @@
       </c>
       <c r="C61" s="2"/>
       <c r="D61" s="5">
-        <v>6963823</v>
+        <v>2899434</v>
       </c>
       <c r="E61" s="5">
-        <v>1842</v>
+        <v>5185</v>
       </c>
       <c r="F61" s="5">
         <v>804</v>
@@ -2087,10 +2087,10 @@
       </c>
       <c r="C62" s="2"/>
       <c r="D62" s="5">
-        <v>8356587</v>
+        <v>3479320</v>
       </c>
       <c r="E62" s="5">
-        <v>2027</v>
+        <v>5707</v>
       </c>
       <c r="F62" s="5">
         <v>884</v>
@@ -2111,10 +2111,10 @@
       </c>
       <c r="C63" s="2"/>
       <c r="D63" s="5">
-        <v>10027904</v>
+        <v>4175184</v>
       </c>
       <c r="E63" s="5">
-        <v>2145</v>
+        <v>6038</v>
       </c>
       <c r="F63" s="5">
         <v>972</v>
@@ -2135,10 +2135,10 @@
       </c>
       <c r="C64" s="2"/>
       <c r="D64" s="5">
-        <v>12033484</v>
+        <v>5010220</v>
       </c>
       <c r="E64" s="5">
-        <v>2274</v>
+        <v>6402</v>
       </c>
       <c r="F64" s="5">
         <v>1069</v>
@@ -2159,10 +2159,10 @@
       </c>
       <c r="C65" s="2"/>
       <c r="D65" s="5">
-        <v>14440180</v>
+        <v>6012264</v>
       </c>
       <c r="E65" s="5">
-        <v>2407</v>
+        <v>6776</v>
       </c>
       <c r="F65" s="5">
         <v>1175</v>
@@ -2183,10 +2183,10 @@
       </c>
       <c r="C66" s="2"/>
       <c r="D66" s="5">
-        <v>17328216</v>
+        <v>7214716</v>
       </c>
       <c r="E66" s="5">
-        <v>2544</v>
+        <v>7161</v>
       </c>
       <c r="F66" s="5">
         <v>1292</v>
@@ -2207,10 +2207,10 @@
       </c>
       <c r="C67" s="2"/>
       <c r="D67" s="5">
-        <v>20793859</v>
+        <v>8657659</v>
       </c>
       <c r="E67" s="5">
-        <v>2684</v>
+        <v>7556</v>
       </c>
       <c r="F67" s="5">
         <v>1421</v>
@@ -2231,10 +2231,10 @@
       </c>
       <c r="C68" s="2"/>
       <c r="D68" s="5">
-        <v>24952630</v>
+        <v>10389190</v>
       </c>
       <c r="E68" s="5">
-        <v>2838</v>
+        <v>7988</v>
       </c>
       <c r="F68" s="5">
         <v>1563</v>
@@ -2255,10 +2255,10 @@
       </c>
       <c r="C69" s="2"/>
       <c r="D69" s="5">
-        <v>29943156</v>
+        <v>12467028</v>
       </c>
       <c r="E69" s="5">
-        <v>2995</v>
+        <v>8432</v>
       </c>
       <c r="F69" s="5">
         <v>1719</v>
@@ -2279,10 +2279,10 @@
       </c>
       <c r="C70" s="2"/>
       <c r="D70" s="5">
-        <v>35931787</v>
+        <v>14960433</v>
       </c>
       <c r="E70" s="5">
-        <v>3157</v>
+        <v>8887</v>
       </c>
       <c r="F70" s="5">
         <v>1890</v>
@@ -2303,10 +2303,10 @@
       </c>
       <c r="C71" s="2"/>
       <c r="D71" s="5">
-        <v>43118144</v>
+        <v>17952519</v>
       </c>
       <c r="E71" s="5">
-        <v>3323</v>
+        <v>9355</v>
       </c>
       <c r="F71" s="5">
         <v>2079</v>
@@ -2327,10 +2327,10 @@
       </c>
       <c r="C72" s="2"/>
       <c r="D72" s="5">
-        <v>51741772</v>
+        <v>21543022</v>
       </c>
       <c r="E72" s="5">
-        <v>4247</v>
+        <v>15942</v>
       </c>
       <c r="F72" s="5">
         <v>2286</v>
@@ -2351,10 +2351,10 @@
       </c>
       <c r="C73" s="2"/>
       <c r="D73" s="5">
-        <v>62090126</v>
+        <v>25851626</v>
       </c>
       <c r="E73" s="5">
-        <v>4472</v>
+        <v>16785</v>
       </c>
       <c r="F73" s="5">
         <v>2514</v>
@@ -2375,10 +2375,10 @@
       </c>
       <c r="C74" s="2"/>
       <c r="D74" s="5">
-        <v>74508151</v>
+        <v>31021951</v>
       </c>
       <c r="E74" s="5">
-        <v>4702</v>
+        <v>17650</v>
       </c>
       <c r="F74" s="5">
         <v>2765</v>
@@ -2399,10 +2399,10 @@
       </c>
       <c r="C75" s="2"/>
       <c r="D75" s="5">
-        <v>89409781</v>
+        <v>37226341</v>
       </c>
       <c r="E75" s="5">
-        <v>4938</v>
+        <v>18536</v>
       </c>
       <c r="F75" s="5">
         <v>3041</v>
@@ -2423,10 +2423,10 @@
       </c>
       <c r="C76" s="2"/>
       <c r="D76" s="5">
-        <v>107291737</v>
+        <v>44671609</v>
       </c>
       <c r="E76" s="5">
-        <v>5194</v>
+        <v>19494</v>
       </c>
       <c r="F76" s="5">
         <v>3345</v>
@@ -2447,10 +2447,10 @@
       </c>
       <c r="C77" s="2"/>
       <c r="D77" s="5">
-        <v>128750084</v>
+        <v>53605930</v>
       </c>
       <c r="E77" s="5">
-        <v>5456</v>
+        <v>20477</v>
       </c>
       <c r="F77" s="5">
         <v>3679</v>
@@ -2471,10 +2471,10 @@
       </c>
       <c r="C78" s="2"/>
       <c r="D78" s="5">
-        <v>154500100</v>
+        <v>64327116</v>
       </c>
       <c r="E78" s="5">
-        <v>5724</v>
+        <v>21484</v>
       </c>
       <c r="F78" s="5">
         <v>4046</v>
@@ -2495,10 +2495,10 @@
       </c>
       <c r="C79" s="2"/>
       <c r="D79" s="5">
-        <v>185400120</v>
+        <v>77192539</v>
       </c>
       <c r="E79" s="5">
-        <v>5999</v>
+        <v>22516</v>
       </c>
       <c r="F79" s="5">
         <v>4450</v>
@@ -2519,10 +2519,10 @@
       </c>
       <c r="C80" s="2"/>
       <c r="D80" s="5">
-        <v>222480144</v>
+        <v>92631046</v>
       </c>
       <c r="E80" s="5">
-        <v>6295</v>
+        <v>23627</v>
       </c>
       <c r="F80" s="5">
         <v>4895</v>
@@ -2543,10 +2543,10 @@
       </c>
       <c r="C81" s="2"/>
       <c r="D81" s="5">
-        <v>266976172</v>
+        <v>111157255</v>
       </c>
       <c r="E81" s="5">
-        <v>6598</v>
+        <v>24765</v>
       </c>
       <c r="F81" s="5">
         <v>5384</v>
@@ -2567,10 +2567,10 @@
       </c>
       <c r="C82" s="2"/>
       <c r="D82" s="5">
-        <v>320371406</v>
+        <v>133388706</v>
       </c>
       <c r="E82" s="5">
-        <v>7155</v>
+        <v>26856</v>
       </c>
       <c r="F82" s="5">
         <v>5922</v>
@@ -2591,10 +2591,10 @@
       </c>
       <c r="C83" s="2"/>
       <c r="D83" s="5">
-        <v>384445687</v>
+        <v>160066447</v>
       </c>
       <c r="E83" s="5">
-        <v>7601</v>
+        <v>28529</v>
       </c>
       <c r="F83" s="5">
         <v>7106</v>
@@ -2615,10 +2615,10 @@
       </c>
       <c r="C84" s="2"/>
       <c r="D84" s="5">
-        <v>461334824</v>
+        <v>192079736</v>
       </c>
       <c r="E84" s="5">
-        <v>8060</v>
+        <v>30252</v>
       </c>
       <c r="F84" s="5">
         <v>8527</v>
@@ -2639,10 +2639,10 @@
       </c>
       <c r="C85" s="2"/>
       <c r="D85" s="5">
-        <v>553601788</v>
+        <v>230495683</v>
       </c>
       <c r="E85" s="5">
-        <v>8551</v>
+        <v>32092</v>
       </c>
       <c r="F85" s="5">
         <v>10232</v>
@@ -2663,10 +2663,10 @@
       </c>
       <c r="C86" s="2"/>
       <c r="D86" s="5">
-        <v>664322145</v>
+        <v>276594819</v>
       </c>
       <c r="E86" s="5">
-        <v>9055</v>
+        <v>33987</v>
       </c>
       <c r="F86" s="5">
         <v>12278</v>
@@ -2687,10 +2687,10 @@
       </c>
       <c r="C87" s="2"/>
       <c r="D87" s="5">
-        <v>797186574</v>
+        <v>331913782</v>
       </c>
       <c r="E87" s="5">
-        <v>9575</v>
+        <v>35936</v>
       </c>
       <c r="F87" s="5">
         <v>14733</v>
@@ -2711,10 +2711,10 @@
       </c>
       <c r="C88" s="2"/>
       <c r="D88" s="5">
-        <v>956623888</v>
+        <v>398296538</v>
       </c>
       <c r="E88" s="5">
-        <v>10128</v>
+        <v>38011</v>
       </c>
       <c r="F88" s="5">
         <v>17679</v>
@@ -2735,10 +2735,10 @@
       </c>
       <c r="C89" s="2"/>
       <c r="D89" s="5">
-        <v>1147948665</v>
+        <v>477955845</v>
       </c>
       <c r="E89" s="5">
-        <v>10696</v>
+        <v>40145</v>
       </c>
       <c r="F89" s="5">
         <v>21214</v>
@@ -2759,10 +2759,10 @@
       </c>
       <c r="C90" s="2"/>
       <c r="D90" s="5">
-        <v>1377538398</v>
+        <v>573547014</v>
       </c>
       <c r="E90" s="5">
-        <v>11280</v>
+        <v>42336</v>
       </c>
       <c r="F90" s="5">
         <v>25456</v>
@@ -2783,10 +2783,10 @@
       </c>
       <c r="C91" s="2"/>
       <c r="D91" s="5">
-        <v>1653046077</v>
+        <v>688256416</v>
       </c>
       <c r="E91" s="5">
-        <v>11901</v>
+        <v>44665</v>
       </c>
       <c r="F91" s="5">
         <v>30547</v>
@@ -2807,10 +2807,10 @@
       </c>
       <c r="C92" s="2"/>
       <c r="D92" s="5">
-        <v>1983655292</v>
+        <v>825907699</v>
       </c>
       <c r="E92" s="5">
-        <v>12970</v>
+        <v>48679</v>
       </c>
       <c r="F92" s="5">
         <v>36656</v>
@@ -2831,10 +2831,10 @@
       </c>
       <c r="C93" s="2"/>
       <c r="D93" s="5">
-        <v>2380386350</v>
+        <v>991089238</v>
       </c>
       <c r="E93" s="5">
-        <v>13646</v>
+        <v>51216</v>
       </c>
       <c r="F93" s="5">
         <v>43987</v>
@@ -2855,10 +2855,10 @@
       </c>
       <c r="C94" s="2"/>
       <c r="D94" s="5">
-        <v>2856463620</v>
+        <v>1189307085</v>
       </c>
       <c r="E94" s="5">
-        <v>14363</v>
+        <v>53906</v>
       </c>
       <c r="F94" s="5">
         <v>52784</v>
@@ -2879,10 +2879,10 @@
       </c>
       <c r="C95" s="2"/>
       <c r="D95" s="5">
-        <v>3427756344</v>
+        <v>1427168502</v>
       </c>
       <c r="E95" s="5">
-        <v>15098</v>
+        <v>56665</v>
       </c>
       <c r="F95" s="5">
         <v>63340</v>
@@ -2903,10 +2903,10 @@
       </c>
       <c r="C96" s="2"/>
       <c r="D96" s="5">
-        <v>4113307612</v>
+        <v>1712602202</v>
       </c>
       <c r="E96" s="5">
-        <v>15851</v>
+        <v>59493</v>
       </c>
       <c r="F96" s="5">
         <v>76008</v>
@@ -2927,10 +2927,10 @@
       </c>
       <c r="C97" s="2"/>
       <c r="D97" s="5">
-        <v>4935969134</v>
+        <v>2055122642</v>
       </c>
       <c r="E97" s="5">
-        <v>16648</v>
+        <v>62484</v>
       </c>
       <c r="F97" s="5">
         <v>91209</v>
@@ -2951,10 +2951,10 @@
       </c>
       <c r="C98" s="2"/>
       <c r="D98" s="5">
-        <v>5923162960</v>
+        <v>2466147170</v>
       </c>
       <c r="E98" s="5">
-        <v>17465</v>
+        <v>65548</v>
       </c>
       <c r="F98" s="5">
         <v>109450</v>
@@ -2975,10 +2975,10 @@
       </c>
       <c r="C99" s="2"/>
       <c r="D99" s="5">
-        <v>7107795552</v>
+        <v>2959376604</v>
       </c>
       <c r="E99" s="5">
-        <v>18301</v>
+        <v>68685</v>
       </c>
       <c r="F99" s="5">
         <v>131340</v>
@@ -2999,10 +2999,10 @@
       </c>
       <c r="C100" s="2"/>
       <c r="D100" s="5">
-        <v>8529354662</v>
+        <v>3551251924</v>
       </c>
       <c r="E100" s="5">
-        <v>19183</v>
+        <v>71997</v>
       </c>
       <c r="F100" s="5">
         <v>157608</v>
@@ -3023,10 +3023,10 @@
       </c>
       <c r="C101" s="2"/>
       <c r="D101" s="5">
-        <v>10235225594</v>
+        <v>4261502308</v>
       </c>
       <c r="E101" s="5">
-        <v>20087</v>
+        <v>75388</v>
       </c>
       <c r="F101" s="5">
         <v>189129</v>
@@ -3048,10 +3048,10 @@
       </c>
       <c r="C102" s="2"/>
       <c r="D102" s="5">
-        <v>12282270712</v>
+        <v>4900727654</v>
       </c>
       <c r="E102" s="5">
-        <v>33245</v>
+        <v>124774</v>
       </c>
       <c r="F102" s="5">
         <v>226954</v>
@@ -3073,10 +3073,10 @@
       </c>
       <c r="C103" s="2"/>
       <c r="D103" s="5">
-        <v>13510497783</v>
+        <v>5635836802</v>
       </c>
       <c r="E103" s="5">
-        <v>34786</v>
+        <v>130557</v>
       </c>
       <c r="F103" s="5">
         <v>272344</v>
@@ -3098,10 +3098,10 @@
       </c>
       <c r="C104" s="2"/>
       <c r="D104" s="5">
-        <v>14861547561</v>
+        <v>6481212322</v>
       </c>
       <c r="E104" s="5">
-        <v>36362</v>
+        <v>136471</v>
       </c>
       <c r="F104" s="5">
         <v>326812</v>
@@ -3123,10 +3123,10 @@
       </c>
       <c r="C105" s="2"/>
       <c r="D105" s="5">
-        <v>16347702317</v>
+        <v>7453394170</v>
       </c>
       <c r="E105" s="5">
-        <v>37973</v>
+        <v>142516</v>
       </c>
       <c r="F105" s="5">
         <v>392174</v>
@@ -3148,10 +3148,10 @@
       </c>
       <c r="C106" s="2"/>
       <c r="D106" s="5">
-        <v>17982472548</v>
+        <v>8571403295</v>
       </c>
       <c r="E106" s="5">
-        <v>39667</v>
+        <v>148875</v>
       </c>
       <c r="F106" s="5">
         <v>470608</v>
@@ -3173,10 +3173,10 @@
       </c>
       <c r="C107" s="2"/>
       <c r="D107" s="5">
-        <v>19780719802</v>
+        <v>9857113789</v>
       </c>
       <c r="E107" s="5">
-        <v>41398</v>
+        <v>155373</v>
       </c>
       <c r="F107" s="5">
         <v>564729</v>
@@ -3198,10 +3198,10 @@
       </c>
       <c r="C108" s="2"/>
       <c r="D108" s="5">
-        <v>21758791782</v>
+        <v>11335680857</v>
       </c>
       <c r="E108" s="5">
-        <v>43167</v>
+        <v>162009</v>
       </c>
       <c r="F108" s="5">
         <v>677674</v>
@@ -3223,10 +3223,10 @@
       </c>
       <c r="C109" s="2"/>
       <c r="D109" s="5">
-        <v>23934670960</v>
+        <v>13036032985</v>
       </c>
       <c r="E109" s="5">
-        <v>45024</v>
+        <v>168981</v>
       </c>
       <c r="F109" s="5">
         <v>813208</v>
@@ -3248,10 +3248,10 @@
       </c>
       <c r="C110" s="2"/>
       <c r="D110" s="5">
-        <v>26328138056</v>
+        <v>14991437932</v>
       </c>
       <c r="E110" s="5">
-        <v>46921</v>
+        <v>176098</v>
       </c>
       <c r="F110" s="5">
         <v>975849</v>
@@ -3273,10 +3273,10 @@
       </c>
       <c r="C111" s="2"/>
       <c r="D111" s="5">
-        <v>28960951861</v>
+        <v>17240153621</v>
       </c>
       <c r="E111" s="5">
-        <v>48856</v>
+        <v>183363</v>
       </c>
       <c r="F111" s="5">
         <v>1171018</v>
@@ -3298,10 +3298,10 @@
       </c>
       <c r="C112" s="2"/>
       <c r="D112" s="5">
-        <v>31857047047</v>
+        <v>19826176664</v>
       </c>
       <c r="E112" s="5">
-        <v>59368</v>
+        <v>222813</v>
       </c>
       <c r="F112" s="5">
         <v>1405221</v>
@@ -3323,10 +3323,10 @@
       </c>
       <c r="C113" s="2"/>
       <c r="D113" s="5">
-        <v>35679892692</v>
+        <v>22800103163</v>
       </c>
       <c r="E113" s="5">
-        <v>61784</v>
+        <v>231883</v>
       </c>
       <c r="F113" s="5">
         <v>1826787</v>
@@ -3348,10 +3348,10 @@
       </c>
       <c r="C114" s="2"/>
       <c r="D114" s="5">
-        <v>39961479815</v>
+        <v>26220118637</v>
       </c>
       <c r="E114" s="5">
-        <v>64249</v>
+        <v>241134</v>
       </c>
       <c r="F114" s="5">
         <v>2374823</v>
@@ -3373,10 +3373,10 @@
       </c>
       <c r="C115" s="2"/>
       <c r="D115" s="5">
-        <v>44756857392</v>
+        <v>30153136432</v>
       </c>
       <c r="E115" s="5">
-        <v>66831</v>
+        <v>250823</v>
       </c>
       <c r="F115" s="5">
         <v>3087269</v>
@@ -3398,10 +3398,10 @@
       </c>
       <c r="C116" s="2"/>
       <c r="D116" s="5">
-        <v>50127680279</v>
+        <v>34676106896</v>
       </c>
       <c r="E116" s="5">
-        <v>69463</v>
+        <v>260703</v>
       </c>
       <c r="F116" s="5">
         <v>4013449</v>
@@ -3423,10 +3423,10 @@
       </c>
       <c r="C117" s="2"/>
       <c r="D117" s="5">
-        <v>56143001912</v>
+        <v>39877522930</v>
       </c>
       <c r="E117" s="5">
-        <v>72147</v>
+        <v>270774</v>
       </c>
       <c r="F117" s="5">
         <v>5217483</v>
@@ -3448,10 +3448,10 @@
       </c>
       <c r="C118" s="2"/>
       <c r="D118" s="5">
-        <v>62880162141</v>
+        <v>45859151369</v>
       </c>
       <c r="E118" s="5">
-        <v>74953</v>
+        <v>281308</v>
       </c>
       <c r="F118" s="5">
         <v>6782727</v>
@@ -3473,10 +3473,10 @@
       </c>
       <c r="C119" s="2"/>
       <c r="D119" s="5">
-        <v>70425781597</v>
+        <v>52738024074</v>
       </c>
       <c r="E119" s="5">
-        <v>77814</v>
+        <v>292043</v>
       </c>
       <c r="F119" s="5">
         <v>8817545</v>
@@ -3498,10 +3498,10 @@
       </c>
       <c r="C120" s="2"/>
       <c r="D120" s="5">
-        <v>78876875388</v>
+        <v>60648727685</v>
       </c>
       <c r="E120" s="5">
-        <v>80728</v>
+        <v>302979</v>
       </c>
       <c r="F120" s="5">
         <v>11462808</v>
@@ -3523,10 +3523,10 @@
       </c>
       <c r="C121" s="2"/>
       <c r="D121" s="5">
-        <v>88342100434</v>
+        <v>69746036837</v>
       </c>
       <c r="E121" s="5">
-        <v>83772</v>
+        <v>314404</v>
       </c>
       <c r="F121" s="5">
         <v>14901650</v>
@@ -3548,10 +3548,10 @@
       </c>
       <c r="C122" s="2"/>
       <c r="D122" s="5">
-        <v>98943152486</v>
+        <v>80207942362</v>
       </c>
       <c r="E122" s="5">
-        <v>99283</v>
+        <v>372618</v>
       </c>
       <c r="F122" s="5">
         <v>19372145</v>
@@ -3573,10 +3573,10 @@
       </c>
       <c r="C123" s="2"/>
       <c r="D123" s="5">
-        <v>110816330784</v>
+        <v>92239133716</v>
       </c>
       <c r="E123" s="5">
-        <v>155717</v>
+        <v>584421</v>
       </c>
       <c r="F123" s="5">
         <v>25183788</v>
@@ -3598,10 +3598,10 @@
       </c>
       <c r="C124" s="2"/>
       <c r="D124" s="5">
-        <v>124114290478</v>
+        <v>106075003773</v>
       </c>
       <c r="E124" s="5">
-        <v>161415</v>
+        <v>605805</v>
       </c>
       <c r="F124" s="5">
         <v>32738924</v>
@@ -3623,10 +3623,10 @@
       </c>
       <c r="C125" s="2"/>
       <c r="D125" s="5">
-        <v>139008005335</v>
+        <v>121986254338</v>
       </c>
       <c r="E125" s="5">
-        <v>167215</v>
+        <v>627574</v>
       </c>
       <c r="F125" s="5">
         <v>42560601</v>
@@ -3648,10 +3648,10 @@
       </c>
       <c r="C126" s="2"/>
       <c r="D126" s="5">
-        <v>155688965975</v>
+        <v>140284192488</v>
       </c>
       <c r="E126" s="5">
-        <v>173118</v>
+        <v>649726</v>
       </c>
       <c r="F126" s="5">
         <v>55328781</v>
@@ -3673,10 +3673,10 @@
       </c>
       <c r="C127" s="2"/>
       <c r="D127" s="5">
-        <v>174371641892</v>
+        <v>161326821361</v>
       </c>
       <c r="E127" s="5">
-        <v>179270</v>
+        <v>672817</v>
       </c>
       <c r="F127" s="5">
         <v>71927415</v>
@@ -3698,10 +3698,10 @@
       </c>
       <c r="C128" s="2"/>
       <c r="D128" s="5">
-        <v>195296238919</v>
+        <v>185525844565</v>
       </c>
       <c r="E128" s="5">
-        <v>185530</v>
+        <v>696311</v>
       </c>
       <c r="F128" s="5">
         <v>93505639</v>
@@ -3723,10 +3723,10 @@
       </c>
       <c r="C129" s="2"/>
       <c r="D129" s="5">
-        <v>218731787589</v>
+        <v>213354721249</v>
       </c>
       <c r="E129" s="5">
-        <v>191897</v>
+        <v>720209</v>
       </c>
       <c r="F129" s="5">
         <v>121557330</v>
@@ -3748,10 +3748,10 @@
       </c>
       <c r="C130" s="2"/>
       <c r="D130" s="5">
-        <v>244979602099</v>
+        <v>245357929436</v>
       </c>
       <c r="E130" s="5">
-        <v>198528</v>
+        <v>745092</v>
       </c>
       <c r="F130" s="5">
         <v>158024529</v>
@@ -3773,10 +3773,10 @@
       </c>
       <c r="C131" s="2"/>
       <c r="D131" s="5">
-        <v>274377154350</v>
+        <v>282161618851</v>
       </c>
       <c r="E131" s="5">
-        <v>205271</v>
+        <v>770399</v>
       </c>
       <c r="F131" s="5">
         <v>205431887</v>
@@ -3798,10 +3798,10 @@
       </c>
       <c r="C132" s="2"/>
       <c r="D132" s="5">
-        <v>307302412872</v>
+        <v>324485861678</v>
       </c>
       <c r="E132" s="5">
-        <v>238642</v>
+        <v>895644</v>
       </c>
       <c r="F132" s="5">
         <v>267061453</v>
@@ -3823,10 +3823,10 @@
       </c>
       <c r="C133" s="2"/>
       <c r="D133" s="5">
-        <v>344178702416</v>
+        <v>373158740929</v>
       </c>
       <c r="E133" s="5">
-        <v>246664</v>
+        <v>925754</v>
       </c>
       <c r="F133" s="5">
         <v>347179888</v>
@@ -3848,10 +3848,10 @@
       </c>
       <c r="C134" s="2"/>
       <c r="D134" s="5">
-        <v>385480146705</v>
+        <v>429132552068</v>
       </c>
       <c r="E134" s="5">
-        <v>254820</v>
+        <v>956362</v>
       </c>
       <c r="F134" s="5">
         <v>451333854</v>
@@ -3873,10 +3873,10 @@
       </c>
       <c r="C135" s="2"/>
       <c r="D135" s="5">
-        <v>431737764309</v>
+        <v>493502434878</v>
       </c>
       <c r="E135" s="5">
-        <v>263108</v>
+        <v>987467</v>
       </c>
       <c r="F135" s="5">
         <v>586734010</v>
@@ -3898,10 +3898,10 @@
       </c>
       <c r="C136" s="2"/>
       <c r="D136" s="5">
-        <v>483546296026</v>
+        <v>567527800109</v>
       </c>
       <c r="E136" s="5">
-        <v>271721</v>
+        <v>1019794</v>
       </c>
       <c r="F136" s="5">
         <v>762754213</v>
@@ -3923,10 +3923,10 @@
       </c>
       <c r="C137" s="2"/>
       <c r="D137" s="5">
-        <v>541571851549</v>
+        <v>652656970125</v>
       </c>
       <c r="E137" s="5">
-        <v>280473</v>
+        <v>1052642</v>
       </c>
       <c r="F137" s="5">
         <v>991580476</v>
@@ -3948,10 +3948,10 @@
       </c>
       <c r="C138" s="2"/>
       <c r="D138" s="5">
-        <v>606560473734</v>
+        <v>750555515643</v>
       </c>
       <c r="E138" s="5">
-        <v>289364</v>
+        <v>1086010</v>
       </c>
       <c r="F138" s="5">
         <v>1289054618</v>
@@ -3973,10 +3973,10 @@
       </c>
       <c r="C139" s="2"/>
       <c r="D139" s="5">
-        <v>679347730582</v>
+        <v>863138842989</v>
       </c>
       <c r="E139" s="5">
-        <v>298596</v>
+        <v>1120658</v>
       </c>
       <c r="F139" s="5">
         <v>1675771003</v>
@@ -3998,10 +3998,10 @@
       </c>
       <c r="C140" s="2"/>
       <c r="D140" s="5">
-        <v>760869458251</v>
+        <v>992609669437</v>
       </c>
       <c r="E140" s="5">
-        <v>307973</v>
+        <v>1155851</v>
       </c>
       <c r="F140" s="5">
         <v>2178502303</v>
@@ -4023,10 +4023,10 @@
       </c>
       <c r="C141" s="2"/>
       <c r="D141" s="5">
-        <v>852173793241</v>
+        <v>1141501119852</v>
       </c>
       <c r="E141" s="5">
-        <v>317495</v>
+        <v>1191586</v>
       </c>
       <c r="F141" s="5">
         <v>2832052993</v>
@@ -4048,10 +4048,10 @@
       </c>
       <c r="C142" s="2"/>
       <c r="D142" s="5">
-        <v>954434648429</v>
+        <v>1312726287829</v>
       </c>
       <c r="E142" s="5">
-        <v>363748</v>
+        <v>1365178</v>
       </c>
       <c r="F142" s="5">
         <v>3681668890</v>
@@ -4073,10 +4073,10 @@
       </c>
       <c r="C143" s="2"/>
       <c r="D143" s="5">
-        <v>1068966806240</v>
+        <v>1509635231003</v>
       </c>
       <c r="E143" s="5">
-        <v>502073</v>
+        <v>1884324</v>
       </c>
       <c r="F143" s="5">
         <v>4786169557</v>
@@ -4098,10 +4098,10 @@
       </c>
       <c r="C144" s="2"/>
       <c r="D144" s="5">
-        <v>1197242822988</v>
+        <v>1736080515653</v>
       </c>
       <c r="E144" s="5">
-        <v>517223</v>
+        <v>1941182</v>
       </c>
       <c r="F144" s="5">
         <v>6222020424</v>
@@ -4123,10 +4123,10 @@
       </c>
       <c r="C145" s="2"/>
       <c r="D145" s="5">
-        <v>1340911961746</v>
+        <v>1996492593000</v>
       </c>
       <c r="E145" s="5">
-        <v>532927</v>
+        <v>2000123</v>
       </c>
       <c r="F145" s="5">
         <v>8088626551</v>
@@ -4148,10 +4148,10 @@
       </c>
       <c r="C146" s="2"/>
       <c r="D146" s="5">
-        <v>1501821397155</v>
+        <v>2295966481950</v>
       </c>
       <c r="E146" s="5">
-        <v>548867</v>
+        <v>2059945</v>
       </c>
       <c r="F146" s="5">
         <v>10515214516</v>
@@ -4173,10 +4173,10 @@
       </c>
       <c r="C147" s="2"/>
       <c r="D147" s="5">
-        <v>1682039964813</v>
+        <v>2640361454242</v>
       </c>
       <c r="E147" s="5">
-        <v>565041</v>
+        <v>2120650</v>
       </c>
       <c r="F147" s="5">
         <v>13669778870</v>
@@ -4198,10 +4198,10 @@
       </c>
       <c r="C148" s="2"/>
       <c r="D148" s="5">
-        <v>1883884760590</v>
+        <v>3036415672378</v>
       </c>
       <c r="E148" s="5">
-        <v>581795</v>
+        <v>2183526</v>
       </c>
       <c r="F148" s="5">
         <v>17770712531</v>
@@ -4223,10 +4223,10 @@
       </c>
       <c r="C149" s="2"/>
       <c r="D149" s="5">
-        <v>2109950931860</v>
+        <v>3491878023234</v>
       </c>
       <c r="E149" s="5">
-        <v>598793</v>
+        <v>2247322</v>
       </c>
       <c r="F149" s="5">
         <v>23101926290</v>
@@ -4248,10 +4248,10 @@
       </c>
       <c r="C150" s="2"/>
       <c r="D150" s="5">
-        <v>2363145043683</v>
+        <v>4015659726719</v>
       </c>
       <c r="E150" s="5">
-        <v>616036</v>
+        <v>2312035</v>
       </c>
       <c r="F150" s="5">
         <v>30032504177</v>
@@ -4273,10 +4273,10 @@
       </c>
       <c r="C151" s="2"/>
       <c r="D151" s="5">
-        <v>2646722448924</v>
+        <v>4618008685726</v>
       </c>
       <c r="E151" s="5">
-        <v>633883</v>
+        <v>2379017</v>
       </c>
       <c r="F151" s="5">
         <v>39042255430</v>
@@ -4298,10 +4298,10 @@
       </c>
       <c r="C152" s="2"/>
       <c r="D152" s="5">
-        <v>2964329142794</v>
+        <v>5079809554298</v>
       </c>
       <c r="E152" s="5">
-        <v>717183</v>
+        <v>2691650</v>
       </c>
       <c r="F152" s="5">
         <v>50754932059</v>
@@ -4323,10 +4323,10 @@
       </c>
       <c r="C153" s="2"/>
       <c r="D153" s="5">
-        <v>3320048639929</v>
+        <v>5587790509727</v>
       </c>
       <c r="E153" s="5">
-        <v>737375</v>
+        <v>2767434</v>
       </c>
       <c r="F153" s="5">
         <v>65981411676</v>
@@ -4348,10 +4348,10 @@
       </c>
       <c r="C154" s="2"/>
       <c r="D154" s="5">
-        <v>3718454476720</v>
+        <v>6146569560699</v>
       </c>
       <c r="E154" s="5">
-        <v>758260</v>
+        <v>2845818</v>
       </c>
       <c r="F154" s="5">
         <v>85775835178</v>
@@ -4373,10 +4373,10 @@
       </c>
       <c r="C155" s="2"/>
       <c r="D155" s="5">
-        <v>4164669013926</v>
+        <v>6761226516768</v>
       </c>
       <c r="E155" s="5">
-        <v>779437</v>
+        <v>2925295</v>
       </c>
       <c r="F155" s="5">
         <v>111508585731</v>
@@ -4398,10 +4398,10 @@
       </c>
       <c r="C156" s="2"/>
       <c r="D156" s="5">
-        <v>4664429295597</v>
+        <v>7437349168444</v>
       </c>
       <c r="E156" s="5">
-        <v>800905</v>
+        <v>3005868</v>
       </c>
       <c r="F156" s="5">
         <v>144961161450</v>
@@ -4423,10 +4423,10 @@
       </c>
       <c r="C157" s="2"/>
       <c r="D157" s="5">
-        <v>5224160811068</v>
+        <v>8181084085288</v>
       </c>
       <c r="E157" s="5">
-        <v>823095</v>
+        <v>3089146</v>
       </c>
       <c r="F157" s="5">
         <v>188449509885</v>
@@ -4448,10 +4448,10 @@
       </c>
       <c r="C158" s="2"/>
       <c r="D158" s="5">
-        <v>5851060108396</v>
+        <v>8999192493816</v>
       </c>
       <c r="E158" s="5">
-        <v>845587</v>
+        <v>3173563</v>
       </c>
       <c r="F158" s="5">
         <v>244984362850</v>
@@ -4473,10 +4473,10 @@
       </c>
       <c r="C159" s="2"/>
       <c r="D159" s="5">
-        <v>6553187321403</v>
+        <v>9899111743197</v>
       </c>
       <c r="E159" s="5">
-        <v>868383</v>
+        <v>3259116</v>
       </c>
       <c r="F159" s="5">
         <v>318479671705</v>
@@ -4498,10 +4498,10 @@
       </c>
       <c r="C160" s="2"/>
       <c r="D160" s="5">
-        <v>7339569799971</v>
+        <v>10889022917516</v>
       </c>
       <c r="E160" s="5">
-        <v>891929</v>
+        <v>3347488</v>
       </c>
       <c r="F160" s="5">
         <v>414023573216</v>
@@ -4523,10 +4523,10 @@
       </c>
       <c r="C161" s="2"/>
       <c r="D161" s="5">
-        <v>8220318175967</v>
+        <v>11977925209267</v>
       </c>
       <c r="E161" s="5">
-        <v>915790</v>
+        <v>3437039</v>
       </c>
       <c r="F161" s="5">
         <v>538230645180</v>
@@ -4548,10 +4548,10 @@
       </c>
       <c r="C162" s="2"/>
       <c r="D162" s="5">
-        <v>9206756357083</v>
+        <v>13175717730193</v>
       </c>
       <c r="E162" s="5">
-        <v>1697711</v>
+        <v>6371658</v>
       </c>
       <c r="F162" s="5">
         <v>699699838734</v>
@@ -4573,10 +4573,10 @@
       </c>
       <c r="C163" s="2"/>
       <c r="D163" s="5">
-        <v>10311567119933</v>
+        <v>14493289503212</v>
       </c>
       <c r="E163" s="5">
-        <v>1742785</v>
+        <v>6540826</v>
       </c>
       <c r="F163" s="5">
         <v>979579774227</v>
@@ -4598,10 +4598,10 @@
       </c>
       <c r="C164" s="2"/>
       <c r="D164" s="5">
-        <v>11548955174325</v>
+        <v>15942618453533</v>
       </c>
       <c r="E164" s="5">
-        <v>1788450</v>
+        <v>6712207</v>
       </c>
       <c r="F164" s="5">
         <v>1371411683917</v>
@@ -4623,10 +4623,10 @@
       </c>
       <c r="C165" s="2"/>
       <c r="D165" s="5">
-        <v>12934829795244</v>
+        <v>17536880298886</v>
       </c>
       <c r="E165" s="5">
-        <v>1834705</v>
+        <v>6885805</v>
       </c>
       <c r="F165" s="5">
         <v>1919976357483</v>
@@ -4648,10 +4648,10 @@
       </c>
       <c r="C166" s="2"/>
       <c r="D166" s="5">
-        <v>14487009370673</v>
+        <v>19290568328774</v>
       </c>
       <c r="E166" s="5">
-        <v>1882424</v>
+        <v>7064898</v>
       </c>
       <c r="F166" s="5">
         <v>2687966900476</v>
@@ -4673,10 +4673,10 @@
       </c>
       <c r="C167" s="2"/>
       <c r="D167" s="5">
-        <v>16225450495153</v>
+        <v>21219625161651</v>
       </c>
       <c r="E167" s="5">
-        <v>1930755</v>
+        <v>7246290</v>
       </c>
       <c r="F167" s="5">
         <v>3763153660666</v>
@@ -4698,10 +4698,10 @@
       </c>
       <c r="C168" s="2"/>
       <c r="D168" s="5">
-        <v>18172504554571</v>
+        <v>23341587677816</v>
       </c>
       <c r="E168" s="5">
-        <v>1979699</v>
+        <v>7429981</v>
       </c>
       <c r="F168" s="5">
         <v>5268415124932</v>
@@ -4723,10 +4723,10 @@
       </c>
       <c r="C169" s="2"/>
       <c r="D169" s="5">
-        <v>20353205101119</v>
+        <v>25675746445597</v>
       </c>
       <c r="E169" s="5">
-        <v>2030162</v>
+        <v>7619373</v>
       </c>
       <c r="F169" s="5">
         <v>7375781174904</v>
@@ -4748,10 +4748,10 @@
       </c>
       <c r="C170" s="2"/>
       <c r="D170" s="5">
-        <v>22795589713253</v>
+        <v>28243321090156</v>
       </c>
       <c r="E170" s="5">
-        <v>2081260</v>
+        <v>7811148</v>
       </c>
       <c r="F170" s="5">
         <v>10326093644865</v>
@@ -4773,10 +4773,10 @@
       </c>
       <c r="C171" s="2"/>
       <c r="D171" s="5">
-        <v>25531060478843</v>
+        <v>31067653199171</v>
       </c>
       <c r="E171" s="5">
-        <v>2132993</v>
+        <v>8005308</v>
       </c>
       <c r="F171" s="5">
         <v>14456531102811</v>
@@ -4798,10 +4798,10 @@
       </c>
       <c r="C172" s="2"/>
       <c r="D172" s="5">
-        <v>28594787736304</v>
+        <v>34174418519088</v>
       </c>
       <c r="E172" s="5">
-        <v>2368494</v>
+        <v>8889161</v>
       </c>
       <c r="F172" s="5">
         <v>20239143543935</v>
@@ -4823,10 +4823,10 @@
       </c>
       <c r="C173" s="2"/>
       <c r="D173" s="5">
-        <v>32026162264660</v>
+        <v>37591860370996</v>
       </c>
       <c r="E173" s="5">
-        <v>2426958</v>
+        <v>9108581</v>
       </c>
       <c r="F173" s="5">
         <v>28334800961509</v>
@@ -4848,10 +4848,10 @@
       </c>
       <c r="C174" s="2"/>
       <c r="D174" s="5">
-        <v>35869301736419</v>
+        <v>41351046408095</v>
       </c>
       <c r="E174" s="5">
-        <v>2486135</v>
+        <v>9330679</v>
       </c>
       <c r="F174" s="5">
         <v>39668721346112</v>
@@ -4873,10 +4873,10 @@
       </c>
       <c r="C175" s="2"/>
       <c r="D175" s="5">
-        <v>40173617944789</v>
+        <v>45486151048904</v>
       </c>
       <c r="E175" s="5">
-        <v>2547082</v>
+        <v>9559416</v>
       </c>
       <c r="F175" s="5">
         <v>55536209884556</v>
@@ -4898,10 +4898,10 @@
       </c>
       <c r="C176" s="2"/>
       <c r="D176" s="5">
-        <v>44994452098163</v>
+        <v>50034766153794</v>
       </c>
       <c r="E176" s="5">
-        <v>2608766</v>
+        <v>9790924</v>
       </c>
       <c r="F176" s="5">
         <v>77750693838378</v>
@@ -4923,10 +4923,10 @@
       </c>
       <c r="C177" s="2"/>
       <c r="D177" s="5">
-        <v>50393786349942</v>
+        <v>55038242769173</v>
       </c>
       <c r="E177" s="5">
-        <v>2671189</v>
+        <v>10025203</v>
       </c>
       <c r="F177" s="5">
         <v>108850971373729</v>
@@ -4948,10 +4948,10 @@
       </c>
       <c r="C178" s="2"/>
       <c r="D178" s="5">
-        <v>56441040711935</v>
+        <v>60542067046090</v>
       </c>
       <c r="E178" s="5">
-        <v>2735445</v>
+        <v>10266363</v>
       </c>
       <c r="F178" s="5">
         <v>152391359923221</v>
@@ -4973,10 +4973,10 @@
       </c>
       <c r="C179" s="2"/>
       <c r="D179" s="5">
-        <v>63213965597367</v>
+        <v>66596273750699</v>
       </c>
       <c r="E179" s="5">
-        <v>2800465</v>
+        <v>10510387</v>
       </c>
       <c r="F179" s="5">
         <v>213347903892509</v>
@@ -4998,10 +4998,10 @@
       </c>
       <c r="C180" s="2"/>
       <c r="D180" s="5">
-        <v>70799641469051</v>
+        <v>73255901125768</v>
       </c>
       <c r="E180" s="5">
-        <v>2866248</v>
+        <v>10757277</v>
       </c>
       <c r="F180" s="5">
         <v>298687065449513</v>
@@ -5023,10 +5023,10 @@
       </c>
       <c r="C181" s="2"/>
       <c r="D181" s="5">
-        <v>79295598445337</v>
+        <v>80581491238344</v>
       </c>
       <c r="E181" s="5">
-        <v>2933930</v>
+        <v>11011294</v>
       </c>
       <c r="F181" s="5">
         <v>418161891629318</v>
@@ -5048,10 +5048,10 @@
       </c>
       <c r="C182" s="2"/>
       <c r="D182" s="5">
-        <v>88811070258777</v>
+        <v>88639640362178</v>
       </c>
       <c r="E182" s="5">
-        <v>6143375</v>
+        <v>23056617</v>
       </c>
       <c r="F182" s="5">
         <v>585426648281045</v>
@@ -5073,10 +5073,10 @@
       </c>
       <c r="C183" s="2"/>
       <c r="D183" s="5">
-        <v>99468398689830</v>
+        <v>97503604398395</v>
       </c>
       <c r="E183" s="5">
-        <v>6285094</v>
+        <v>23588498</v>
       </c>
       <c r="F183" s="5">
         <v>848868640007515</v>
@@ -5098,10 +5098,10 @@
       </c>
       <c r="C184" s="2"/>
       <c r="D184" s="5">
-        <v>111404606532610</v>
+        <v>107253964838235</v>
       </c>
       <c r="E184" s="5">
-        <v>6430832</v>
+        <v>24135465</v>
       </c>
       <c r="F184" s="5">
         <v>1230859528010896</v>
@@ -5123,10 +5123,10 @@
       </c>
       <c r="C185" s="2"/>
       <c r="D185" s="5">
-        <v>124773159316523</v>
+        <v>117979361322059</v>
       </c>
       <c r="E185" s="5">
-        <v>6578239</v>
+        <v>24688697</v>
       </c>
       <c r="F185" s="5">
         <v>1784746315615799</v>
@@ -5148,10 +5148,10 @@
       </c>
       <c r="C186" s="2"/>
       <c r="D186" s="5">
-        <v>139745938434506</v>
+        <v>129777297454265</v>
       </c>
       <c r="E186" s="5">
-        <v>6727317</v>
+        <v>25248201</v>
       </c>
       <c r="F186" s="5">
         <v>2587882157642908</v>
@@ -5173,10 +5173,10 @@
       </c>
       <c r="C187" s="2"/>
       <c r="D187" s="5">
-        <v>156515451046647</v>
+        <v>142755027199692</v>
       </c>
       <c r="E187" s="5">
-        <v>6880551</v>
+        <v>25823301</v>
       </c>
       <c r="F187" s="5">
         <v>3752429128582216</v>
@@ -5198,10 +5198,10 @@
       </c>
       <c r="C188" s="2"/>
       <c r="D188" s="5">
-        <v>175297305172245</v>
+        <v>157030529919661</v>
       </c>
       <c r="E188" s="5">
-        <v>7035509</v>
+        <v>26404876</v>
       </c>
       <c r="F188" s="5">
         <v>5441022236444213</v>
@@ -5223,10 +5223,10 @@
       </c>
       <c r="C189" s="2"/>
       <c r="D189" s="5">
-        <v>196332981792914</v>
+        <v>172733582911627</v>
       </c>
       <c r="E189" s="5">
-        <v>7192194</v>
+        <v>26992924</v>
       </c>
       <c r="F189" s="5">
         <v>7889482242844109</v>
@@ -5248,10 +5248,10 @@
       </c>
       <c r="C190" s="2"/>
       <c r="D190" s="5">
-        <v>219892939608064</v>
+        <v>190006941202790</v>
       </c>
       <c r="E190" s="5">
-        <v>7353173</v>
+        <v>27597090</v>
       </c>
       <c r="F190" s="5">
         <v>1.1439749252123958E+16</v>
@@ -5273,10 +5273,10 @@
       </c>
       <c r="C191" s="2"/>
       <c r="D191" s="5">
-        <v>246280092361032</v>
+        <v>209007635323069</v>
       </c>
       <c r="E191" s="5">
-        <v>7515933</v>
+        <v>28207947</v>
       </c>
       <c r="F191" s="5">
         <v>1.6587636415579738E+16</v>
@@ -5298,10 +5298,10 @@
       </c>
       <c r="C192" s="2"/>
       <c r="D192" s="5">
-        <v>275833703444356</v>
+        <v>229908398855376</v>
       </c>
       <c r="E192" s="5">
-        <v>8229081</v>
+        <v>30884452</v>
       </c>
       <c r="F192" s="5">
         <v>2.405207280259062E+16</v>
@@ -5323,10 +5323,10 @@
       </c>
       <c r="C193" s="2"/>
       <c r="D193" s="5">
-        <v>308933747857679</v>
+        <v>252899238740914</v>
       </c>
       <c r="E193" s="5">
-        <v>8410129</v>
+        <v>31563935</v>
       </c>
       <c r="F193" s="5">
         <v>3.4875505563756396E+16</v>
@@ -5348,10 +5348,10 @@
       </c>
       <c r="C194" s="2"/>
       <c r="D194" s="5">
-        <v>346005797600601</v>
+        <v>278189162615005</v>
       </c>
       <c r="E194" s="5">
-        <v>8593146</v>
+        <v>32250822</v>
       </c>
       <c r="F194" s="5">
         <v>5.0569483067446776E+16</v>
@@ -5373,10 +5373,10 @@
       </c>
       <c r="C195" s="2"/>
       <c r="D195" s="5">
-        <v>387526493312673</v>
+        <v>306008078876506</v>
       </c>
       <c r="E195" s="5">
-        <v>8778134</v>
+        <v>32945092</v>
       </c>
       <c r="F195" s="5">
         <v>7.3325750447797824E+16</v>
@@ -5398,10 +5398,10 @@
       </c>
       <c r="C196" s="2"/>
       <c r="D196" s="5">
-        <v>434029672510194</v>
+        <v>336608886764157</v>
       </c>
       <c r="E196" s="5">
-        <v>8968029</v>
+        <v>33657782</v>
       </c>
       <c r="F196" s="5">
         <v>1.0632233814930685E+17</v>
@@ -5423,10 +5423,10 @@
       </c>
       <c r="C197" s="2"/>
       <c r="D197" s="5">
-        <v>486113233211417</v>
+        <v>370269775440573</v>
       </c>
       <c r="E197" s="5">
-        <v>9159955</v>
+        <v>34378105</v>
       </c>
       <c r="F197" s="5">
         <v>1.5416739031649491E+17</v>
@@ -5448,10 +5448,10 @@
       </c>
       <c r="C198" s="2"/>
       <c r="D198" s="5">
-        <v>544446821196787</v>
+        <v>407296752984630</v>
       </c>
       <c r="E198" s="5">
-        <v>9353914</v>
+        <v>35106047</v>
       </c>
       <c r="F198" s="5">
         <v>2.235427159589176E+17</v>
@@ -5473,10 +5473,10 @@
       </c>
       <c r="C199" s="2"/>
       <c r="D199" s="5">
-        <v>609780439740402</v>
+        <v>448026428283093</v>
       </c>
       <c r="E199" s="5">
-        <v>9552935</v>
+        <v>35852990</v>
       </c>
       <c r="F199" s="5">
         <v>3.2413693814043053E+17</v>
@@ -5498,10 +5498,10 @@
       </c>
       <c r="C200" s="2"/>
       <c r="D200" s="5">
-        <v>682954092509250</v>
+        <v>492829071111402</v>
       </c>
       <c r="E200" s="5">
-        <v>9754052</v>
+        <v>36607796</v>
       </c>
       <c r="F200" s="5">
         <v>4.6999856030362426E+17</v>
@@ -5523,10 +5523,10 @@
       </c>
       <c r="C201" s="2"/>
       <c r="D201" s="5">
-        <v>764908583610360</v>
+        <v>542111978222542</v>
       </c>
       <c r="E201" s="5">
-        <v>9957263</v>
+        <v>37370468</v>
       </c>
       <c r="F201" s="5">
         <v>6.814979124402551E+17</v>
@@ -5548,10 +5548,10 @@
       </c>
       <c r="C202" s="2"/>
       <c r="D202" s="5">
-        <v>856697613643603</v>
+        <v>596323176044796</v>
       </c>
       <c r="E202" s="5">
-        <v>11562671</v>
+        <v>43395701</v>
       </c>
       <c r="F202" s="5">
         <v>9.5409707741635712E+17</v>
@@ -5573,10 +5573,10 @@
       </c>
       <c r="C203" s="2"/>
       <c r="D203" s="5">
-        <v>959501327280836</v>
+        <v>655955493649276</v>
       </c>
       <c r="E203" s="5">
-        <v>11741664</v>
+        <v>44067476</v>
       </c>
       <c r="F203" s="5">
         <v>1.3357359083829E+18</v>
@@ -5598,10 +5598,10 @@
       </c>
       <c r="C204" s="2"/>
       <c r="D204" s="5">
-        <v>1074641486554536</v>
+        <v>721551043014204</v>
       </c>
       <c r="E204" s="5">
-        <v>11925652</v>
+        <v>44757999</v>
       </c>
       <c r="F204" s="5">
         <v>1.8700302717360599E+18</v>
@@ -5623,10 +5623,10 @@
       </c>
       <c r="C205" s="2"/>
       <c r="D205" s="5">
-        <v>1203598464941080</v>
+        <v>793706147315625</v>
       </c>
       <c r="E205" s="5">
-        <v>12111071</v>
+        <v>45453896</v>
       </c>
       <c r="F205" s="5">
         <v>2.6180423804304835E+18</v>
@@ -5648,10 +5648,10 @@
       </c>
       <c r="C206" s="2"/>
       <c r="D206" s="5">
-        <v>1348030280734009</v>
+        <v>873076762047188</v>
       </c>
       <c r="E206" s="5">
-        <v>12297920</v>
+        <v>46155153</v>
       </c>
       <c r="F206" s="5">
         <v>3.6652593326026767E+18</v>
@@ -5673,10 +5673,10 @@
       </c>
       <c r="C207" s="2"/>
       <c r="D207" s="5">
-        <v>1509793914422090</v>
+        <v>960384438251907</v>
       </c>
       <c r="E207" s="5">
-        <v>12486200</v>
+        <v>46861786</v>
       </c>
       <c r="F207" s="5">
         <v>5.1313630656437473E+18</v>
@@ -5698,10 +5698,10 @@
       </c>
       <c r="C208" s="2"/>
       <c r="D208" s="5">
-        <v>1690969184152741</v>
+        <v>1056422882077097</v>
       </c>
       <c r="E208" s="5">
-        <v>12679643</v>
+        <v>47587792</v>
       </c>
       <c r="F208" s="5">
         <v>7.1839082919012454E+18</v>
@@ -5723,10 +5723,10 @@
       </c>
       <c r="C209" s="2"/>
       <c r="D209" s="5">
-        <v>1893885486251070</v>
+        <v>1162065170284806</v>
       </c>
       <c r="E209" s="5">
-        <v>12874574</v>
+        <v>48319383</v>
       </c>
       <c r="F209" s="5">
         <v>1.0057471608661744E+19</v>
@@ -5748,10 +5748,10 @@
       </c>
       <c r="C210" s="2"/>
       <c r="D210" s="5">
-        <v>2121151744601198</v>
+        <v>1278271687313286</v>
       </c>
       <c r="E210" s="5">
-        <v>13070992</v>
+        <v>49056559</v>
       </c>
       <c r="F210" s="5">
         <v>1.4080460252126439E+19</v>
@@ -5773,10 +5773,10 @@
       </c>
       <c r="C211" s="2"/>
       <c r="D211" s="5">
-        <v>2375689953953342</v>
+        <v>1406098856044614</v>
       </c>
       <c r="E211" s="5">
-        <v>13268897</v>
+        <v>49799312</v>
       </c>
       <c r="F211" s="5">
         <v>1.9712644352977015E+19</v>
@@ -5798,10 +5798,10 @@
       </c>
       <c r="C212" s="2"/>
       <c r="D212" s="5">
-        <v>2660772748427743</v>
+        <v>1546708741649075</v>
       </c>
       <c r="E212" s="5">
-        <v>14045420</v>
+        <v>52713675</v>
       </c>
       <c r="F212" s="5">
         <v>2.7597702094167818E+19</v>
@@ -5823,10 +5823,10 @@
       </c>
       <c r="C213" s="2"/>
       <c r="D213" s="5">
-        <v>2980065478239072</v>
+        <v>1701379615813982</v>
       </c>
       <c r="E213" s="5">
-        <v>14258919</v>
+        <v>53514952</v>
       </c>
       <c r="F213" s="5">
         <v>3.8636782931834946E+19</v>
@@ -5848,10 +5848,10 @@
       </c>
       <c r="C214" s="2"/>
       <c r="D214" s="5">
-        <v>3337673335627761</v>
+        <v>1871517577395380</v>
       </c>
       <c r="E214" s="5">
-        <v>14474029</v>
+        <v>54322281</v>
       </c>
       <c r="F214" s="5">
         <v>5.4091496104568922E+19</v>
@@ -5873,10 +5873,10 @@
       </c>
       <c r="C215" s="2"/>
       <c r="D215" s="5">
-        <v>3738194135903092</v>
+        <v>2058669335134918</v>
       </c>
       <c r="E215" s="5">
-        <v>14690749</v>
+        <v>55135645</v>
       </c>
       <c r="F215" s="5">
         <v>7.5728094546396479E+19</v>
@@ -5898,10 +5898,10 @@
       </c>
       <c r="C216" s="2"/>
       <c r="D216" s="5">
-        <v>4186777432211463</v>
+        <v>2264536268648410</v>
       </c>
       <c r="E216" s="5">
-        <v>14913215</v>
+        <v>55970584</v>
       </c>
       <c r="F216" s="5">
         <v>1.0601933236495506E+20</v>
@@ -5923,10 +5923,10 @@
       </c>
       <c r="C217" s="2"/>
       <c r="D217" s="5">
-        <v>4689190724076839</v>
+        <v>2490989895513251</v>
       </c>
       <c r="E217" s="5">
-        <v>15137352</v>
+        <v>56811789</v>
       </c>
       <c r="F217" s="5">
         <v>1.4842706531093709E+20</v>
@@ -5948,10 +5948,10 @@
       </c>
       <c r="C218" s="2"/>
       <c r="D218" s="5">
-        <v>5251893610966060</v>
+        <v>2740088885064576</v>
       </c>
       <c r="E218" s="5">
-        <v>15363161</v>
+        <v>57659270</v>
       </c>
       <c r="F218" s="5">
         <v>2.0779789143531192E+20</v>
@@ -5973,10 +5973,10 @@
       </c>
       <c r="C219" s="2"/>
       <c r="D219" s="5">
-        <v>5882120844281988</v>
+        <v>3014097773571034</v>
       </c>
       <c r="E219" s="5">
-        <v>15590642</v>
+        <v>58513025</v>
       </c>
       <c r="F219" s="5">
         <v>2.9091704800943666E+20</v>
@@ -5998,10 +5998,10 @@
       </c>
       <c r="C220" s="2"/>
       <c r="D220" s="5">
-        <v>6587975345595827</v>
+        <v>3315507550928137</v>
       </c>
       <c r="E220" s="5">
-        <v>15824054</v>
+        <v>59389044</v>
       </c>
       <c r="F220" s="5">
         <v>4.072838672132113E+20</v>
@@ -6023,10 +6023,10 @@
       </c>
       <c r="C221" s="2"/>
       <c r="D221" s="5">
-        <v>7378532387067327</v>
+        <v>3647058306020951</v>
       </c>
       <c r="E221" s="5">
-        <v>16059200</v>
+        <v>60271564</v>
       </c>
       <c r="F221" s="5">
         <v>5.701974140984958E+20</v>
@@ -6048,10 +6048,10 @@
       </c>
       <c r="C222" s="2"/>
       <c r="D222" s="5">
-        <v>8263956273515407</v>
+        <v>4011764136623046</v>
       </c>
       <c r="E222" s="5">
-        <v>16961227</v>
+        <v>63656951</v>
       </c>
       <c r="F222" s="5">
         <v>7.9827637973789403E+20</v>
@@ -6073,10 +6073,10 @@
       </c>
       <c r="C223" s="2"/>
       <c r="D223" s="5">
-        <v>9255631026337256</v>
+        <v>4412940550285351</v>
       </c>
       <c r="E223" s="5">
-        <v>17209581</v>
+        <v>64589041</v>
       </c>
       <c r="F223" s="5">
         <v>1.1175869316330515E+21</v>
@@ -6098,10 +6098,10 @@
       </c>
       <c r="C224" s="2"/>
       <c r="D224" s="5">
-        <v>1.0366306749497728E+16</v>
+        <v>4854234605313886</v>
       </c>
       <c r="E224" s="5">
-        <v>17464305</v>
+        <v>65545046</v>
       </c>
       <c r="F224" s="5">
         <v>1.564621704286272E+21</v>
@@ -6123,10 +6123,10 @@
       </c>
       <c r="C225" s="2"/>
       <c r="D225" s="5">
-        <v>1.1610263559437456E+16</v>
+        <v>5339658065845275</v>
       </c>
       <c r="E225" s="5">
-        <v>17720900</v>
+        <v>66508063</v>
       </c>
       <c r="F225" s="5">
         <v>2.1904703860007806E+21</v>
@@ -6148,10 +6148,10 @@
       </c>
       <c r="C226" s="2"/>
       <c r="D226" s="5">
-        <v>1.3003495186569952E+16</v>
+        <v>5873623872429803</v>
       </c>
       <c r="E226" s="5">
-        <v>17979367</v>
+        <v>67478117</v>
       </c>
       <c r="F226" s="5">
         <v>3.0666585404010927E+21</v>
@@ -6173,10 +6173,10 @@
       </c>
       <c r="C227" s="2"/>
       <c r="D227" s="5">
-        <v>1.4563914608958348E+16</v>
+        <v>6460986259672784</v>
       </c>
       <c r="E227" s="5">
-        <v>18239705</v>
+        <v>68455183</v>
       </c>
       <c r="F227" s="5">
         <v>4.2933219565615296E+21</v>
@@ -6198,10 +6198,10 @@
       </c>
       <c r="C228" s="2"/>
       <c r="D228" s="5">
-        <v>1.6311584362033352E+16</v>
+        <v>7107084885640063</v>
       </c>
       <c r="E228" s="5">
-        <v>18506613</v>
+        <v>69456914</v>
       </c>
       <c r="F228" s="5">
         <v>6.0106507391861407E+21</v>
@@ -6223,10 +6223,10 @@
       </c>
       <c r="C229" s="2"/>
       <c r="D229" s="5">
-        <v>1.8268974485477356E+16</v>
+        <v>7817793374204070</v>
       </c>
       <c r="E229" s="5">
-        <v>18775460</v>
+        <v>70465923</v>
       </c>
       <c r="F229" s="5">
         <v>8.4149110348605964E+21</v>
@@ -6248,10 +6248,10 @@
       </c>
       <c r="C230" s="2"/>
       <c r="D230" s="5">
-        <v>2.046125142373464E+16</v>
+        <v>8599572711624478</v>
       </c>
       <c r="E230" s="5">
-        <v>19046246</v>
+        <v>71482208</v>
       </c>
       <c r="F230" s="5">
         <v>1.1780875448804834E+22</v>
@@ -6273,10 +6273,10 @@
       </c>
       <c r="C231" s="2"/>
       <c r="D231" s="5">
-        <v>2.29166015945828E+16</v>
+        <v>9459529982786926</v>
       </c>
       <c r="E231" s="5">
-        <v>19318970</v>
+        <v>72505761</v>
       </c>
       <c r="F231" s="5">
         <v>1.6493225628326766E+22</v>
@@ -6298,10 +6298,10 @@
       </c>
       <c r="C232" s="2"/>
       <c r="D232" s="5">
-        <v>2.566659378593274E+16</v>
+        <v>1.040548298106562E+16</v>
       </c>
       <c r="E232" s="5">
-        <v>20367037</v>
+        <v>76439246</v>
       </c>
       <c r="F232" s="5">
         <v>2.3090515879657472E+22</v>
@@ -6323,10 +6323,10 @@
       </c>
       <c r="C233" s="2"/>
       <c r="D233" s="5">
-        <v>2.8746585040244672E+16</v>
+        <v>1.1446031279172182E+16</v>
       </c>
       <c r="E233" s="5">
-        <v>20659583</v>
+        <v>77537199</v>
       </c>
       <c r="F233" s="5">
         <v>3.2326722231520461E+22</v>
@@ -6348,10 +6348,10 @@
       </c>
       <c r="C234" s="2"/>
       <c r="D234" s="5">
-        <v>3.2196175245074036E+16</v>
+        <v>1.2590634407089402E+16</v>
       </c>
       <c r="E234" s="5">
-        <v>20954214</v>
+        <v>78642975</v>
       </c>
       <c r="F234" s="5">
         <v>4.5257411124128645E+22</v>
@@ -6373,10 +6373,10 @@
       </c>
       <c r="C235" s="2"/>
       <c r="D235" s="5">
-        <v>3.605971627448292E+16</v>
+        <v>1.3849697847798344E+16</v>
       </c>
       <c r="E235" s="5">
-        <v>21250932</v>
+        <v>79756582</v>
       </c>
       <c r="F235" s="5">
         <v>6.3360375573780103E+22</v>
@@ -6398,10 +6398,10 @@
       </c>
       <c r="C236" s="2"/>
       <c r="D236" s="5">
-        <v>4.0386882227420872E+16</v>
+        <v>1.523466763257818E+16</v>
       </c>
       <c r="E236" s="5">
-        <v>21554906</v>
+        <v>80897421</v>
       </c>
       <c r="F236" s="5">
         <v>8.8704525803292144E+22</v>
@@ -6423,10 +6423,10 @@
       </c>
       <c r="C237" s="2"/>
       <c r="D237" s="5">
-        <v>4.5233308094711384E+16</v>
+        <v>1.6758134395836E+16</v>
       </c>
       <c r="E237" s="5">
-        <v>21861039</v>
+        <v>82046364</v>
       </c>
       <c r="F237" s="5">
         <v>1.24186336124609E+23</v>
@@ -6448,10 +6448,10 @@
       </c>
       <c r="C238" s="2"/>
       <c r="D238" s="5">
-        <v>5.0661305066076752E+16</v>
+        <v>1.84339478354196E+16</v>
       </c>
       <c r="E238" s="5">
-        <v>22169330</v>
+        <v>83203410</v>
       </c>
       <c r="F238" s="5">
         <v>1.738608705744526E+23</v>
@@ -6473,10 +6473,10 @@
       </c>
       <c r="C239" s="2"/>
       <c r="D239" s="5">
-        <v>5.6740661674005968E+16</v>
+        <v>2.027734261896156E+16</v>
       </c>
       <c r="E239" s="5">
-        <v>22479779</v>
+        <v>84368552</v>
       </c>
       <c r="F239" s="5">
         <v>2.4340521880423363E+23</v>
@@ -6498,10 +6498,10 @@
       </c>
       <c r="C240" s="2"/>
       <c r="D240" s="5">
-        <v>6.3549541074886688E+16</v>
+        <v>2.2305076880857716E+16</v>
       </c>
       <c r="E240" s="5">
-        <v>22797705</v>
+        <v>85561753</v>
       </c>
       <c r="F240" s="5">
         <v>3.4076730632592704E+23</v>
@@ -6523,10 +6523,10 @@
       </c>
       <c r="C241" s="2"/>
       <c r="D241" s="5">
-        <v>7.1175486003873096E+16</v>
+        <v>2.4535584568943488E+16</v>
       </c>
       <c r="E241" s="5">
-        <v>23117862</v>
+        <v>86763332</v>
       </c>
       <c r="F241" s="5">
         <v>4.7707422885629783E+23</v>
@@ -6548,10 +6548,10 @@
       </c>
       <c r="C242" s="2"/>
       <c r="D242" s="5">
-        <v>7.9716544324337872E+16</v>
+        <v>2.698914302583784E+16</v>
       </c>
       <c r="E242" s="5">
-        <v>24324790</v>
+        <v>91293036</v>
       </c>
       <c r="F242" s="5">
         <v>6.6790392039881687E+23</v>
@@ -6573,10 +6573,10 @@
       </c>
       <c r="C243" s="2"/>
       <c r="D243" s="5">
-        <v>8.9282529643258432E+16</v>
+        <v>2.9688057328421628E+16</v>
       </c>
       <c r="E243" s="5">
-        <v>24661662</v>
+        <v>92557347</v>
       </c>
       <c r="F243" s="5">
         <v>9.3506548855834351E+23</v>
@@ -6598,10 +6598,10 @@
       </c>
       <c r="C244" s="2"/>
       <c r="D244" s="5">
-        <v>9.9996433200449456E+16</v>
+        <v>3.2656863061263792E+16</v>
       </c>
       <c r="E244" s="5">
-        <v>25006524</v>
+        <v>93851644</v>
       </c>
       <c r="F244" s="5">
         <v>1.3090916839816807E+24</v>
@@ -6623,10 +6623,10 @@
       </c>
       <c r="C245" s="2"/>
       <c r="D245" s="5">
-        <v>1.1199600518450341E+17</v>
+        <v>3.5922549367390176E+16</v>
       </c>
       <c r="E245" s="5">
-        <v>25353780</v>
+        <v>95154922</v>
       </c>
       <c r="F245" s="5">
         <v>1.832728357574353E+24</v>
@@ -6648,10 +6648,10 @@
       </c>
       <c r="C246" s="2"/>
       <c r="D246" s="5">
-        <v>1.2543552580664382E+17</v>
+        <v>3.95148043041292E+16</v>
       </c>
       <c r="E246" s="5">
-        <v>25703431</v>
+        <v>96467192</v>
       </c>
       <c r="F246" s="5">
         <v>2.5658197006040939E+24</v>
@@ -6673,10 +6673,10 @@
       </c>
       <c r="C247" s="2"/>
       <c r="D247" s="5">
-        <v>1.404877889034411E+17</v>
+        <v>4.346628473454212E+16</v>
       </c>
       <c r="E247" s="5">
-        <v>26055476</v>
+        <v>97788453</v>
       </c>
       <c r="F247" s="5">
         <v>3.5921475808457311E+24</v>
@@ -6698,10 +6698,10 @@
       </c>
       <c r="C248" s="2"/>
       <c r="D248" s="5">
-        <v>1.5734632357185405E+17</v>
+        <v>4.7812913207996336E+16</v>
       </c>
       <c r="E248" s="5">
-        <v>26415746</v>
+        <v>99140575</v>
       </c>
       <c r="F248" s="5">
         <v>5.0290066131840228E+24</v>
@@ -6723,10 +6723,10 @@
       </c>
       <c r="C249" s="2"/>
       <c r="D249" s="5">
-        <v>1.7622788240047654E+17</v>
+        <v>5.2594204528795976E+16</v>
       </c>
       <c r="E249" s="5">
-        <v>26778489</v>
+        <v>100501978</v>
       </c>
       <c r="F249" s="5">
         <v>7.0406092584576311E+24</v>
@@ -6748,10 +6748,10 @@
       </c>
       <c r="C250" s="2"/>
       <c r="D250" s="5">
-        <v>1.9737522828853376E+17</v>
+        <v>5.7853624981675576E+16</v>
       </c>
       <c r="E250" s="5">
-        <v>27143706</v>
+        <v>101872672</v>
       </c>
       <c r="F250" s="5">
         <v>9.8568529618406831E+24</v>
@@ -6773,10 +6773,10 @@
       </c>
       <c r="C251" s="2"/>
       <c r="D251" s="5">
-        <v>2.2106025568315782E+17</v>
+        <v>6.3638987479843136E+16</v>
       </c>
       <c r="E251" s="5">
-        <v>27511397</v>
+        <v>103252647</v>
       </c>
       <c r="F251" s="5">
         <v>1.3799594146576956E+25</v>
@@ -6798,10 +6798,10 @@
       </c>
       <c r="C252" s="2"/>
       <c r="D252" s="5">
-        <v>2.475874863651368E+17</v>
+        <v>7.0002886227827456E+16</v>
       </c>
       <c r="E252" s="5">
-        <v>36404957</v>
+        <v>136630950</v>
       </c>
       <c r="F252" s="5">
         <v>2.0009411512536584E+25</v>
@@ -6823,10 +6823,10 @@
       </c>
       <c r="C253" s="2"/>
       <c r="D253" s="5">
-        <v>2.7729798472895325E+17</v>
+        <v>7.7003174850610208E+16</v>
       </c>
       <c r="E253" s="5">
-        <v>36899331</v>
+        <v>138486370</v>
       </c>
       <c r="F253" s="5">
         <v>2.9013646693178048E+25</v>
@@ -6848,10 +6848,10 @@
       </c>
       <c r="C254" s="2"/>
       <c r="D254" s="5">
-        <v>3.1057374289642765E+17</v>
+        <v>8.4703492335671232E+16</v>
       </c>
       <c r="E254" s="5">
-        <v>37397039</v>
+        <v>140354312</v>
       </c>
       <c r="F254" s="5">
         <v>4.206978770510817E+25</v>
@@ -6873,10 +6873,10 @@
       </c>
       <c r="C255" s="2"/>
       <c r="D255" s="5">
-        <v>3.4784259204399898E+17</v>
+        <v>9.3173841569238368E+16</v>
       </c>
       <c r="E255" s="5">
-        <v>37898082</v>
+        <v>142234776</v>
       </c>
       <c r="F255" s="5">
         <v>6.1001192172406847E+25</v>
@@ -6898,10 +6898,10 @@
       </c>
       <c r="C256" s="2"/>
       <c r="D256" s="5">
-        <v>3.8958370308927891E+17</v>
+        <v>1.0249122572616221E+17</v>
       </c>
       <c r="E256" s="5">
-        <v>38410491</v>
+        <v>144157892</v>
       </c>
       <c r="F256" s="5">
         <v>8.8451728649989929E+25</v>
@@ -6923,10 +6923,10 @@
       </c>
       <c r="C257" s="2"/>
       <c r="D257" s="5">
-        <v>4.3633374745999245E+17</v>
+        <v>1.1274034829877843E+17</v>
       </c>
       <c r="E257" s="5">
-        <v>38926341</v>
+        <v>146093915</v>
       </c>
       <c r="F257" s="5">
         <v>1.282550065424854E+26</v>
@@ -6948,10 +6948,10 @@
       </c>
       <c r="C258" s="2"/>
       <c r="D258" s="5">
-        <v>4.8869379715519162E+17</v>
+        <v>1.2401438312865629E+17</v>
       </c>
       <c r="E258" s="5">
-        <v>39445632</v>
+        <v>148042858</v>
       </c>
       <c r="F258" s="5">
         <v>1.8596975948660382E+26</v>
@@ -6973,10 +6973,10 @@
       </c>
       <c r="C259" s="2"/>
       <c r="D259" s="5">
-        <v>5.4733705281381466E+17</v>
+        <v>1.3641582144152192E+17</v>
       </c>
       <c r="E259" s="5">
-        <v>39968364</v>
+        <v>150004720</v>
       </c>
       <c r="F259" s="5">
         <v>2.6965615125557555E+26</v>
@@ -6998,10 +6998,10 @@
       </c>
       <c r="C260" s="2"/>
       <c r="D260" s="5">
-        <v>6.1301749915147251E+17</v>
+        <v>1.5005740358567411E+17</v>
       </c>
       <c r="E260" s="5">
-        <v>40502786</v>
+        <v>152010456</v>
       </c>
       <c r="F260" s="5">
         <v>3.9100141932058453E+26</v>
@@ -7023,10 +7023,10 @@
       </c>
       <c r="C261" s="2"/>
       <c r="D261" s="5">
-        <v>6.8657959904964928E+17</v>
+        <v>1.6506314394424154E+17</v>
       </c>
       <c r="E261" s="5">
-        <v>41040756</v>
+        <v>154029500</v>
       </c>
       <c r="F261" s="5">
         <v>5.6695205801484756E+26</v>
@@ -7048,10 +7048,10 @@
       </c>
       <c r="C262" s="2"/>
       <c r="D262" s="5">
-        <v>7.689691509356073E+17</v>
+        <v>1.815694583386657E+17</v>
       </c>
       <c r="E262" s="5">
-        <v>43041303</v>
+        <v>161537731</v>
       </c>
       <c r="F262" s="5">
         <v>8.2208048412152888E+26</v>
@@ -7073,10 +7073,10 @@
       </c>
       <c r="C263" s="2"/>
       <c r="D263" s="5">
-        <v>8.6124544904788019E+17</v>
+        <v>1.9972640417253229E+17</v>
       </c>
       <c r="E263" s="5">
-        <v>43605497</v>
+        <v>163655194</v>
       </c>
       <c r="F263" s="5">
         <v>1.1920167019762168E+27</v>
@@ -7098,10 +7098,10 @@
       </c>
       <c r="C264" s="2"/>
       <c r="D264" s="5">
-        <v>9.6459490293362586E+17</v>
+        <v>2.1969904458978554E+17</v>
       </c>
       <c r="E264" s="5">
-        <v>44182130</v>
+        <v>165819345</v>
       </c>
       <c r="F264" s="5">
         <v>1.7284242178655144E+27</v>
@@ -7123,10 +7123,10 @@
       </c>
       <c r="C265" s="2"/>
       <c r="D265" s="5">
-        <v>1.0803462912856611E+18</v>
+        <v>2.416689490487641E+17</v>
       </c>
       <c r="E265" s="5">
-        <v>44762550</v>
+        <v>167997714</v>
       </c>
       <c r="F265" s="5">
         <v>2.5062151159049959E+27</v>
@@ -7148,10 +7148,10 @@
       </c>
       <c r="C266" s="2"/>
       <c r="D266" s="5">
-        <v>1.2099878462399406E+18</v>
+        <v>2.6583584395364051E+17</v>
       </c>
       <c r="E266" s="5">
-        <v>45346758</v>
+        <v>170190303</v>
       </c>
       <c r="F266" s="5">
         <v>3.634011918062244E+27</v>
@@ -7173,10 +7173,10 @@
       </c>
       <c r="C267" s="2"/>
       <c r="D267" s="5">
-        <v>1.3551863877887337E+18</v>
+        <v>2.9241942834900461E+17</v>
       </c>
       <c r="E267" s="5">
-        <v>45934754</v>
+        <v>172397097</v>
       </c>
       <c r="F267" s="5">
         <v>5.2693172811902539E+27</v>
@@ -7198,10 +7198,10 @@
       </c>
       <c r="C268" s="2"/>
       <c r="D268" s="5">
-        <v>1.5178087543233818E+18</v>
+        <v>3.2166137118390509E+17</v>
       </c>
       <c r="E268" s="5">
-        <v>46535533</v>
+        <v>174651866</v>
       </c>
       <c r="F268" s="5">
         <v>7.640510057725868E+27</v>
@@ -7223,10 +7223,10 @@
       </c>
       <c r="C269" s="2"/>
       <c r="D269" s="5">
-        <v>1.6999458048421878E+18</v>
+        <v>3.5382750830229562E+17</v>
       </c>
       <c r="E269" s="5">
-        <v>47140215</v>
+        <v>176921300</v>
       </c>
       <c r="F269" s="5">
         <v>1.1078739583702508E+28</v>
@@ -7248,10 +7248,10 @@
       </c>
       <c r="C270" s="2"/>
       <c r="D270" s="5">
-        <v>1.9039393014232504E+18</v>
+        <v>3.8921025913252518E+17</v>
       </c>
       <c r="E270" s="5">
-        <v>47748800</v>
+        <v>179205375</v>
       </c>
       <c r="F270" s="5">
         <v>1.6064172396368638E+28</v>
@@ -7273,10 +7273,10 @@
       </c>
       <c r="C271" s="2"/>
       <c r="D271" s="5">
-        <v>2.1324120175940406E+18</v>
+        <v>4.2813128504577773E+17</v>
       </c>
       <c r="E271" s="5">
-        <v>48361289</v>
+        <v>181504090</v>
       </c>
       <c r="F271" s="5">
         <v>2.3293049974734522E+28</v>
@@ -7298,10 +7298,10 @@
       </c>
       <c r="C272" s="2"/>
       <c r="D272" s="5">
-        <v>2.3883014597053256E+18</v>
+        <v>4.7094441355035552E+17</v>
       </c>
       <c r="E272" s="5">
-        <v>50647483</v>
+        <v>190084376</v>
       </c>
       <c r="F272" s="5">
         <v>3.3774922463365056E+28</v>
@@ -7323,10 +7323,10 @@
       </c>
       <c r="C273" s="2"/>
       <c r="D273" s="5">
-        <v>2.6748976348699648E+18</v>
+        <v>5.180388549053911E+17</v>
       </c>
       <c r="E273" s="5">
-        <v>51298469</v>
+        <v>192527583</v>
       </c>
       <c r="F273" s="5">
         <v>4.8973637571879329E+28</v>
@@ -7348,10 +7348,10 @@
       </c>
       <c r="C274" s="2"/>
       <c r="D274" s="5">
-        <v>2.9958853510543611E+18</v>
+        <v>5.6984274039593024E+17</v>
       </c>
       <c r="E274" s="5">
-        <v>51953611</v>
+        <v>194986394</v>
       </c>
       <c r="F274" s="5">
         <v>7.1011774479225024E+28</v>
@@ -7373,10 +7373,10 @@
       </c>
       <c r="C275" s="2"/>
       <c r="D275" s="5">
-        <v>3.355391593180885E+18</v>
+        <v>6.2682701443552333E+17</v>
       </c>
       <c r="E275" s="5">
-        <v>52612911</v>
+        <v>197460793</v>
       </c>
       <c r="F275" s="5">
         <v>1.0296707299487628E+29</v>
@@ -7398,10 +7398,10 @@
       </c>
       <c r="C276" s="2"/>
       <c r="D276" s="5">
-        <v>3.7580385843625917E+18</v>
+        <v>6.8950971587907571E+17</v>
       </c>
       <c r="E276" s="5">
-        <v>53286155</v>
+        <v>199987537</v>
       </c>
       <c r="F276" s="5">
         <v>1.493022558425706E+29</v>
@@ -7423,10 +7423,10 @@
       </c>
       <c r="C277" s="2"/>
       <c r="D277" s="5">
-        <v>4.209003214486103E+18</v>
+        <v>7.584606874669833E+17</v>
       </c>
       <c r="E277" s="5">
-        <v>53963679</v>
+        <v>202530340</v>
       </c>
       <c r="F277" s="5">
         <v>2.1648827097172737E+29</v>
@@ -7448,10 +7448,10 @@
       </c>
       <c r="C278" s="2"/>
       <c r="D278" s="5">
-        <v>4.7140836002244362E+18</v>
+        <v>8.3430675621368166E+17</v>
       </c>
       <c r="E278" s="5">
-        <v>54645483</v>
+        <v>205089215</v>
       </c>
       <c r="F278" s="5">
         <v>3.1390799290900469E+29</v>
@@ -7473,10 +7473,10 @@
       </c>
       <c r="C279" s="2"/>
       <c r="D279" s="5">
-        <v>5.2797736322513695E+18</v>
+        <v>9.1773743183504986E+17</v>
       </c>
       <c r="E279" s="5">
-        <v>55331568</v>
+        <v>207664150</v>
       </c>
       <c r="F279" s="5">
         <v>4.5516658971805678E+29</v>
@@ -7498,10 +7498,10 @@
       </c>
       <c r="C280" s="2"/>
       <c r="D280" s="5">
-        <v>5.9133464681215345E+18</v>
+        <v>1.0095111750185549E+18</v>
       </c>
       <c r="E280" s="5">
-        <v>56031969</v>
+        <v>210292816</v>
       </c>
       <c r="F280" s="5">
         <v>6.5999155509118237E+29</v>
@@ -7523,10 +7523,10 @@
       </c>
       <c r="C281" s="2"/>
       <c r="D281" s="5">
-        <v>6.6229480442961193E+18</v>
+        <v>1.1104622925204105E+18</v>
       </c>
       <c r="E281" s="5">
-        <v>56736775</v>
+        <v>212938014</v>
       </c>
       <c r="F281" s="5">
         <v>9.5698775488221441E+29</v>
@@ -7548,10 +7548,10 @@
       </c>
       <c r="C282" s="2"/>
       <c r="D282" s="5">
-        <v>7.4177018096116541E+18</v>
+        <v>1.2215085217724516E+18</v>
       </c>
       <c r="E282" s="5">
-        <v>59329461</v>
+        <v>222668590</v>
       </c>
       <c r="F282" s="5">
         <v>1.387632244579211E+30</v>
@@ -7573,10 +7573,10 @@
       </c>
       <c r="C283" s="2"/>
       <c r="D283" s="5">
-        <v>8.3078260267650529E+18</v>
+        <v>1.3436593739496968E+18</v>
       </c>
       <c r="E283" s="5">
-        <v>60066475</v>
+        <v>225434665</v>
       </c>
       <c r="F283" s="5">
         <v>2.0120667546398558E+30</v>
@@ -7598,10 +7598,10 @@
       </c>
       <c r="C284" s="2"/>
       <c r="D284" s="5">
-        <v>9.3047651499768607E+18</v>
+        <v>1.4780253113446666E+18</v>
       </c>
       <c r="E284" s="5">
-        <v>60818664</v>
+        <v>228257692</v>
       </c>
       <c r="F284" s="5">
         <v>2.9174967942277906E+30</v>
@@ -7623,10 +7623,10 @@
       </c>
       <c r="C285" s="2"/>
       <c r="D285" s="5">
-        <v>1.0421336967974085E+19</v>
+        <v>1.6258278424791334E+18</v>
       </c>
       <c r="E285" s="5">
-        <v>61575535</v>
+        <v>231098299</v>
       </c>
       <c r="F285" s="5">
         <v>4.2303703516302961E+30</v>
@@ -7648,10 +7648,10 @@
       </c>
       <c r="C286" s="2"/>
       <c r="D286" s="5">
-        <v>1.1671897404130976E+19</v>
+        <v>1.7884106267270469E+18</v>
       </c>
       <c r="E286" s="5">
-        <v>62337085</v>
+        <v>233956460</v>
       </c>
       <c r="F286" s="5">
         <v>6.1340370098639291E+30</v>
@@ -7673,10 +7673,10 @@
       </c>
       <c r="C287" s="2"/>
       <c r="D287" s="5">
-        <v>1.3072525092626694E+19</v>
+        <v>1.9672516893997517E+18</v>
       </c>
       <c r="E287" s="5">
-        <v>63103316</v>
+        <v>236832187</v>
       </c>
       <c r="F287" s="5">
         <v>8.8943536643026963E+30</v>
@@ -7698,10 +7698,10 @@
       </c>
       <c r="C288" s="2"/>
       <c r="D288" s="5">
-        <v>1.4641228103741899E+19</v>
+        <v>2.1639768583397271E+18</v>
       </c>
       <c r="E288" s="5">
-        <v>63885118</v>
+        <v>239766363</v>
       </c>
       <c r="F288" s="5">
         <v>1.2896812813238908E+31</v>
@@ -7723,10 +7723,10 @@
       </c>
       <c r="C289" s="2"/>
       <c r="D289" s="5">
-        <v>1.6398175476190929E+19</v>
+        <v>2.3803745441737001E+18</v>
       </c>
       <c r="E289" s="5">
-        <v>64671734</v>
+        <v>242718601</v>
       </c>
       <c r="F289" s="5">
         <v>1.8700378579196416E+31</v>
@@ -7748,10 +7748,10 @@
       </c>
       <c r="C290" s="2"/>
       <c r="D290" s="5">
-        <v>1.8365956533333842E+19</v>
+        <v>2.6184119985910702E+18</v>
       </c>
       <c r="E290" s="5">
-        <v>65463163</v>
+        <v>245688903</v>
       </c>
       <c r="F290" s="5">
         <v>2.7115548939834801E+31</v>
@@ -7773,10 +7773,10 @@
       </c>
       <c r="C291" s="2"/>
       <c r="D291" s="5">
-        <v>2.0569871317333905E+19</v>
+        <v>2.8802531984501775E+18</v>
       </c>
       <c r="E291" s="5">
-        <v>66259405</v>
+        <v>248677267</v>
       </c>
       <c r="F291" s="5">
         <v>3.931754596276046E+31</v>
@@ -7798,10 +7798,10 @@
       </c>
       <c r="C292" s="2"/>
       <c r="D292" s="5">
-        <v>2.3038255875413975E+19</v>
+        <v>3.1682785182951956E+18</v>
       </c>
       <c r="E292" s="5">
-        <v>69200878</v>
+        <v>259716875</v>
       </c>
       <c r="F292" s="5">
         <v>5.7010441646002668E+31</v>
@@ -7823,10 +7823,10 @@
       </c>
       <c r="C293" s="2"/>
       <c r="D293" s="5">
-        <v>2.5802846580463653E+19</v>
+        <v>3.4851063701247155E+18</v>
       </c>
       <c r="E293" s="5">
-        <v>70043982</v>
+        <v>262881105</v>
       </c>
       <c r="F293" s="5">
         <v>8.2665140386703858E+31</v>
@@ -7848,10 +7848,10 @@
       </c>
       <c r="C294" s="2"/>
       <c r="D294" s="5">
-        <v>2.8899188170119295E+19</v>
+        <v>3.8336170071371873E+18</v>
       </c>
       <c r="E294" s="5">
-        <v>70892191</v>
+        <v>266064516</v>
       </c>
       <c r="F294" s="5">
         <v>1.1986445356072058E+32</v>
@@ -7873,10 +7873,10 @@
       </c>
       <c r="C295" s="2"/>
       <c r="D295" s="5">
-        <v>3.2367090750533612E+19</v>
+        <v>4.2169787078509066E+18</v>
       </c>
       <c r="E295" s="5">
-        <v>71745505</v>
+        <v>269267078</v>
       </c>
       <c r="F295" s="5">
         <v>1.7380345766304485E+32</v>
@@ -7898,10 +7898,10 @@
       </c>
       <c r="C296" s="2"/>
       <c r="D296" s="5">
-        <v>3.6251141640597647E+19</v>
+        <v>4.6386765786359972E+18</v>
       </c>
       <c r="E296" s="5">
-        <v>72615718</v>
+        <v>272533066</v>
       </c>
       <c r="F296" s="5">
         <v>2.5201501361141504E+32</v>
@@ -7923,10 +7923,10 @@
       </c>
       <c r="C297" s="2"/>
       <c r="D297" s="5">
-        <v>4.0601278637469368E+19</v>
+        <v>5.1025442364995973E+18</v>
       </c>
       <c r="E297" s="5">
-        <v>73491177</v>
+        <v>275818739</v>
       </c>
       <c r="F297" s="5">
         <v>3.6542176973655177E+32</v>
@@ -7948,10 +7948,10 @@
       </c>
       <c r="C298" s="2"/>
       <c r="D298" s="5">
-        <v>4.5473432073965699E+19</v>
+        <v>5.6127986601495572E+18</v>
       </c>
       <c r="E298" s="5">
-        <v>74371882</v>
+        <v>279124099</v>
       </c>
       <c r="F298" s="5">
         <v>5.2986156611800007E+32</v>
@@ -7973,10 +7973,10 @@
       </c>
       <c r="C299" s="2"/>
       <c r="D299" s="5">
-        <v>5.0930243922841592E+19</v>
+        <v>6.1740785261645138E+18</v>
       </c>
       <c r="E299" s="5">
-        <v>75257833</v>
+        <v>282449144</v>
       </c>
       <c r="F299" s="5">
         <v>7.6829927087110012E+32</v>
@@ -7998,10 +7998,10 @@
       </c>
       <c r="C300" s="2"/>
       <c r="D300" s="5">
-        <v>5.7041873193582592E+19</v>
+        <v>6.7914863787809659E+18</v>
       </c>
       <c r="E300" s="5">
-        <v>76161108</v>
+        <v>285839221</v>
       </c>
       <c r="F300" s="5">
         <v>1.1140339427630951E+33</v>
@@ -8023,10 +8023,10 @@
       </c>
       <c r="C301" s="2"/>
       <c r="D301" s="5">
-        <v>6.3886897976812511E+19</v>
+        <v>7.4706350166590628E+18</v>
       </c>
       <c r="E301" s="5">
-        <v>77069771</v>
+        <v>289249507</v>
       </c>
       <c r="F301" s="5">
         <v>1.615349217006488E+33</v>
@@ -8048,10 +8048,10 @@
       </c>
       <c r="C302" s="2"/>
       <c r="D302" s="5">
-        <v>7.1553325734030017E+19</v>
+        <v>8.2176985183249695E+18</v>
       </c>
       <c r="E302" s="5">
-        <v>80383326</v>
+        <v>301685569</v>
       </c>
       <c r="F302" s="5">
         <v>2.3422563646594074E+33</v>

</xml_diff>